<commit_message>
Atualização de bases das ligas, do dia: 2024-01-29 às 07-55
</commit_message>
<xml_diff>
--- a/Belgium First Division A/Belgium First Division A.xlsx
+++ b/Belgium First Division A/Belgium First Division A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4891" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4915" uniqueCount="54">
   <si>
     <t>id</t>
   </si>
@@ -537,7 +537,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC974"/>
+  <dimension ref="A1:AC980"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -18078,7 +18078,7 @@
         <v>196</v>
       </c>
       <c r="B198">
-        <v>3640746</v>
+        <v>3640938</v>
       </c>
       <c r="C198" t="s">
         <v>28</v>
@@ -18090,40 +18090,40 @@
         <v>44436.5625</v>
       </c>
       <c r="F198" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G198" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="H198">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I198">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J198" t="s">
         <v>51</v>
       </c>
       <c r="K198">
-        <v>2.1</v>
+        <v>1.666</v>
       </c>
       <c r="L198">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="M198">
-        <v>3.3</v>
+        <v>5</v>
       </c>
       <c r="N198">
-        <v>2.3</v>
+        <v>1.6</v>
       </c>
       <c r="O198">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="P198">
-        <v>3</v>
+        <v>5.25</v>
       </c>
       <c r="Q198">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="R198">
         <v>2.05</v>
@@ -18132,13 +18132,13 @@
         <v>1.8</v>
       </c>
       <c r="T198">
-        <v>2.25</v>
+        <v>3</v>
       </c>
       <c r="U198">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="V198">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="W198">
         <v>-1</v>
@@ -18147,7 +18147,7 @@
         <v>-1</v>
       </c>
       <c r="Y198">
-        <v>2</v>
+        <v>4.25</v>
       </c>
       <c r="Z198">
         <v>-1</v>
@@ -18156,10 +18156,10 @@
         <v>0.8</v>
       </c>
       <c r="AB198">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC198">
-        <v>0.825</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="199" spans="1:29">
@@ -18167,7 +18167,7 @@
         <v>197</v>
       </c>
       <c r="B199">
-        <v>3640938</v>
+        <v>3640746</v>
       </c>
       <c r="C199" t="s">
         <v>28</v>
@@ -18179,40 +18179,40 @@
         <v>44436.5625</v>
       </c>
       <c r="F199" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G199" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="H199">
+        <v>0</v>
+      </c>
+      <c r="I199">
         <v>1</v>
-      </c>
-      <c r="I199">
-        <v>2</v>
       </c>
       <c r="J199" t="s">
         <v>51</v>
       </c>
       <c r="K199">
-        <v>1.666</v>
+        <v>2.1</v>
       </c>
       <c r="L199">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="M199">
-        <v>5</v>
+        <v>3.3</v>
       </c>
       <c r="N199">
-        <v>1.6</v>
+        <v>2.3</v>
       </c>
       <c r="O199">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="P199">
-        <v>5.25</v>
+        <v>3</v>
       </c>
       <c r="Q199">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="R199">
         <v>2.05</v>
@@ -18221,13 +18221,13 @@
         <v>1.8</v>
       </c>
       <c r="T199">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="U199">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="V199">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="W199">
         <v>-1</v>
@@ -18236,7 +18236,7 @@
         <v>-1</v>
       </c>
       <c r="Y199">
-        <v>4.25</v>
+        <v>2</v>
       </c>
       <c r="Z199">
         <v>-1</v>
@@ -18245,10 +18245,10 @@
         <v>0.8</v>
       </c>
       <c r="AB199">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC199">
-        <v>-0</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="200" spans="1:29">
@@ -19235,7 +19235,7 @@
         <v>209</v>
       </c>
       <c r="B211">
-        <v>3639269</v>
+        <v>3640754</v>
       </c>
       <c r="C211" t="s">
         <v>28</v>
@@ -19247,76 +19247,76 @@
         <v>44451.66666666666</v>
       </c>
       <c r="F211" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G211" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="H211">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I211">
         <v>1</v>
       </c>
       <c r="J211" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K211">
-        <v>2</v>
+        <v>2.7</v>
       </c>
       <c r="L211">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="M211">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="N211">
-        <v>2.8</v>
+        <v>2.45</v>
       </c>
       <c r="O211">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="P211">
-        <v>2.3</v>
+        <v>2.75</v>
       </c>
       <c r="Q211">
         <v>0</v>
       </c>
       <c r="R211">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="S211">
-        <v>1.8</v>
+        <v>1.975</v>
       </c>
       <c r="T211">
         <v>3</v>
       </c>
       <c r="U211">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="V211">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="W211">
-        <v>-1</v>
+        <v>1.45</v>
       </c>
       <c r="X211">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Y211">
         <v>-1</v>
       </c>
       <c r="Z211">
+        <v>0.875</v>
+      </c>
+      <c r="AA211">
+        <v>-1</v>
+      </c>
+      <c r="AB211">
         <v>0</v>
       </c>
-      <c r="AA211">
+      <c r="AC211">
         <v>-0</v>
-      </c>
-      <c r="AB211">
-        <v>-1</v>
-      </c>
-      <c r="AC211">
-        <v>1.025</v>
       </c>
     </row>
     <row r="212" spans="1:29">
@@ -19324,7 +19324,7 @@
         <v>210</v>
       </c>
       <c r="B212">
-        <v>3640754</v>
+        <v>3639269</v>
       </c>
       <c r="C212" t="s">
         <v>28</v>
@@ -19336,76 +19336,76 @@
         <v>44451.66666666666</v>
       </c>
       <c r="F212" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="G212" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="H212">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I212">
         <v>1</v>
       </c>
       <c r="J212" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K212">
-        <v>2.7</v>
+        <v>2</v>
       </c>
       <c r="L212">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="M212">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="N212">
-        <v>2.45</v>
+        <v>2.8</v>
       </c>
       <c r="O212">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="P212">
-        <v>2.75</v>
+        <v>2.3</v>
       </c>
       <c r="Q212">
         <v>0</v>
       </c>
       <c r="R212">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="S212">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="T212">
         <v>3</v>
       </c>
       <c r="U212">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="V212">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="W212">
-        <v>1.45</v>
+        <v>-1</v>
       </c>
       <c r="X212">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Y212">
         <v>-1</v>
       </c>
       <c r="Z212">
-        <v>0.875</v>
+        <v>0</v>
       </c>
       <c r="AA212">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="AB212">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC212">
-        <v>-0</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="213" spans="1:29">
@@ -21104,7 +21104,7 @@
         <v>230</v>
       </c>
       <c r="B232">
-        <v>3640771</v>
+        <v>3640768</v>
       </c>
       <c r="C232" t="s">
         <v>28</v>
@@ -21116,49 +21116,49 @@
         <v>44465.66666666666</v>
       </c>
       <c r="F232" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G232" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="H232">
+        <v>3</v>
+      </c>
+      <c r="I232">
         <v>0</v>
       </c>
-      <c r="I232">
-        <v>2</v>
-      </c>
       <c r="J232" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K232">
-        <v>2.05</v>
+        <v>1.25</v>
       </c>
       <c r="L232">
-        <v>3.6</v>
+        <v>5.5</v>
       </c>
       <c r="M232">
-        <v>3.1</v>
+        <v>9</v>
       </c>
       <c r="N232">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="O232">
-        <v>3.8</v>
+        <v>5</v>
       </c>
       <c r="P232">
-        <v>3.4</v>
+        <v>8</v>
       </c>
       <c r="Q232">
-        <v>-0.25</v>
+        <v>-1.5</v>
       </c>
       <c r="R232">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="S232">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="T232">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="U232">
         <v>1.95</v>
@@ -21167,19 +21167,19 @@
         <v>1.9</v>
       </c>
       <c r="W232">
-        <v>-1</v>
+        <v>0.3</v>
       </c>
       <c r="X232">
         <v>-1</v>
       </c>
       <c r="Y232">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Z232">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA232">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AB232">
         <v>-1</v>
@@ -21193,7 +21193,7 @@
         <v>231</v>
       </c>
       <c r="B233">
-        <v>3640768</v>
+        <v>3640771</v>
       </c>
       <c r="C233" t="s">
         <v>28</v>
@@ -21205,49 +21205,49 @@
         <v>44465.66666666666</v>
       </c>
       <c r="F233" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G233" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="H233">
+        <v>0</v>
+      </c>
+      <c r="I233">
+        <v>2</v>
+      </c>
+      <c r="J233" t="s">
+        <v>51</v>
+      </c>
+      <c r="K233">
+        <v>2.05</v>
+      </c>
+      <c r="L233">
+        <v>3.6</v>
+      </c>
+      <c r="M233">
+        <v>3.1</v>
+      </c>
+      <c r="N233">
+        <v>2</v>
+      </c>
+      <c r="O233">
+        <v>3.8</v>
+      </c>
+      <c r="P233">
+        <v>3.4</v>
+      </c>
+      <c r="Q233">
+        <v>-0.25</v>
+      </c>
+      <c r="R233">
+        <v>1.825</v>
+      </c>
+      <c r="S233">
+        <v>2.025</v>
+      </c>
+      <c r="T233">
         <v>3</v>
-      </c>
-      <c r="I233">
-        <v>0</v>
-      </c>
-      <c r="J233" t="s">
-        <v>52</v>
-      </c>
-      <c r="K233">
-        <v>1.25</v>
-      </c>
-      <c r="L233">
-        <v>5.5</v>
-      </c>
-      <c r="M233">
-        <v>9</v>
-      </c>
-      <c r="N233">
-        <v>1.3</v>
-      </c>
-      <c r="O233">
-        <v>5</v>
-      </c>
-      <c r="P233">
-        <v>8</v>
-      </c>
-      <c r="Q233">
-        <v>-1.5</v>
-      </c>
-      <c r="R233">
-        <v>1.925</v>
-      </c>
-      <c r="S233">
-        <v>1.925</v>
-      </c>
-      <c r="T233">
-        <v>3.5</v>
       </c>
       <c r="U233">
         <v>1.95</v>
@@ -21256,19 +21256,19 @@
         <v>1.9</v>
       </c>
       <c r="W233">
-        <v>0.3</v>
+        <v>-1</v>
       </c>
       <c r="X233">
         <v>-1</v>
       </c>
       <c r="Y233">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Z233">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AA233">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AB233">
         <v>-1</v>
@@ -27067,7 +27067,7 @@
         <v>297</v>
       </c>
       <c r="B299">
-        <v>3640831</v>
+        <v>3640834</v>
       </c>
       <c r="C299" t="s">
         <v>28</v>
@@ -27079,76 +27079,76 @@
         <v>44534.60416666666</v>
       </c>
       <c r="F299" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G299" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H299">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I299">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J299" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K299">
-        <v>2.25</v>
+        <v>2.4</v>
       </c>
       <c r="L299">
         <v>3.5</v>
       </c>
       <c r="M299">
+        <v>2.75</v>
+      </c>
+      <c r="N299">
+        <v>2.25</v>
+      </c>
+      <c r="O299">
+        <v>3.5</v>
+      </c>
+      <c r="P299">
         <v>3</v>
       </c>
-      <c r="N299">
-        <v>3</v>
-      </c>
-      <c r="O299">
-        <v>3.4</v>
-      </c>
-      <c r="P299">
-        <v>2.3</v>
-      </c>
       <c r="Q299">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R299">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="S299">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="T299">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="U299">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="V299">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="W299">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="X299">
         <v>-1</v>
       </c>
       <c r="Y299">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="Z299">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AA299">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AB299">
+        <v>0.4</v>
+      </c>
+      <c r="AC299">
         <v>-0.5</v>
-      </c>
-      <c r="AC299">
-        <v>0.5125</v>
       </c>
     </row>
     <row r="300" spans="1:29">
@@ -27156,7 +27156,7 @@
         <v>298</v>
       </c>
       <c r="B300">
-        <v>3640834</v>
+        <v>3640831</v>
       </c>
       <c r="C300" t="s">
         <v>28</v>
@@ -27168,76 +27168,76 @@
         <v>44534.60416666666</v>
       </c>
       <c r="F300" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G300" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H300">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I300">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J300" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K300">
-        <v>2.4</v>
+        <v>2.25</v>
       </c>
       <c r="L300">
         <v>3.5</v>
       </c>
       <c r="M300">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="N300">
+        <v>3</v>
+      </c>
+      <c r="O300">
+        <v>3.4</v>
+      </c>
+      <c r="P300">
+        <v>2.3</v>
+      </c>
+      <c r="Q300">
+        <v>0.25</v>
+      </c>
+      <c r="R300">
+        <v>1.825</v>
+      </c>
+      <c r="S300">
+        <v>2.025</v>
+      </c>
+      <c r="T300">
         <v>2.25</v>
       </c>
-      <c r="O300">
-        <v>3.5</v>
-      </c>
-      <c r="P300">
-        <v>3</v>
-      </c>
-      <c r="Q300">
-        <v>-0.25</v>
-      </c>
-      <c r="R300">
-        <v>2</v>
-      </c>
-      <c r="S300">
-        <v>1.85</v>
-      </c>
-      <c r="T300">
-        <v>2.75</v>
-      </c>
       <c r="U300">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="V300">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="W300">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="X300">
         <v>-1</v>
       </c>
       <c r="Y300">
-        <v>-1</v>
+        <v>1.3</v>
       </c>
       <c r="Z300">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AA300">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AB300">
-        <v>0.4</v>
+        <v>-0.5</v>
       </c>
       <c r="AC300">
-        <v>-0.5</v>
+        <v>0.5125</v>
       </c>
     </row>
     <row r="301" spans="1:29">
@@ -27868,7 +27868,7 @@
         <v>306</v>
       </c>
       <c r="B308">
-        <v>3640943</v>
+        <v>3640840</v>
       </c>
       <c r="C308" t="s">
         <v>28</v>
@@ -27880,76 +27880,76 @@
         <v>44541.60416666666</v>
       </c>
       <c r="F308" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G308" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H308">
         <v>1</v>
       </c>
       <c r="I308">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J308" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K308">
-        <v>1.615</v>
+        <v>1.909</v>
       </c>
       <c r="L308">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="M308">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N308">
-        <v>1.95</v>
+        <v>2.9</v>
       </c>
       <c r="O308">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="P308">
-        <v>3.8</v>
+        <v>2.5</v>
       </c>
       <c r="Q308">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R308">
-        <v>2</v>
+        <v>1.775</v>
       </c>
       <c r="S308">
-        <v>1.85</v>
+        <v>2.1</v>
       </c>
       <c r="T308">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="U308">
-        <v>1.825</v>
+        <v>2.05</v>
       </c>
       <c r="V308">
-        <v>2.025</v>
+        <v>1.8</v>
       </c>
       <c r="W308">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="X308">
         <v>-1</v>
       </c>
       <c r="Y308">
-        <v>-1</v>
+        <v>1.5</v>
       </c>
       <c r="Z308">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AA308">
-        <v>-1</v>
+        <v>1.1</v>
       </c>
       <c r="AB308">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AC308">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="309" spans="1:29">
@@ -27957,7 +27957,7 @@
         <v>307</v>
       </c>
       <c r="B309">
-        <v>3640840</v>
+        <v>3640943</v>
       </c>
       <c r="C309" t="s">
         <v>28</v>
@@ -27969,76 +27969,76 @@
         <v>44541.60416666666</v>
       </c>
       <c r="F309" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G309" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H309">
         <v>1</v>
       </c>
       <c r="I309">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J309" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K309">
-        <v>1.909</v>
+        <v>1.615</v>
       </c>
       <c r="L309">
+        <v>4.2</v>
+      </c>
+      <c r="M309">
+        <v>5</v>
+      </c>
+      <c r="N309">
+        <v>1.95</v>
+      </c>
+      <c r="O309">
         <v>3.6</v>
       </c>
-      <c r="M309">
-        <v>4</v>
-      </c>
-      <c r="N309">
-        <v>2.9</v>
-      </c>
-      <c r="O309">
-        <v>3.1</v>
-      </c>
       <c r="P309">
+        <v>3.8</v>
+      </c>
+      <c r="Q309">
+        <v>-0.5</v>
+      </c>
+      <c r="R309">
+        <v>2</v>
+      </c>
+      <c r="S309">
+        <v>1.85</v>
+      </c>
+      <c r="T309">
         <v>2.5</v>
       </c>
-      <c r="Q309">
-        <v>0.25</v>
-      </c>
-      <c r="R309">
-        <v>1.775</v>
-      </c>
-      <c r="S309">
-        <v>2.1</v>
-      </c>
-      <c r="T309">
-        <v>2.25</v>
-      </c>
       <c r="U309">
-        <v>2.05</v>
+        <v>1.825</v>
       </c>
       <c r="V309">
-        <v>1.8</v>
+        <v>2.025</v>
       </c>
       <c r="W309">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="X309">
         <v>-1</v>
       </c>
       <c r="Y309">
-        <v>1.5</v>
+        <v>-1</v>
       </c>
       <c r="Z309">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AA309">
-        <v>1.1</v>
+        <v>-1</v>
       </c>
       <c r="AB309">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AC309">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="310" spans="1:29">
@@ -28580,7 +28580,7 @@
         <v>314</v>
       </c>
       <c r="B316">
-        <v>3640849</v>
+        <v>3640842</v>
       </c>
       <c r="C316" t="s">
         <v>28</v>
@@ -28592,76 +28592,76 @@
         <v>44544.70833333334</v>
       </c>
       <c r="F316" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="G316" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="H316">
+        <v>2</v>
+      </c>
+      <c r="I316">
         <v>0</v>
       </c>
-      <c r="I316">
-        <v>2</v>
-      </c>
       <c r="J316" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K316">
-        <v>2.55</v>
+        <v>1.363</v>
       </c>
       <c r="L316">
-        <v>3.4</v>
+        <v>5.5</v>
       </c>
       <c r="M316">
-        <v>2.625</v>
+        <v>6.5</v>
       </c>
       <c r="N316">
-        <v>2.2</v>
+        <v>1.363</v>
       </c>
       <c r="O316">
-        <v>3.4</v>
+        <v>5</v>
       </c>
       <c r="P316">
-        <v>3.1</v>
+        <v>7.5</v>
       </c>
       <c r="Q316">
-        <v>-0.25</v>
+        <v>-1.25</v>
       </c>
       <c r="R316">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="S316">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="T316">
         <v>2.75</v>
       </c>
       <c r="U316">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V316">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W316">
-        <v>-1</v>
+        <v>0.363</v>
       </c>
       <c r="X316">
         <v>-1</v>
       </c>
       <c r="Y316">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="Z316">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA316">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB316">
         <v>-1</v>
       </c>
       <c r="AC316">
-        <v>0.875</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="317" spans="1:29">
@@ -28669,7 +28669,7 @@
         <v>315</v>
       </c>
       <c r="B317">
-        <v>3640842</v>
+        <v>3640849</v>
       </c>
       <c r="C317" t="s">
         <v>28</v>
@@ -28681,76 +28681,76 @@
         <v>44544.70833333334</v>
       </c>
       <c r="F317" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G317" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H317">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I317">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J317" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K317">
-        <v>1.363</v>
+        <v>2.55</v>
       </c>
       <c r="L317">
-        <v>5.5</v>
+        <v>3.4</v>
       </c>
       <c r="M317">
-        <v>6.5</v>
+        <v>2.625</v>
       </c>
       <c r="N317">
-        <v>1.363</v>
+        <v>2.2</v>
       </c>
       <c r="O317">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="P317">
-        <v>7.5</v>
+        <v>3.1</v>
       </c>
       <c r="Q317">
-        <v>-1.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R317">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="S317">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="T317">
         <v>2.75</v>
       </c>
       <c r="U317">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V317">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W317">
-        <v>0.363</v>
+        <v>-1</v>
       </c>
       <c r="X317">
         <v>-1</v>
       </c>
       <c r="Y317">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="Z317">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA317">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB317">
         <v>-1</v>
       </c>
       <c r="AC317">
-        <v>0.95</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="318" spans="1:29">
@@ -28758,7 +28758,7 @@
         <v>316</v>
       </c>
       <c r="B318">
-        <v>3640848</v>
+        <v>3639281</v>
       </c>
       <c r="C318" t="s">
         <v>28</v>
@@ -28770,76 +28770,76 @@
         <v>44545.61458333334</v>
       </c>
       <c r="F318" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G318" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H318">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I318">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J318" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K318">
+        <v>5.5</v>
+      </c>
+      <c r="L318">
+        <v>4.333</v>
+      </c>
+      <c r="M318">
+        <v>1.533</v>
+      </c>
+      <c r="N318">
+        <v>7.5</v>
+      </c>
+      <c r="O318">
+        <v>5.25</v>
+      </c>
+      <c r="P318">
+        <v>1.363</v>
+      </c>
+      <c r="Q318">
+        <v>1.5</v>
+      </c>
+      <c r="R318">
+        <v>1.875</v>
+      </c>
+      <c r="S318">
+        <v>1.975</v>
+      </c>
+      <c r="T318">
         <v>3.5</v>
       </c>
-      <c r="L318">
-        <v>3.6</v>
-      </c>
-      <c r="M318">
-        <v>2</v>
-      </c>
-      <c r="N318">
-        <v>4.5</v>
-      </c>
-      <c r="O318">
-        <v>3.75</v>
-      </c>
-      <c r="P318">
-        <v>1.75</v>
-      </c>
-      <c r="Q318">
-        <v>0.75</v>
-      </c>
-      <c r="R318">
-        <v>1.8</v>
-      </c>
-      <c r="S318">
-        <v>2.05</v>
-      </c>
-      <c r="T318">
-        <v>2.75</v>
-      </c>
       <c r="U318">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V318">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W318">
-        <v>3.5</v>
+        <v>-1</v>
       </c>
       <c r="X318">
         <v>-1</v>
       </c>
       <c r="Y318">
-        <v>-1</v>
+        <v>0.363</v>
       </c>
       <c r="Z318">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA318">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB318">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC318">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="319" spans="1:29">
@@ -28847,7 +28847,7 @@
         <v>317</v>
       </c>
       <c r="B319">
-        <v>3639281</v>
+        <v>3640848</v>
       </c>
       <c r="C319" t="s">
         <v>28</v>
@@ -28859,76 +28859,76 @@
         <v>44545.61458333334</v>
       </c>
       <c r="F319" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G319" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H319">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I319">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J319" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K319">
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="L319">
-        <v>4.333</v>
+        <v>3.6</v>
       </c>
       <c r="M319">
-        <v>1.533</v>
+        <v>2</v>
       </c>
       <c r="N319">
-        <v>7.5</v>
+        <v>4.5</v>
       </c>
       <c r="O319">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="P319">
-        <v>1.363</v>
+        <v>1.75</v>
       </c>
       <c r="Q319">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="R319">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="S319">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="T319">
+        <v>2.75</v>
+      </c>
+      <c r="U319">
+        <v>1.925</v>
+      </c>
+      <c r="V319">
+        <v>1.925</v>
+      </c>
+      <c r="W319">
         <v>3.5</v>
       </c>
-      <c r="U319">
-        <v>1.9</v>
-      </c>
-      <c r="V319">
-        <v>1.95</v>
-      </c>
-      <c r="W319">
-        <v>-1</v>
-      </c>
       <c r="X319">
         <v>-1</v>
       </c>
       <c r="Y319">
-        <v>0.363</v>
+        <v>-1</v>
       </c>
       <c r="Z319">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA319">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB319">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AC319">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="320" spans="1:29">
@@ -32496,7 +32496,7 @@
         <v>358</v>
       </c>
       <c r="B360">
-        <v>3640946</v>
+        <v>3640881</v>
       </c>
       <c r="C360" t="s">
         <v>28</v>
@@ -32508,76 +32508,76 @@
         <v>44587.70833333334</v>
       </c>
       <c r="F360" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G360" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H360">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I360">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J360" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K360">
+        <v>1.571</v>
+      </c>
+      <c r="L360">
+        <v>4</v>
+      </c>
+      <c r="M360">
+        <v>5.5</v>
+      </c>
+      <c r="N360">
+        <v>1.7</v>
+      </c>
+      <c r="O360">
+        <v>3.75</v>
+      </c>
+      <c r="P360">
+        <v>5</v>
+      </c>
+      <c r="Q360">
+        <v>-0.75</v>
+      </c>
+      <c r="R360">
         <v>1.95</v>
       </c>
-      <c r="L360">
-        <v>3.6</v>
-      </c>
-      <c r="M360">
-        <v>3.6</v>
-      </c>
-      <c r="N360">
-        <v>2.375</v>
-      </c>
-      <c r="O360">
-        <v>3.3</v>
-      </c>
-      <c r="P360">
-        <v>2.9</v>
-      </c>
-      <c r="Q360">
-        <v>-0.25</v>
-      </c>
-      <c r="R360">
-        <v>2.1</v>
-      </c>
       <c r="S360">
-        <v>1.775</v>
+        <v>1.9</v>
       </c>
       <c r="T360">
         <v>2.5</v>
       </c>
       <c r="U360">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="V360">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="W360">
-        <v>1.375</v>
+        <v>-1</v>
       </c>
       <c r="X360">
         <v>-1</v>
       </c>
       <c r="Y360">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="Z360">
-        <v>1.1</v>
+        <v>-1</v>
       </c>
       <c r="AA360">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB360">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC360">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="361" spans="1:29">
@@ -32585,7 +32585,7 @@
         <v>359</v>
       </c>
       <c r="B361">
-        <v>3640881</v>
+        <v>3640946</v>
       </c>
       <c r="C361" t="s">
         <v>28</v>
@@ -32597,76 +32597,76 @@
         <v>44587.70833333334</v>
       </c>
       <c r="F361" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G361" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H361">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I361">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J361" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K361">
-        <v>1.571</v>
+        <v>1.95</v>
       </c>
       <c r="L361">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M361">
-        <v>5.5</v>
+        <v>3.6</v>
       </c>
       <c r="N361">
-        <v>1.7</v>
+        <v>2.375</v>
       </c>
       <c r="O361">
-        <v>3.75</v>
+        <v>3.3</v>
       </c>
       <c r="P361">
-        <v>5</v>
+        <v>2.9</v>
       </c>
       <c r="Q361">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R361">
-        <v>1.95</v>
+        <v>2.1</v>
       </c>
       <c r="S361">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="T361">
         <v>2.5</v>
       </c>
       <c r="U361">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="V361">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="W361">
-        <v>-1</v>
+        <v>1.375</v>
       </c>
       <c r="X361">
         <v>-1</v>
       </c>
       <c r="Y361">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="Z361">
-        <v>-1</v>
+        <v>1.1</v>
       </c>
       <c r="AA361">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB361">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AC361">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="362" spans="1:29">
@@ -34721,7 +34721,7 @@
         <v>383</v>
       </c>
       <c r="B385">
-        <v>3640905</v>
+        <v>3640908</v>
       </c>
       <c r="C385" t="s">
         <v>28</v>
@@ -34733,58 +34733,58 @@
         <v>44604.60416666666</v>
       </c>
       <c r="F385" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G385" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H385">
         <v>3</v>
       </c>
       <c r="I385">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J385" t="s">
         <v>52</v>
       </c>
       <c r="K385">
-        <v>2.7</v>
+        <v>2.05</v>
       </c>
       <c r="L385">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M385">
-        <v>2.45</v>
+        <v>3.3</v>
       </c>
       <c r="N385">
-        <v>2.55</v>
+        <v>1.8</v>
       </c>
       <c r="O385">
-        <v>3.25</v>
+        <v>3.8</v>
       </c>
       <c r="P385">
-        <v>2.7</v>
+        <v>4</v>
       </c>
       <c r="Q385">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="R385">
-        <v>1.9</v>
+        <v>2.05</v>
       </c>
       <c r="S385">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="T385">
         <v>2.5</v>
       </c>
       <c r="U385">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="V385">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="W385">
-        <v>1.55</v>
+        <v>0.8</v>
       </c>
       <c r="X385">
         <v>-1</v>
@@ -34793,13 +34793,13 @@
         <v>-1</v>
       </c>
       <c r="Z385">
-        <v>0.8999999999999999</v>
+        <v>1.05</v>
       </c>
       <c r="AA385">
         <v>-1</v>
       </c>
       <c r="AB385">
-        <v>0.8999999999999999</v>
+        <v>0.825</v>
       </c>
       <c r="AC385">
         <v>-1</v>
@@ -34810,7 +34810,7 @@
         <v>384</v>
       </c>
       <c r="B386">
-        <v>3640908</v>
+        <v>3640905</v>
       </c>
       <c r="C386" t="s">
         <v>28</v>
@@ -34822,58 +34822,58 @@
         <v>44604.60416666666</v>
       </c>
       <c r="F386" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G386" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H386">
         <v>3</v>
       </c>
       <c r="I386">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J386" t="s">
         <v>52</v>
       </c>
       <c r="K386">
-        <v>2.05</v>
+        <v>2.7</v>
       </c>
       <c r="L386">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M386">
-        <v>3.3</v>
+        <v>2.45</v>
       </c>
       <c r="N386">
-        <v>1.8</v>
+        <v>2.55</v>
       </c>
       <c r="O386">
-        <v>3.8</v>
+        <v>3.25</v>
       </c>
       <c r="P386">
-        <v>4</v>
+        <v>2.7</v>
       </c>
       <c r="Q386">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="R386">
-        <v>2.05</v>
+        <v>1.9</v>
       </c>
       <c r="S386">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="T386">
         <v>2.5</v>
       </c>
       <c r="U386">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="V386">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="W386">
-        <v>0.8</v>
+        <v>1.55</v>
       </c>
       <c r="X386">
         <v>-1</v>
@@ -34882,13 +34882,13 @@
         <v>-1</v>
       </c>
       <c r="Z386">
-        <v>1.05</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA386">
         <v>-1</v>
       </c>
       <c r="AB386">
-        <v>0.825</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC386">
         <v>-1</v>
@@ -38103,7 +38103,7 @@
         <v>421</v>
       </c>
       <c r="B423">
-        <v>3823355</v>
+        <v>3823362</v>
       </c>
       <c r="C423" t="s">
         <v>28</v>
@@ -38115,13 +38115,13 @@
         <v>44632.60416666666</v>
       </c>
       <c r="F423" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G423" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H423">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I423">
         <v>0</v>
@@ -38130,43 +38130,43 @@
         <v>52</v>
       </c>
       <c r="K423">
-        <v>2.3</v>
+        <v>1.65</v>
       </c>
       <c r="L423">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="M423">
-        <v>2.8</v>
+        <v>5.25</v>
       </c>
       <c r="N423">
-        <v>2.45</v>
+        <v>1.571</v>
       </c>
       <c r="O423">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="P423">
-        <v>2.75</v>
+        <v>5.75</v>
       </c>
       <c r="Q423">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="R423">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="S423">
-        <v>2.05</v>
+        <v>1.85</v>
       </c>
       <c r="T423">
         <v>2.5</v>
       </c>
       <c r="U423">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="V423">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="W423">
-        <v>1.45</v>
+        <v>0.571</v>
       </c>
       <c r="X423">
         <v>-1</v>
@@ -38175,16 +38175,16 @@
         <v>-1</v>
       </c>
       <c r="Z423">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AA423">
         <v>-1</v>
       </c>
       <c r="AB423">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC423">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="424" spans="1:29">
@@ -38192,7 +38192,7 @@
         <v>422</v>
       </c>
       <c r="B424">
-        <v>3823362</v>
+        <v>3823355</v>
       </c>
       <c r="C424" t="s">
         <v>28</v>
@@ -38204,13 +38204,13 @@
         <v>44632.60416666666</v>
       </c>
       <c r="F424" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G424" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H424">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I424">
         <v>0</v>
@@ -38219,43 +38219,43 @@
         <v>52</v>
       </c>
       <c r="K424">
-        <v>1.65</v>
+        <v>2.3</v>
       </c>
       <c r="L424">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="M424">
-        <v>5.25</v>
+        <v>2.8</v>
       </c>
       <c r="N424">
-        <v>1.571</v>
+        <v>2.45</v>
       </c>
       <c r="O424">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="P424">
-        <v>5.75</v>
+        <v>2.75</v>
       </c>
       <c r="Q424">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="R424">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="S424">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="T424">
         <v>2.5</v>
       </c>
       <c r="U424">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="V424">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="W424">
-        <v>0.571</v>
+        <v>1.45</v>
       </c>
       <c r="X424">
         <v>-1</v>
@@ -38264,16 +38264,16 @@
         <v>-1</v>
       </c>
       <c r="Z424">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AA424">
         <v>-1</v>
       </c>
       <c r="AB424">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC424">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="425" spans="1:29">
@@ -43087,7 +43087,7 @@
         <v>477</v>
       </c>
       <c r="B479">
-        <v>5208622</v>
+        <v>5208464</v>
       </c>
       <c r="C479" t="s">
         <v>28</v>
@@ -43099,34 +43099,34 @@
         <v>44772.55208333334</v>
       </c>
       <c r="F479" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G479" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="H479">
         <v>2</v>
       </c>
       <c r="I479">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J479" t="s">
         <v>52</v>
       </c>
       <c r="K479">
-        <v>1.85</v>
+        <v>2.4</v>
       </c>
       <c r="L479">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="M479">
-        <v>3.75</v>
+        <v>2.625</v>
       </c>
       <c r="N479">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="O479">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="P479">
         <v>2.15</v>
@@ -43135,22 +43135,22 @@
         <v>0.25</v>
       </c>
       <c r="R479">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="S479">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="T479">
         <v>2.75</v>
       </c>
       <c r="U479">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="V479">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="W479">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="X479">
         <v>-1</v>
@@ -43159,16 +43159,16 @@
         <v>-1</v>
       </c>
       <c r="Z479">
-        <v>0.95</v>
+        <v>0.875</v>
       </c>
       <c r="AA479">
         <v>-1</v>
       </c>
       <c r="AB479">
-        <v>-1</v>
+        <v>0.4875</v>
       </c>
       <c r="AC479">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="480" spans="1:29">
@@ -43176,7 +43176,7 @@
         <v>478</v>
       </c>
       <c r="B480">
-        <v>5208464</v>
+        <v>5208622</v>
       </c>
       <c r="C480" t="s">
         <v>28</v>
@@ -43188,34 +43188,34 @@
         <v>44772.55208333334</v>
       </c>
       <c r="F480" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G480" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="H480">
         <v>2</v>
       </c>
       <c r="I480">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J480" t="s">
         <v>52</v>
       </c>
       <c r="K480">
-        <v>2.4</v>
+        <v>1.85</v>
       </c>
       <c r="L480">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="M480">
-        <v>2.625</v>
+        <v>3.75</v>
       </c>
       <c r="N480">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
       <c r="O480">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P480">
         <v>2.15</v>
@@ -43224,22 +43224,22 @@
         <v>0.25</v>
       </c>
       <c r="R480">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="S480">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="T480">
         <v>2.75</v>
       </c>
       <c r="U480">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="V480">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="W480">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="X480">
         <v>-1</v>
@@ -43248,16 +43248,16 @@
         <v>-1</v>
       </c>
       <c r="Z480">
-        <v>0.875</v>
+        <v>0.95</v>
       </c>
       <c r="AA480">
         <v>-1</v>
       </c>
       <c r="AB480">
-        <v>0.4875</v>
+        <v>-1</v>
       </c>
       <c r="AC480">
-        <v>-0.5</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="481" spans="1:29">
@@ -52165,7 +52165,7 @@
         <v>579</v>
       </c>
       <c r="B581">
-        <v>5208527</v>
+        <v>5208664</v>
       </c>
       <c r="C581" t="s">
         <v>28</v>
@@ -52177,13 +52177,13 @@
         <v>44853.65625</v>
       </c>
       <c r="F581" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="G581" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H581">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I581">
         <v>0</v>
@@ -52192,43 +52192,43 @@
         <v>52</v>
       </c>
       <c r="K581">
-        <v>1.363</v>
+        <v>2.625</v>
       </c>
       <c r="L581">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="M581">
-        <v>7</v>
+        <v>2.55</v>
       </c>
       <c r="N581">
-        <v>1.571</v>
+        <v>2.25</v>
       </c>
       <c r="O581">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="P581">
-        <v>5.25</v>
+        <v>3.1</v>
       </c>
       <c r="Q581">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="R581">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="S581">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="T581">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U581">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="V581">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="W581">
-        <v>0.571</v>
+        <v>1.25</v>
       </c>
       <c r="X581">
         <v>-1</v>
@@ -52237,16 +52237,16 @@
         <v>-1</v>
       </c>
       <c r="Z581">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AA581">
         <v>-1</v>
       </c>
       <c r="AB581">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC581">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="582" spans="1:29">
@@ -52254,7 +52254,7 @@
         <v>580</v>
       </c>
       <c r="B582">
-        <v>5208664</v>
+        <v>5208527</v>
       </c>
       <c r="C582" t="s">
         <v>28</v>
@@ -52266,13 +52266,13 @@
         <v>44853.65625</v>
       </c>
       <c r="F582" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="G582" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H582">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I582">
         <v>0</v>
@@ -52281,43 +52281,43 @@
         <v>52</v>
       </c>
       <c r="K582">
-        <v>2.625</v>
+        <v>1.363</v>
       </c>
       <c r="L582">
-        <v>3.4</v>
+        <v>5</v>
       </c>
       <c r="M582">
-        <v>2.55</v>
+        <v>7</v>
       </c>
       <c r="N582">
-        <v>2.25</v>
+        <v>1.571</v>
       </c>
       <c r="O582">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="P582">
-        <v>3.1</v>
+        <v>5.25</v>
       </c>
       <c r="Q582">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="R582">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="S582">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="T582">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U582">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="V582">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="W582">
-        <v>1.25</v>
+        <v>0.571</v>
       </c>
       <c r="X582">
         <v>-1</v>
@@ -52326,16 +52326,16 @@
         <v>-1</v>
       </c>
       <c r="Z582">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="AA582">
         <v>-1</v>
       </c>
       <c r="AB582">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AC582">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="583" spans="1:29">
@@ -55814,7 +55814,7 @@
         <v>620</v>
       </c>
       <c r="B622">
-        <v>5208685</v>
+        <v>5208686</v>
       </c>
       <c r="C622" t="s">
         <v>28</v>
@@ -55826,76 +55826,76 @@
         <v>44918.6875</v>
       </c>
       <c r="F622" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="G622" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H622">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I622">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J622" t="s">
         <v>53</v>
       </c>
       <c r="K622">
-        <v>1.7</v>
+        <v>2.45</v>
       </c>
       <c r="L622">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="M622">
-        <v>4.333</v>
+        <v>2.5</v>
       </c>
       <c r="N622">
-        <v>1.363</v>
+        <v>2.3</v>
       </c>
       <c r="O622">
-        <v>4.5</v>
+        <v>3.4</v>
       </c>
       <c r="P622">
-        <v>7</v>
+        <v>2.7</v>
       </c>
       <c r="Q622">
-        <v>-1.25</v>
+        <v>0</v>
       </c>
       <c r="R622">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="S622">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="T622">
         <v>2.75</v>
       </c>
       <c r="U622">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="V622">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="W622">
         <v>-1</v>
       </c>
       <c r="X622">
-        <v>3.5</v>
+        <v>2.4</v>
       </c>
       <c r="Y622">
         <v>-1</v>
       </c>
       <c r="Z622">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA622">
-        <v>0.95</v>
+        <v>-0</v>
       </c>
       <c r="AB622">
         <v>-1</v>
       </c>
       <c r="AC622">
-        <v>1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="623" spans="1:29">
@@ -55903,7 +55903,7 @@
         <v>621</v>
       </c>
       <c r="B623">
-        <v>5208686</v>
+        <v>5208685</v>
       </c>
       <c r="C623" t="s">
         <v>28</v>
@@ -55915,76 +55915,76 @@
         <v>44918.6875</v>
       </c>
       <c r="F623" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="G623" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H623">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I623">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J623" t="s">
         <v>53</v>
       </c>
       <c r="K623">
-        <v>2.45</v>
+        <v>1.7</v>
       </c>
       <c r="L623">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="M623">
-        <v>2.5</v>
+        <v>4.333</v>
       </c>
       <c r="N623">
-        <v>2.3</v>
+        <v>1.363</v>
       </c>
       <c r="O623">
-        <v>3.4</v>
+        <v>4.5</v>
       </c>
       <c r="P623">
-        <v>2.7</v>
+        <v>7</v>
       </c>
       <c r="Q623">
-        <v>0</v>
+        <v>-1.25</v>
       </c>
       <c r="R623">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="S623">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="T623">
         <v>2.75</v>
       </c>
       <c r="U623">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V623">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="W623">
         <v>-1</v>
       </c>
       <c r="X623">
-        <v>2.4</v>
+        <v>3.5</v>
       </c>
       <c r="Y623">
         <v>-1</v>
       </c>
       <c r="Z623">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA623">
-        <v>-0</v>
+        <v>0.95</v>
       </c>
       <c r="AB623">
         <v>-1</v>
       </c>
       <c r="AC623">
-        <v>0.875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="624" spans="1:29">
@@ -56704,7 +56704,7 @@
         <v>630</v>
       </c>
       <c r="B632">
-        <v>5208691</v>
+        <v>5208561</v>
       </c>
       <c r="C632" t="s">
         <v>28</v>
@@ -56716,49 +56716,49 @@
         <v>44933.59375</v>
       </c>
       <c r="F632" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G632" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H632">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I632">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J632" t="s">
         <v>51</v>
       </c>
       <c r="K632">
-        <v>1.95</v>
+        <v>1.75</v>
       </c>
       <c r="L632">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="M632">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="N632">
-        <v>2.15</v>
+        <v>1.7</v>
       </c>
       <c r="O632">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="P632">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="Q632">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R632">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="S632">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="T632">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U632">
         <v>1.925</v>
@@ -56773,19 +56773,19 @@
         <v>-1</v>
       </c>
       <c r="Y632">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="Z632">
         <v>-1</v>
       </c>
       <c r="AA632">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AB632">
         <v>0.925</v>
       </c>
-      <c r="AB632">
-        <v>-1</v>
-      </c>
       <c r="AC632">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="633" spans="1:29">
@@ -56793,7 +56793,7 @@
         <v>631</v>
       </c>
       <c r="B633">
-        <v>5208561</v>
+        <v>5208691</v>
       </c>
       <c r="C633" t="s">
         <v>28</v>
@@ -56805,49 +56805,49 @@
         <v>44933.59375</v>
       </c>
       <c r="F633" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G633" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H633">
+        <v>0</v>
+      </c>
+      <c r="I633">
         <v>1</v>
-      </c>
-      <c r="I633">
-        <v>2</v>
       </c>
       <c r="J633" t="s">
         <v>51</v>
       </c>
       <c r="K633">
-        <v>1.75</v>
+        <v>1.95</v>
       </c>
       <c r="L633">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="M633">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="N633">
-        <v>1.7</v>
+        <v>2.15</v>
       </c>
       <c r="O633">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="P633">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="Q633">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R633">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="S633">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="T633">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U633">
         <v>1.925</v>
@@ -56862,19 +56862,19 @@
         <v>-1</v>
       </c>
       <c r="Y633">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="Z633">
         <v>-1</v>
       </c>
       <c r="AA633">
-        <v>0.8500000000000001</v>
+        <v>0.925</v>
       </c>
       <c r="AB633">
+        <v>-1</v>
+      </c>
+      <c r="AC633">
         <v>0.925</v>
-      </c>
-      <c r="AC633">
-        <v>-1</v>
       </c>
     </row>
     <row r="634" spans="1:29">
@@ -58395,7 +58395,7 @@
         <v>649</v>
       </c>
       <c r="B651">
-        <v>5208701</v>
+        <v>5208571</v>
       </c>
       <c r="C651" t="s">
         <v>28</v>
@@ -58407,76 +58407,76 @@
         <v>44944.60416666666</v>
       </c>
       <c r="F651" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G651" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H651">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I651">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J651" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K651">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
       <c r="L651">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="M651">
-        <v>2.05</v>
+        <v>1.75</v>
       </c>
       <c r="N651">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="O651">
-        <v>3.3</v>
+        <v>3.8</v>
       </c>
       <c r="P651">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="Q651">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="R651">
-        <v>2.05</v>
+        <v>1.975</v>
       </c>
       <c r="S651">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="T651">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U651">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="V651">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="W651">
         <v>-1</v>
       </c>
       <c r="X651">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Y651">
-        <v>-1</v>
+        <v>0.7</v>
       </c>
       <c r="Z651">
-        <v>0.5249999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA651">
+        <v>0.875</v>
+      </c>
+      <c r="AB651">
+        <v>0.5</v>
+      </c>
+      <c r="AC651">
         <v>-0.5</v>
-      </c>
-      <c r="AB651">
-        <v>-1</v>
-      </c>
-      <c r="AC651">
-        <v>0.8</v>
       </c>
     </row>
     <row r="652" spans="1:29">
@@ -58484,7 +58484,7 @@
         <v>650</v>
       </c>
       <c r="B652">
-        <v>5208571</v>
+        <v>5208701</v>
       </c>
       <c r="C652" t="s">
         <v>28</v>
@@ -58496,76 +58496,76 @@
         <v>44944.60416666666</v>
       </c>
       <c r="F652" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G652" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H652">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I652">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J652" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K652">
-        <v>4.2</v>
+        <v>3.3</v>
       </c>
       <c r="L652">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="M652">
-        <v>1.75</v>
+        <v>2.05</v>
       </c>
       <c r="N652">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="O652">
-        <v>3.8</v>
+        <v>3.3</v>
       </c>
       <c r="P652">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="Q652">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="R652">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="S652">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="T652">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U652">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="V652">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="W652">
         <v>-1</v>
       </c>
       <c r="X652">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Y652">
-        <v>0.7</v>
+        <v>-1</v>
       </c>
       <c r="Z652">
-        <v>-1</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AA652">
-        <v>0.875</v>
+        <v>-0.5</v>
       </c>
       <c r="AB652">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="AC652">
-        <v>-0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="653" spans="1:29">
@@ -59018,7 +59018,7 @@
         <v>656</v>
       </c>
       <c r="B658">
-        <v>5208577</v>
+        <v>5208575</v>
       </c>
       <c r="C658" t="s">
         <v>28</v>
@@ -59030,40 +59030,40 @@
         <v>44947.59375</v>
       </c>
       <c r="F658" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G658" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H658">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I658">
         <v>2</v>
       </c>
       <c r="J658" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K658">
-        <v>2.625</v>
+        <v>1.95</v>
       </c>
       <c r="L658">
+        <v>3.5</v>
+      </c>
+      <c r="M658">
         <v>3.4</v>
       </c>
-      <c r="M658">
-        <v>2.4</v>
-      </c>
       <c r="N658">
-        <v>3.2</v>
+        <v>1.75</v>
       </c>
       <c r="O658">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="P658">
-        <v>2.05</v>
+        <v>4</v>
       </c>
       <c r="Q658">
-        <v>0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R658">
         <v>2.025</v>
@@ -59072,34 +59072,34 @@
         <v>1.825</v>
       </c>
       <c r="T658">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U658">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="V658">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="W658">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="X658">
         <v>-1</v>
       </c>
       <c r="Y658">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z658">
-        <v>-1</v>
+        <v>0.5125</v>
       </c>
       <c r="AA658">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
       <c r="AB658">
-        <v>0.475</v>
+        <v>1</v>
       </c>
       <c r="AC658">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="659" spans="1:29">
@@ -59107,7 +59107,7 @@
         <v>657</v>
       </c>
       <c r="B659">
-        <v>5208575</v>
+        <v>5208577</v>
       </c>
       <c r="C659" t="s">
         <v>28</v>
@@ -59119,40 +59119,40 @@
         <v>44947.59375</v>
       </c>
       <c r="F659" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G659" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H659">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I659">
         <v>2</v>
       </c>
       <c r="J659" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K659">
-        <v>1.95</v>
+        <v>2.625</v>
       </c>
       <c r="L659">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M659">
+        <v>2.4</v>
+      </c>
+      <c r="N659">
+        <v>3.2</v>
+      </c>
+      <c r="O659">
         <v>3.4</v>
       </c>
-      <c r="N659">
-        <v>1.75</v>
-      </c>
-      <c r="O659">
-        <v>3.6</v>
-      </c>
       <c r="P659">
-        <v>4</v>
+        <v>2.05</v>
       </c>
       <c r="Q659">
-        <v>-0.75</v>
+        <v>0.25</v>
       </c>
       <c r="R659">
         <v>2.025</v>
@@ -59161,34 +59161,34 @@
         <v>1.825</v>
       </c>
       <c r="T659">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U659">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="V659">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="W659">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="X659">
         <v>-1</v>
       </c>
       <c r="Y659">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z659">
-        <v>0.5125</v>
+        <v>-1</v>
       </c>
       <c r="AA659">
+        <v>0.825</v>
+      </c>
+      <c r="AB659">
+        <v>0.475</v>
+      </c>
+      <c r="AC659">
         <v>-0.5</v>
-      </c>
-      <c r="AB659">
-        <v>1</v>
-      </c>
-      <c r="AC659">
-        <v>-1</v>
       </c>
     </row>
     <row r="660" spans="1:29">
@@ -59819,7 +59819,7 @@
         <v>665</v>
       </c>
       <c r="B667">
-        <v>5208580</v>
+        <v>5208579</v>
       </c>
       <c r="C667" t="s">
         <v>28</v>
@@ -59831,34 +59831,34 @@
         <v>44954.59375</v>
       </c>
       <c r="F667" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G667" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H667">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I667">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J667" t="s">
         <v>53</v>
       </c>
       <c r="K667">
-        <v>2.05</v>
+        <v>2.15</v>
       </c>
       <c r="L667">
         <v>3.4</v>
       </c>
       <c r="M667">
+        <v>3</v>
+      </c>
+      <c r="N667">
+        <v>2.2</v>
+      </c>
+      <c r="O667">
         <v>3.2</v>
-      </c>
-      <c r="N667">
-        <v>2.1</v>
-      </c>
-      <c r="O667">
-        <v>3.4</v>
       </c>
       <c r="P667">
         <v>3.1</v>
@@ -59867,25 +59867,25 @@
         <v>-0.25</v>
       </c>
       <c r="R667">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="S667">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="T667">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="U667">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="V667">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="W667">
         <v>-1</v>
       </c>
       <c r="X667">
-        <v>2.4</v>
+        <v>2.2</v>
       </c>
       <c r="Y667">
         <v>-1</v>
@@ -59894,13 +59894,13 @@
         <v>-0.5</v>
       </c>
       <c r="AA667">
-        <v>0.475</v>
+        <v>0.4375</v>
       </c>
       <c r="AB667">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
       <c r="AC667">
-        <v>-1</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="668" spans="1:29">
@@ -59908,7 +59908,7 @@
         <v>666</v>
       </c>
       <c r="B668">
-        <v>5208579</v>
+        <v>5208580</v>
       </c>
       <c r="C668" t="s">
         <v>28</v>
@@ -59920,34 +59920,34 @@
         <v>44954.59375</v>
       </c>
       <c r="F668" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G668" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H668">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I668">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J668" t="s">
         <v>53</v>
       </c>
       <c r="K668">
-        <v>2.15</v>
+        <v>2.05</v>
       </c>
       <c r="L668">
         <v>3.4</v>
       </c>
       <c r="M668">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="N668">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="O668">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="P668">
         <v>3.1</v>
@@ -59956,25 +59956,25 @@
         <v>-0.25</v>
       </c>
       <c r="R668">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="S668">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="T668">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="U668">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="V668">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="W668">
         <v>-1</v>
       </c>
       <c r="X668">
-        <v>2.2</v>
+        <v>2.4</v>
       </c>
       <c r="Y668">
         <v>-1</v>
@@ -59983,13 +59983,13 @@
         <v>-0.5</v>
       </c>
       <c r="AA668">
-        <v>0.4375</v>
+        <v>0.475</v>
       </c>
       <c r="AB668">
-        <v>-0.5</v>
+        <v>0.825</v>
       </c>
       <c r="AC668">
-        <v>0.4375</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="669" spans="1:29">
@@ -61421,7 +61421,7 @@
         <v>683</v>
       </c>
       <c r="B685">
-        <v>5208587</v>
+        <v>5208718</v>
       </c>
       <c r="C685" t="s">
         <v>28</v>
@@ -61433,76 +61433,76 @@
         <v>44967.69791666666</v>
       </c>
       <c r="F685" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="G685" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="H685">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I685">
         <v>1</v>
       </c>
       <c r="J685" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K685">
-        <v>2.3</v>
+        <v>2.55</v>
       </c>
       <c r="L685">
         <v>3.4</v>
       </c>
       <c r="M685">
-        <v>2.9</v>
+        <v>2.45</v>
       </c>
       <c r="N685">
+        <v>2.55</v>
+      </c>
+      <c r="O685">
+        <v>3.4</v>
+      </c>
+      <c r="P685">
         <v>2.5</v>
-      </c>
-      <c r="O685">
-        <v>3.2</v>
-      </c>
-      <c r="P685">
-        <v>2.8</v>
       </c>
       <c r="Q685">
         <v>0</v>
       </c>
       <c r="R685">
+        <v>1.95</v>
+      </c>
+      <c r="S685">
+        <v>1.9</v>
+      </c>
+      <c r="T685">
+        <v>2.75</v>
+      </c>
+      <c r="U685">
+        <v>1.975</v>
+      </c>
+      <c r="V685">
         <v>1.875</v>
       </c>
-      <c r="S685">
-        <v>1.975</v>
-      </c>
-      <c r="T685">
-        <v>2.25</v>
-      </c>
-      <c r="U685">
-        <v>1.8</v>
-      </c>
-      <c r="V685">
-        <v>2.05</v>
-      </c>
       <c r="W685">
-        <v>-1</v>
+        <v>1.55</v>
       </c>
       <c r="X685">
-        <v>2.2</v>
+        <v>-1</v>
       </c>
       <c r="Y685">
         <v>-1</v>
       </c>
       <c r="Z685">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AA685">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="AB685">
+        <v>0.4875</v>
+      </c>
+      <c r="AC685">
         <v>-0.5</v>
-      </c>
-      <c r="AC685">
-        <v>0.5249999999999999</v>
       </c>
     </row>
     <row r="686" spans="1:29">
@@ -61510,7 +61510,7 @@
         <v>684</v>
       </c>
       <c r="B686">
-        <v>5208718</v>
+        <v>5208587</v>
       </c>
       <c r="C686" t="s">
         <v>28</v>
@@ -61522,76 +61522,76 @@
         <v>44967.69791666666</v>
       </c>
       <c r="F686" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="G686" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="H686">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I686">
         <v>1</v>
       </c>
       <c r="J686" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K686">
-        <v>2.55</v>
+        <v>2.3</v>
       </c>
       <c r="L686">
         <v>3.4</v>
       </c>
       <c r="M686">
-        <v>2.45</v>
+        <v>2.9</v>
       </c>
       <c r="N686">
-        <v>2.55</v>
+        <v>2.5</v>
       </c>
       <c r="O686">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="P686">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="Q686">
         <v>0</v>
       </c>
       <c r="R686">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="S686">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="T686">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="U686">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="V686">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="W686">
-        <v>1.55</v>
+        <v>-1</v>
       </c>
       <c r="X686">
-        <v>-1</v>
+        <v>2.2</v>
       </c>
       <c r="Y686">
         <v>-1</v>
       </c>
       <c r="Z686">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="AA686">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="AB686">
-        <v>0.4875</v>
+        <v>-0.5</v>
       </c>
       <c r="AC686">
-        <v>-0.5</v>
+        <v>0.5249999999999999</v>
       </c>
     </row>
     <row r="687" spans="1:29">
@@ -87092,19 +87092,19 @@
         <v>0.5</v>
       </c>
       <c r="R973">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="S973">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="T973">
         <v>2.75</v>
       </c>
       <c r="U973">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="V973">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="W973">
         <v>0</v>
@@ -87154,13 +87154,13 @@
         <v>17</v>
       </c>
       <c r="N974">
-        <v>1.125</v>
+        <v>1.142</v>
       </c>
       <c r="O974">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="P974">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q974">
         <v>-2.25</v>
@@ -87193,6 +87193,450 @@
         <v>0</v>
       </c>
       <c r="AA974">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="975" spans="1:29">
+      <c r="A975" s="1">
+        <v>973</v>
+      </c>
+      <c r="B975">
+        <v>6810165</v>
+      </c>
+      <c r="C975" t="s">
+        <v>28</v>
+      </c>
+      <c r="D975" t="s">
+        <v>28</v>
+      </c>
+      <c r="E975" s="2">
+        <v>45322.61458333334</v>
+      </c>
+      <c r="F975" t="s">
+        <v>41</v>
+      </c>
+      <c r="G975" t="s">
+        <v>29</v>
+      </c>
+      <c r="K975">
+        <v>1.6</v>
+      </c>
+      <c r="L975">
+        <v>4</v>
+      </c>
+      <c r="M975">
+        <v>5</v>
+      </c>
+      <c r="N975">
+        <v>1.6</v>
+      </c>
+      <c r="O975">
+        <v>4</v>
+      </c>
+      <c r="P975">
+        <v>5</v>
+      </c>
+      <c r="Q975">
+        <v>-1</v>
+      </c>
+      <c r="R975">
+        <v>2.05</v>
+      </c>
+      <c r="S975">
+        <v>1.8</v>
+      </c>
+      <c r="T975">
+        <v>2.75</v>
+      </c>
+      <c r="U975">
+        <v>1.95</v>
+      </c>
+      <c r="V975">
+        <v>1.9</v>
+      </c>
+      <c r="W975">
+        <v>0</v>
+      </c>
+      <c r="X975">
+        <v>0</v>
+      </c>
+      <c r="Y975">
+        <v>0</v>
+      </c>
+      <c r="Z975">
+        <v>0</v>
+      </c>
+      <c r="AA975">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="976" spans="1:29">
+      <c r="A976" s="1">
+        <v>974</v>
+      </c>
+      <c r="B976">
+        <v>6810168</v>
+      </c>
+      <c r="C976" t="s">
+        <v>28</v>
+      </c>
+      <c r="D976" t="s">
+        <v>28</v>
+      </c>
+      <c r="E976" s="2">
+        <v>45322.61458333334</v>
+      </c>
+      <c r="F976" t="s">
+        <v>36</v>
+      </c>
+      <c r="G976" t="s">
+        <v>46</v>
+      </c>
+      <c r="K976">
+        <v>4.5</v>
+      </c>
+      <c r="L976">
+        <v>4.2</v>
+      </c>
+      <c r="M976">
+        <v>1.666</v>
+      </c>
+      <c r="N976">
+        <v>4.75</v>
+      </c>
+      <c r="O976">
+        <v>4.2</v>
+      </c>
+      <c r="P976">
+        <v>1.615</v>
+      </c>
+      <c r="Q976">
+        <v>0.75</v>
+      </c>
+      <c r="R976">
+        <v>2.05</v>
+      </c>
+      <c r="S976">
+        <v>1.8</v>
+      </c>
+      <c r="T976">
+        <v>3</v>
+      </c>
+      <c r="U976">
+        <v>1.925</v>
+      </c>
+      <c r="V976">
+        <v>1.925</v>
+      </c>
+      <c r="W976">
+        <v>0</v>
+      </c>
+      <c r="X976">
+        <v>0</v>
+      </c>
+      <c r="Y976">
+        <v>0</v>
+      </c>
+      <c r="Z976">
+        <v>0</v>
+      </c>
+      <c r="AA976">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="977" spans="1:27">
+      <c r="A977" s="1">
+        <v>975</v>
+      </c>
+      <c r="B977">
+        <v>6810164</v>
+      </c>
+      <c r="C977" t="s">
+        <v>28</v>
+      </c>
+      <c r="D977" t="s">
+        <v>28</v>
+      </c>
+      <c r="E977" s="2">
+        <v>45322.70833333334</v>
+      </c>
+      <c r="F977" t="s">
+        <v>48</v>
+      </c>
+      <c r="G977" t="s">
+        <v>50</v>
+      </c>
+      <c r="K977">
+        <v>1.2</v>
+      </c>
+      <c r="L977">
+        <v>7</v>
+      </c>
+      <c r="M977">
+        <v>12</v>
+      </c>
+      <c r="N977">
+        <v>1.2</v>
+      </c>
+      <c r="O977">
+        <v>7</v>
+      </c>
+      <c r="P977">
+        <v>12</v>
+      </c>
+      <c r="Q977">
+        <v>-2</v>
+      </c>
+      <c r="R977">
+        <v>1.95</v>
+      </c>
+      <c r="S977">
+        <v>1.9</v>
+      </c>
+      <c r="T977">
+        <v>3.25</v>
+      </c>
+      <c r="U977">
+        <v>1.9</v>
+      </c>
+      <c r="V977">
+        <v>1.95</v>
+      </c>
+      <c r="W977">
+        <v>0</v>
+      </c>
+      <c r="X977">
+        <v>0</v>
+      </c>
+      <c r="Y977">
+        <v>0</v>
+      </c>
+      <c r="Z977">
+        <v>0</v>
+      </c>
+      <c r="AA977">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="978" spans="1:27">
+      <c r="A978" s="1">
+        <v>976</v>
+      </c>
+      <c r="B978">
+        <v>6810162</v>
+      </c>
+      <c r="C978" t="s">
+        <v>28</v>
+      </c>
+      <c r="D978" t="s">
+        <v>28</v>
+      </c>
+      <c r="E978" s="2">
+        <v>45322.70833333334</v>
+      </c>
+      <c r="F978" t="s">
+        <v>38</v>
+      </c>
+      <c r="G978" t="s">
+        <v>44</v>
+      </c>
+      <c r="K978">
+        <v>4</v>
+      </c>
+      <c r="L978">
+        <v>3.6</v>
+      </c>
+      <c r="M978">
+        <v>1.85</v>
+      </c>
+      <c r="N978">
+        <v>4</v>
+      </c>
+      <c r="O978">
+        <v>3.6</v>
+      </c>
+      <c r="P978">
+        <v>1.85</v>
+      </c>
+      <c r="Q978">
+        <v>0.5</v>
+      </c>
+      <c r="R978">
+        <v>1.925</v>
+      </c>
+      <c r="S978">
+        <v>1.925</v>
+      </c>
+      <c r="T978">
+        <v>2.5</v>
+      </c>
+      <c r="U978">
+        <v>1.9</v>
+      </c>
+      <c r="V978">
+        <v>1.95</v>
+      </c>
+      <c r="W978">
+        <v>0</v>
+      </c>
+      <c r="X978">
+        <v>0</v>
+      </c>
+      <c r="Y978">
+        <v>0</v>
+      </c>
+      <c r="Z978">
+        <v>0</v>
+      </c>
+      <c r="AA978">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="979" spans="1:27">
+      <c r="A979" s="1">
+        <v>977</v>
+      </c>
+      <c r="B979">
+        <v>6810163</v>
+      </c>
+      <c r="C979" t="s">
+        <v>28</v>
+      </c>
+      <c r="D979" t="s">
+        <v>28</v>
+      </c>
+      <c r="E979" s="2">
+        <v>45323.6875</v>
+      </c>
+      <c r="F979" t="s">
+        <v>37</v>
+      </c>
+      <c r="G979" t="s">
+        <v>42</v>
+      </c>
+      <c r="K979">
+        <v>3.6</v>
+      </c>
+      <c r="L979">
+        <v>3.6</v>
+      </c>
+      <c r="M979">
+        <v>1.95</v>
+      </c>
+      <c r="N979">
+        <v>3.6</v>
+      </c>
+      <c r="O979">
+        <v>3.6</v>
+      </c>
+      <c r="P979">
+        <v>1.95</v>
+      </c>
+      <c r="Q979">
+        <v>0.5</v>
+      </c>
+      <c r="R979">
+        <v>1.85</v>
+      </c>
+      <c r="S979">
+        <v>2</v>
+      </c>
+      <c r="T979">
+        <v>2.5</v>
+      </c>
+      <c r="U979">
+        <v>1.9</v>
+      </c>
+      <c r="V979">
+        <v>1.95</v>
+      </c>
+      <c r="W979">
+        <v>0</v>
+      </c>
+      <c r="X979">
+        <v>0</v>
+      </c>
+      <c r="Y979">
+        <v>0</v>
+      </c>
+      <c r="Z979">
+        <v>0</v>
+      </c>
+      <c r="AA979">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="980" spans="1:27">
+      <c r="A980" s="1">
+        <v>978</v>
+      </c>
+      <c r="B980">
+        <v>6810166</v>
+      </c>
+      <c r="C980" t="s">
+        <v>28</v>
+      </c>
+      <c r="D980" t="s">
+        <v>28</v>
+      </c>
+      <c r="E980" s="2">
+        <v>45323.6875</v>
+      </c>
+      <c r="F980" t="s">
+        <v>34</v>
+      </c>
+      <c r="G980" t="s">
+        <v>43</v>
+      </c>
+      <c r="K980">
+        <v>3.5</v>
+      </c>
+      <c r="L980">
+        <v>3.5</v>
+      </c>
+      <c r="M980">
+        <v>2</v>
+      </c>
+      <c r="N980">
+        <v>3.4</v>
+      </c>
+      <c r="O980">
+        <v>3.5</v>
+      </c>
+      <c r="P980">
+        <v>2.05</v>
+      </c>
+      <c r="Q980">
+        <v>0.25</v>
+      </c>
+      <c r="R980">
+        <v>2.05</v>
+      </c>
+      <c r="S980">
+        <v>1.8</v>
+      </c>
+      <c r="T980">
+        <v>2.5</v>
+      </c>
+      <c r="U980">
+        <v>1.975</v>
+      </c>
+      <c r="V980">
+        <v>1.875</v>
+      </c>
+      <c r="W980">
+        <v>0</v>
+      </c>
+      <c r="X980">
+        <v>0</v>
+      </c>
+      <c r="Y980">
+        <v>0</v>
+      </c>
+      <c r="Z980">
+        <v>0</v>
+      </c>
+      <c r="AA980">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-02-02 às 20:58
</commit_message>
<xml_diff>
--- a/Belgium First Division A/Belgium First Division A.xlsx
+++ b/Belgium First Division A/Belgium First Division A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -109,10 +109,10 @@
     <t>Eupen</t>
   </si>
   <si>
-    <t>KV Oostende</t>
+    <t>Cercle Brugge</t>
   </si>
   <si>
-    <t>Cercle Brugge</t>
+    <t>KV Oostende</t>
   </si>
   <si>
     <t>Antwerp</t>
@@ -528,7 +528,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC360"/>
+  <dimension ref="A1:AC361"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -803,7 +803,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5208561</v>
+        <v>5208691</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -818,46 +818,46 @@
         <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>1</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
       </c>
       <c r="J4" t="s">
         <v>49</v>
       </c>
       <c r="K4">
-        <v>1.75</v>
+        <v>1.95</v>
       </c>
       <c r="L4">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="M4">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="N4">
-        <v>1.7</v>
+        <v>2.15</v>
       </c>
       <c r="O4">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="P4">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="Q4">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R4">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="S4">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="T4">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U4">
         <v>1.925</v>
@@ -872,19 +872,19 @@
         <v>-1</v>
       </c>
       <c r="Y4">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="Z4">
         <v>-1</v>
       </c>
       <c r="AA4">
-        <v>0.8500000000000001</v>
+        <v>0.925</v>
       </c>
       <c r="AB4">
+        <v>-1</v>
+      </c>
+      <c r="AC4">
         <v>0.925</v>
-      </c>
-      <c r="AC4">
-        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:29">
@@ -892,7 +892,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5208691</v>
+        <v>5208561</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -907,46 +907,46 @@
         <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5" t="s">
         <v>49</v>
       </c>
       <c r="K5">
-        <v>1.95</v>
+        <v>1.75</v>
       </c>
       <c r="L5">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="M5">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="N5">
-        <v>2.15</v>
+        <v>1.7</v>
       </c>
       <c r="O5">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="P5">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="Q5">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R5">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="S5">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="T5">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U5">
         <v>1.925</v>
@@ -961,19 +961,19 @@
         <v>-1</v>
       </c>
       <c r="Y5">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="Z5">
         <v>-1</v>
       </c>
       <c r="AA5">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AB5">
         <v>0.925</v>
       </c>
-      <c r="AB5">
-        <v>-1</v>
-      </c>
       <c r="AC5">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:29">
@@ -1708,7 +1708,7 @@
         <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -2153,7 +2153,7 @@
         <v>44</v>
       </c>
       <c r="G19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -2494,7 +2494,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>5208571</v>
+        <v>5208701</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
@@ -2509,73 +2509,73 @@
         <v>31</v>
       </c>
       <c r="G23" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K23">
-        <v>4.2</v>
+        <v>3.3</v>
       </c>
       <c r="L23">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="M23">
-        <v>1.75</v>
+        <v>2.05</v>
       </c>
       <c r="N23">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="O23">
-        <v>3.8</v>
+        <v>3.3</v>
       </c>
       <c r="P23">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="Q23">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="R23">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="S23">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="T23">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U23">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="V23">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="W23">
         <v>-1</v>
       </c>
       <c r="X23">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Y23">
-        <v>0.7</v>
+        <v>-1</v>
       </c>
       <c r="Z23">
-        <v>-1</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AA23">
-        <v>0.875</v>
+        <v>-0.5</v>
       </c>
       <c r="AB23">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="AC23">
-        <v>-0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="24" spans="1:29">
@@ -2583,7 +2583,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>5208701</v>
+        <v>5208571</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
@@ -2598,73 +2598,73 @@
         <v>32</v>
       </c>
       <c r="G24" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K24">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
       <c r="L24">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="M24">
-        <v>2.05</v>
+        <v>1.75</v>
       </c>
       <c r="N24">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="O24">
-        <v>3.3</v>
+        <v>3.8</v>
       </c>
       <c r="P24">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="Q24">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="R24">
-        <v>2.05</v>
+        <v>1.975</v>
       </c>
       <c r="S24">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="T24">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U24">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="V24">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="W24">
         <v>-1</v>
       </c>
       <c r="X24">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Y24">
-        <v>-1</v>
+        <v>0.7</v>
       </c>
       <c r="Z24">
-        <v>0.5249999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA24">
+        <v>0.875</v>
+      </c>
+      <c r="AB24">
+        <v>0.5</v>
+      </c>
+      <c r="AC24">
         <v>-0.5</v>
-      </c>
-      <c r="AB24">
-        <v>-1</v>
-      </c>
-      <c r="AC24">
-        <v>0.8</v>
       </c>
     </row>
     <row r="25" spans="1:29">
@@ -2672,7 +2672,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>5208568</v>
+        <v>5208569</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
@@ -2684,73 +2684,73 @@
         <v>44944.69791666666</v>
       </c>
       <c r="F25" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G25" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K25">
-        <v>1.4</v>
+        <v>1.85</v>
       </c>
       <c r="L25">
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="M25">
-        <v>6.5</v>
+        <v>3.8</v>
       </c>
       <c r="N25">
-        <v>1.7</v>
+        <v>1.666</v>
       </c>
       <c r="O25">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P25">
-        <v>4.333</v>
+        <v>4.75</v>
       </c>
       <c r="Q25">
         <v>-0.75</v>
       </c>
       <c r="R25">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="S25">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="T25">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U25">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="V25">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="W25">
-        <v>-1</v>
+        <v>0.6659999999999999</v>
       </c>
       <c r="X25">
         <v>-1</v>
       </c>
       <c r="Y25">
-        <v>3.333</v>
+        <v>-1</v>
       </c>
       <c r="Z25">
-        <v>-1</v>
+        <v>0.4375</v>
       </c>
       <c r="AA25">
-        <v>0.925</v>
+        <v>-0.5</v>
       </c>
       <c r="AB25">
-        <v>0.9750000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="AC25">
         <v>-1</v>
@@ -2761,7 +2761,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>5208569</v>
+        <v>5208568</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
@@ -2773,73 +2773,73 @@
         <v>44944.69791666666</v>
       </c>
       <c r="F26" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26">
         <v>3</v>
       </c>
-      <c r="I26">
-        <v>2</v>
-      </c>
       <c r="J26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K26">
-        <v>1.85</v>
+        <v>1.4</v>
       </c>
       <c r="L26">
-        <v>3.75</v>
+        <v>5</v>
       </c>
       <c r="M26">
-        <v>3.8</v>
+        <v>6.5</v>
       </c>
       <c r="N26">
-        <v>1.666</v>
+        <v>1.7</v>
       </c>
       <c r="O26">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P26">
-        <v>4.75</v>
+        <v>4.333</v>
       </c>
       <c r="Q26">
         <v>-0.75</v>
       </c>
       <c r="R26">
+        <v>1.925</v>
+      </c>
+      <c r="S26">
+        <v>1.925</v>
+      </c>
+      <c r="T26">
+        <v>2.75</v>
+      </c>
+      <c r="U26">
+        <v>1.975</v>
+      </c>
+      <c r="V26">
         <v>1.875</v>
       </c>
-      <c r="S26">
-        <v>1.975</v>
-      </c>
-      <c r="T26">
-        <v>2.5</v>
-      </c>
-      <c r="U26">
-        <v>1.95</v>
-      </c>
-      <c r="V26">
-        <v>1.9</v>
-      </c>
       <c r="W26">
-        <v>0.6659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X26">
         <v>-1</v>
       </c>
       <c r="Y26">
-        <v>-1</v>
+        <v>3.333</v>
       </c>
       <c r="Z26">
-        <v>0.4375</v>
+        <v>-1</v>
       </c>
       <c r="AA26">
-        <v>-0.5</v>
+        <v>0.925</v>
       </c>
       <c r="AB26">
-        <v>0.95</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC26">
         <v>-1</v>
@@ -3218,10 +3218,10 @@
         <v>44947.59375</v>
       </c>
       <c r="F31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" t="s">
         <v>31</v>
-      </c>
-      <c r="G31" t="s">
-        <v>32</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -3918,7 +3918,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>5208579</v>
+        <v>5208580</v>
       </c>
       <c r="C39" t="s">
         <v>28</v>
@@ -3930,34 +3930,34 @@
         <v>44954.59375</v>
       </c>
       <c r="F39" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G39" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J39" t="s">
         <v>48</v>
       </c>
       <c r="K39">
-        <v>2.15</v>
+        <v>2.05</v>
       </c>
       <c r="L39">
         <v>3.4</v>
       </c>
       <c r="M39">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="N39">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="O39">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="P39">
         <v>3.1</v>
@@ -3966,25 +3966,25 @@
         <v>-0.25</v>
       </c>
       <c r="R39">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="S39">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="T39">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="U39">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="V39">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="W39">
         <v>-1</v>
       </c>
       <c r="X39">
-        <v>2.2</v>
+        <v>2.4</v>
       </c>
       <c r="Y39">
         <v>-1</v>
@@ -3993,13 +3993,13 @@
         <v>-0.5</v>
       </c>
       <c r="AA39">
-        <v>0.4375</v>
+        <v>0.475</v>
       </c>
       <c r="AB39">
-        <v>-0.5</v>
+        <v>0.825</v>
       </c>
       <c r="AC39">
-        <v>0.4375</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="40" spans="1:29">
@@ -4007,7 +4007,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>5208580</v>
+        <v>5208579</v>
       </c>
       <c r="C40" t="s">
         <v>28</v>
@@ -4019,34 +4019,34 @@
         <v>44954.59375</v>
       </c>
       <c r="F40" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G40" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="H40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J40" t="s">
         <v>48</v>
       </c>
       <c r="K40">
-        <v>2.05</v>
+        <v>2.15</v>
       </c>
       <c r="L40">
         <v>3.4</v>
       </c>
       <c r="M40">
+        <v>3</v>
+      </c>
+      <c r="N40">
+        <v>2.2</v>
+      </c>
+      <c r="O40">
         <v>3.2</v>
-      </c>
-      <c r="N40">
-        <v>2.1</v>
-      </c>
-      <c r="O40">
-        <v>3.4</v>
       </c>
       <c r="P40">
         <v>3.1</v>
@@ -4055,25 +4055,25 @@
         <v>-0.25</v>
       </c>
       <c r="R40">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="S40">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="T40">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="U40">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="V40">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="W40">
         <v>-1</v>
       </c>
       <c r="X40">
-        <v>2.4</v>
+        <v>2.2</v>
       </c>
       <c r="Y40">
         <v>-1</v>
@@ -4082,13 +4082,13 @@
         <v>-0.5</v>
       </c>
       <c r="AA40">
-        <v>0.475</v>
+        <v>0.4375</v>
       </c>
       <c r="AB40">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
       <c r="AC40">
-        <v>-1</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="41" spans="1:29">
@@ -4286,7 +4286,7 @@
         <v>44955.5</v>
       </c>
       <c r="F43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G43" t="s">
         <v>42</v>
@@ -4642,7 +4642,7 @@
         <v>44960.69791666666</v>
       </c>
       <c r="F47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G47" t="s">
         <v>36</v>
@@ -4731,7 +4731,7 @@
         <v>44961.5</v>
       </c>
       <c r="F48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G48" t="s">
         <v>29</v>
@@ -4808,7 +4808,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>6192614</v>
+        <v>6192613</v>
       </c>
       <c r="C49" t="s">
         <v>28</v>
@@ -4820,76 +4820,76 @@
         <v>44961.59375</v>
       </c>
       <c r="F49" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I49">
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K49">
-        <v>2.55</v>
+        <v>3.25</v>
       </c>
       <c r="L49">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M49">
-        <v>2.45</v>
+        <v>2.05</v>
       </c>
       <c r="N49">
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="O49">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="P49">
-        <v>1.909</v>
+        <v>1.75</v>
       </c>
       <c r="Q49">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="R49">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="S49">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="T49">
         <v>2.5</v>
       </c>
       <c r="U49">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="V49">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="W49">
-        <v>-1</v>
+        <v>3.5</v>
       </c>
       <c r="X49">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y49">
         <v>-1</v>
       </c>
       <c r="Z49">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AA49">
+        <v>-1</v>
+      </c>
+      <c r="AB49">
         <v>0.8999999999999999</v>
       </c>
-      <c r="AA49">
-        <v>-1</v>
-      </c>
-      <c r="AB49">
-        <v>-1</v>
-      </c>
       <c r="AC49">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="50" spans="1:29">
@@ -4897,7 +4897,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>6192613</v>
+        <v>6192614</v>
       </c>
       <c r="C50" t="s">
         <v>28</v>
@@ -4909,76 +4909,76 @@
         <v>44961.59375</v>
       </c>
       <c r="F50" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I50">
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K50">
-        <v>3.25</v>
+        <v>2.55</v>
       </c>
       <c r="L50">
+        <v>3.4</v>
+      </c>
+      <c r="M50">
+        <v>2.45</v>
+      </c>
+      <c r="N50">
+        <v>3.6</v>
+      </c>
+      <c r="O50">
         <v>3.5</v>
       </c>
-      <c r="M50">
-        <v>2.05</v>
-      </c>
-      <c r="N50">
-        <v>4.5</v>
-      </c>
-      <c r="O50">
-        <v>3.75</v>
-      </c>
       <c r="P50">
-        <v>1.75</v>
+        <v>1.909</v>
       </c>
       <c r="Q50">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="R50">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="S50">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="T50">
         <v>2.5</v>
       </c>
       <c r="U50">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="V50">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="W50">
-        <v>3.5</v>
+        <v>-1</v>
       </c>
       <c r="X50">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y50">
         <v>-1</v>
       </c>
       <c r="Z50">
-        <v>0.8500000000000001</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA50">
         <v>-1</v>
       </c>
       <c r="AB50">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC50">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:29">
@@ -5446,7 +5446,7 @@
         <v>37</v>
       </c>
       <c r="G56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -5520,7 +5520,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>5208587</v>
+        <v>5208718</v>
       </c>
       <c r="C57" t="s">
         <v>28</v>
@@ -5532,76 +5532,76 @@
         <v>44967.69791666666</v>
       </c>
       <c r="F57" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G57" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I57">
         <v>1</v>
       </c>
       <c r="J57" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K57">
-        <v>2.3</v>
+        <v>2.55</v>
       </c>
       <c r="L57">
         <v>3.4</v>
       </c>
       <c r="M57">
-        <v>2.9</v>
+        <v>2.45</v>
       </c>
       <c r="N57">
+        <v>2.55</v>
+      </c>
+      <c r="O57">
+        <v>3.4</v>
+      </c>
+      <c r="P57">
         <v>2.5</v>
-      </c>
-      <c r="O57">
-        <v>3.2</v>
-      </c>
-      <c r="P57">
-        <v>2.8</v>
       </c>
       <c r="Q57">
         <v>0</v>
       </c>
       <c r="R57">
+        <v>1.95</v>
+      </c>
+      <c r="S57">
+        <v>1.9</v>
+      </c>
+      <c r="T57">
+        <v>2.75</v>
+      </c>
+      <c r="U57">
+        <v>1.975</v>
+      </c>
+      <c r="V57">
         <v>1.875</v>
       </c>
-      <c r="S57">
-        <v>1.975</v>
-      </c>
-      <c r="T57">
-        <v>2.25</v>
-      </c>
-      <c r="U57">
-        <v>1.8</v>
-      </c>
-      <c r="V57">
-        <v>2.05</v>
-      </c>
       <c r="W57">
-        <v>-1</v>
+        <v>1.55</v>
       </c>
       <c r="X57">
-        <v>2.2</v>
+        <v>-1</v>
       </c>
       <c r="Y57">
         <v>-1</v>
       </c>
       <c r="Z57">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AA57">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="AB57">
+        <v>0.4875</v>
+      </c>
+      <c r="AC57">
         <v>-0.5</v>
-      </c>
-      <c r="AC57">
-        <v>0.5249999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:29">
@@ -5609,7 +5609,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>5208718</v>
+        <v>5208587</v>
       </c>
       <c r="C58" t="s">
         <v>28</v>
@@ -5621,76 +5621,76 @@
         <v>44967.69791666666</v>
       </c>
       <c r="F58" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G58" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I58">
         <v>1</v>
       </c>
       <c r="J58" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K58">
-        <v>2.55</v>
+        <v>2.3</v>
       </c>
       <c r="L58">
         <v>3.4</v>
       </c>
       <c r="M58">
-        <v>2.45</v>
+        <v>2.9</v>
       </c>
       <c r="N58">
-        <v>2.55</v>
+        <v>2.5</v>
       </c>
       <c r="O58">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="P58">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="Q58">
         <v>0</v>
       </c>
       <c r="R58">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="S58">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="T58">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="U58">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="V58">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="W58">
-        <v>1.55</v>
+        <v>-1</v>
       </c>
       <c r="X58">
-        <v>-1</v>
+        <v>2.2</v>
       </c>
       <c r="Y58">
         <v>-1</v>
       </c>
       <c r="Z58">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="AA58">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="AB58">
-        <v>0.4875</v>
+        <v>-0.5</v>
       </c>
       <c r="AC58">
-        <v>-0.5</v>
+        <v>0.5249999999999999</v>
       </c>
     </row>
     <row r="59" spans="1:29">
@@ -6158,7 +6158,7 @@
         <v>35</v>
       </c>
       <c r="G64" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -6511,7 +6511,7 @@
         <v>44975.59375</v>
       </c>
       <c r="F68" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G68" t="s">
         <v>44</v>
@@ -6689,7 +6689,7 @@
         <v>44976.39583333334</v>
       </c>
       <c r="F70" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G70" t="s">
         <v>41</v>
@@ -7226,7 +7226,7 @@
         <v>30</v>
       </c>
       <c r="G76" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H76">
         <v>2</v>
@@ -7315,7 +7315,7 @@
         <v>34</v>
       </c>
       <c r="G77" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H77">
         <v>3</v>
@@ -7846,7 +7846,7 @@
         <v>44988.69791666666</v>
       </c>
       <c r="F83" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G83" t="s">
         <v>41</v>
@@ -8024,7 +8024,7 @@
         <v>44989.59375</v>
       </c>
       <c r="F85" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G85" t="s">
         <v>39</v>
@@ -8828,7 +8828,7 @@
         <v>30</v>
       </c>
       <c r="G94" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H94">
         <v>4</v>
@@ -9362,7 +9362,7 @@
         <v>36</v>
       </c>
       <c r="G100" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H100">
         <v>2</v>
@@ -9448,7 +9448,7 @@
         <v>45002.69791666666</v>
       </c>
       <c r="F101" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G101" t="s">
         <v>34</v>
@@ -9614,7 +9614,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>5208612</v>
+        <v>5208613</v>
       </c>
       <c r="C103" t="s">
         <v>28</v>
@@ -9626,76 +9626,76 @@
         <v>45003.59375</v>
       </c>
       <c r="F103" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G103" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H103">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I103">
+        <v>2</v>
+      </c>
+      <c r="J103" t="s">
+        <v>49</v>
+      </c>
+      <c r="K103">
+        <v>3.3</v>
+      </c>
+      <c r="L103">
+        <v>3.3</v>
+      </c>
+      <c r="M103">
+        <v>2.05</v>
+      </c>
+      <c r="N103">
+        <v>2.8</v>
+      </c>
+      <c r="O103">
+        <v>3.3</v>
+      </c>
+      <c r="P103">
+        <v>2.3</v>
+      </c>
+      <c r="Q103">
+        <v>0.25</v>
+      </c>
+      <c r="R103">
+        <v>1.85</v>
+      </c>
+      <c r="S103">
+        <v>2</v>
+      </c>
+      <c r="T103">
+        <v>2.75</v>
+      </c>
+      <c r="U103">
+        <v>1.9</v>
+      </c>
+      <c r="V103">
+        <v>1.95</v>
+      </c>
+      <c r="W103">
+        <v>-1</v>
+      </c>
+      <c r="X103">
+        <v>-1</v>
+      </c>
+      <c r="Y103">
+        <v>1.3</v>
+      </c>
+      <c r="Z103">
+        <v>-1</v>
+      </c>
+      <c r="AA103">
         <v>1</v>
       </c>
-      <c r="J103" t="s">
-        <v>50</v>
-      </c>
-      <c r="K103">
-        <v>1.45</v>
-      </c>
-      <c r="L103">
-        <v>4</v>
-      </c>
-      <c r="M103">
-        <v>6</v>
-      </c>
-      <c r="N103">
-        <v>1.5</v>
-      </c>
-      <c r="O103">
-        <v>3.75</v>
-      </c>
-      <c r="P103">
-        <v>6.5</v>
-      </c>
-      <c r="Q103">
-        <v>-1</v>
-      </c>
-      <c r="R103">
-        <v>2</v>
-      </c>
-      <c r="S103">
-        <v>1.85</v>
-      </c>
-      <c r="T103">
-        <v>2.25</v>
-      </c>
-      <c r="U103">
-        <v>2.025</v>
-      </c>
-      <c r="V103">
-        <v>1.825</v>
-      </c>
-      <c r="W103">
-        <v>0.5</v>
-      </c>
-      <c r="X103">
-        <v>-1</v>
-      </c>
-      <c r="Y103">
-        <v>-1</v>
-      </c>
-      <c r="Z103">
-        <v>0</v>
-      </c>
-      <c r="AA103">
-        <v>-0</v>
-      </c>
       <c r="AB103">
-        <v>1.025</v>
+        <v>0.45</v>
       </c>
       <c r="AC103">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="104" spans="1:29">
@@ -9703,7 +9703,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>5208613</v>
+        <v>5208612</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9715,76 +9715,76 @@
         <v>45003.59375</v>
       </c>
       <c r="F104" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="G104" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H104">
+        <v>2</v>
+      </c>
+      <c r="I104">
         <v>1</v>
       </c>
-      <c r="I104">
-        <v>2</v>
-      </c>
       <c r="J104" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K104">
-        <v>3.3</v>
+        <v>1.45</v>
       </c>
       <c r="L104">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="M104">
-        <v>2.05</v>
+        <v>6</v>
       </c>
       <c r="N104">
-        <v>2.8</v>
+        <v>1.5</v>
       </c>
       <c r="O104">
-        <v>3.3</v>
+        <v>3.75</v>
       </c>
       <c r="P104">
-        <v>2.3</v>
+        <v>6.5</v>
       </c>
       <c r="Q104">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="R104">
+        <v>2</v>
+      </c>
+      <c r="S104">
         <v>1.85</v>
       </c>
-      <c r="S104">
-        <v>2</v>
-      </c>
       <c r="T104">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="U104">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="V104">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="W104">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA104">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="AB104">
-        <v>0.45</v>
+        <v>1.025</v>
       </c>
       <c r="AC104">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -10338,7 +10338,7 @@
         <v>45017.45833333334</v>
       </c>
       <c r="F111" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G111" t="s">
         <v>45</v>
@@ -10605,7 +10605,7 @@
         <v>45017.65625</v>
       </c>
       <c r="F114" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G114" t="s">
         <v>29</v>
@@ -11587,7 +11587,7 @@
         <v>33</v>
       </c>
       <c r="G125" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H125">
         <v>2</v>
@@ -11765,7 +11765,7 @@
         <v>46</v>
       </c>
       <c r="G127" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H127">
         <v>5</v>
@@ -12017,7 +12017,7 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>5424405</v>
+        <v>5424406</v>
       </c>
       <c r="C130" t="s">
         <v>28</v>
@@ -12032,70 +12032,70 @@
         <v>32</v>
       </c>
       <c r="G130" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H130">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I130">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J130" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K130">
-        <v>1.75</v>
+        <v>2.4</v>
       </c>
       <c r="L130">
         <v>3.5</v>
       </c>
       <c r="M130">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N130">
-        <v>1.65</v>
+        <v>2.4</v>
       </c>
       <c r="O130">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="P130">
-        <v>5.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q130">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="R130">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="S130">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="T130">
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="U130">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="V130">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="W130">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X130">
         <v>-1</v>
       </c>
       <c r="Y130">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z130">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA130">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB130">
-        <v>1</v>
+        <v>1.025</v>
       </c>
       <c r="AC130">
         <v>-1</v>
@@ -12106,7 +12106,7 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>5424406</v>
+        <v>5424405</v>
       </c>
       <c r="C131" t="s">
         <v>28</v>
@@ -12121,70 +12121,70 @@
         <v>31</v>
       </c>
       <c r="G131" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="H131">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I131">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J131" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K131">
-        <v>2.4</v>
+        <v>1.75</v>
       </c>
       <c r="L131">
         <v>3.5</v>
       </c>
       <c r="M131">
-        <v>2.75</v>
+        <v>5</v>
       </c>
       <c r="N131">
-        <v>2.4</v>
+        <v>1.65</v>
       </c>
       <c r="O131">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="P131">
-        <v>2.75</v>
+        <v>5.25</v>
       </c>
       <c r="Q131">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="R131">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="S131">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="T131">
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
       <c r="U131">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="V131">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="W131">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="X131">
         <v>-1</v>
       </c>
       <c r="Y131">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z131">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA131">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB131">
-        <v>1.025</v>
+        <v>1</v>
       </c>
       <c r="AC131">
         <v>-1</v>
@@ -12818,7 +12818,7 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>6389819</v>
+        <v>6390066</v>
       </c>
       <c r="C139" t="s">
         <v>28</v>
@@ -12830,73 +12830,73 @@
         <v>45039.5625</v>
       </c>
       <c r="F139" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G139" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="H139">
         <v>2</v>
       </c>
       <c r="I139">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J139" t="s">
         <v>49</v>
       </c>
       <c r="K139">
-        <v>5.25</v>
+        <v>3</v>
       </c>
       <c r="L139">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="M139">
-        <v>1.533</v>
+        <v>2.15</v>
       </c>
       <c r="N139">
-        <v>6.5</v>
+        <v>2.8</v>
       </c>
       <c r="O139">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="P139">
-        <v>1.4</v>
+        <v>2.25</v>
       </c>
       <c r="Q139">
+        <v>0.25</v>
+      </c>
+      <c r="R139">
+        <v>1.825</v>
+      </c>
+      <c r="S139">
+        <v>2.025</v>
+      </c>
+      <c r="T139">
+        <v>3</v>
+      </c>
+      <c r="U139">
+        <v>1.8</v>
+      </c>
+      <c r="V139">
+        <v>2.05</v>
+      </c>
+      <c r="W139">
+        <v>-1</v>
+      </c>
+      <c r="X139">
+        <v>-1</v>
+      </c>
+      <c r="Y139">
         <v>1.25</v>
       </c>
-      <c r="R139">
-        <v>1.9</v>
-      </c>
-      <c r="S139">
-        <v>1.95</v>
-      </c>
-      <c r="T139">
-        <v>3.25</v>
-      </c>
-      <c r="U139">
-        <v>2</v>
-      </c>
-      <c r="V139">
-        <v>1.85</v>
-      </c>
-      <c r="W139">
-        <v>-1</v>
-      </c>
-      <c r="X139">
-        <v>-1</v>
-      </c>
-      <c r="Y139">
-        <v>0.3999999999999999</v>
-      </c>
       <c r="Z139">
         <v>-1</v>
       </c>
       <c r="AA139">
-        <v>0.95</v>
+        <v>1.025</v>
       </c>
       <c r="AB139">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AC139">
         <v>-1</v>
@@ -12907,7 +12907,7 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>6389865</v>
+        <v>6390043</v>
       </c>
       <c r="C140" t="s">
         <v>28</v>
@@ -12919,49 +12919,49 @@
         <v>45039.5625</v>
       </c>
       <c r="F140" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G140" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H140">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I140">
         <v>2</v>
       </c>
       <c r="J140" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K140">
+        <v>1.222</v>
+      </c>
+      <c r="L140">
+        <v>5.75</v>
+      </c>
+      <c r="M140">
+        <v>11</v>
+      </c>
+      <c r="N140">
+        <v>1.142</v>
+      </c>
+      <c r="O140">
+        <v>7.5</v>
+      </c>
+      <c r="P140">
+        <v>15</v>
+      </c>
+      <c r="Q140">
+        <v>-2.25</v>
+      </c>
+      <c r="R140">
+        <v>1.975</v>
+      </c>
+      <c r="S140">
+        <v>1.875</v>
+      </c>
+      <c r="T140">
         <v>3.5</v>
-      </c>
-      <c r="L140">
-        <v>3.6</v>
-      </c>
-      <c r="M140">
-        <v>1.95</v>
-      </c>
-      <c r="N140">
-        <v>2.8</v>
-      </c>
-      <c r="O140">
-        <v>3.5</v>
-      </c>
-      <c r="P140">
-        <v>2.3</v>
-      </c>
-      <c r="Q140">
-        <v>0.25</v>
-      </c>
-      <c r="R140">
-        <v>1.8</v>
-      </c>
-      <c r="S140">
-        <v>2.05</v>
-      </c>
-      <c r="T140">
-        <v>3</v>
       </c>
       <c r="U140">
         <v>1.95</v>
@@ -12973,22 +12973,22 @@
         <v>-1</v>
       </c>
       <c r="X140">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y140">
-        <v>-1</v>
+        <v>14</v>
       </c>
       <c r="Z140">
-        <v>0.4</v>
+        <v>-1</v>
       </c>
       <c r="AA140">
-        <v>-0.5</v>
+        <v>0.875</v>
       </c>
       <c r="AB140">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC140">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="141" spans="1:29">
@@ -13085,7 +13085,7 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>6390043</v>
+        <v>6390693</v>
       </c>
       <c r="C142" t="s">
         <v>28</v>
@@ -13097,76 +13097,76 @@
         <v>45039.5625</v>
       </c>
       <c r="F142" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G142" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H142">
+        <v>3</v>
+      </c>
+      <c r="I142">
+        <v>2</v>
+      </c>
+      <c r="J142" t="s">
+        <v>50</v>
+      </c>
+      <c r="K142">
+        <v>2.5</v>
+      </c>
+      <c r="L142">
+        <v>3.6</v>
+      </c>
+      <c r="M142">
+        <v>2.45</v>
+      </c>
+      <c r="N142">
+        <v>2.4</v>
+      </c>
+      <c r="O142">
+        <v>3.8</v>
+      </c>
+      <c r="P142">
+        <v>2.45</v>
+      </c>
+      <c r="Q142">
+        <v>0</v>
+      </c>
+      <c r="R142">
+        <v>1.9</v>
+      </c>
+      <c r="S142">
+        <v>1.95</v>
+      </c>
+      <c r="T142">
+        <v>3.25</v>
+      </c>
+      <c r="U142">
+        <v>2</v>
+      </c>
+      <c r="V142">
+        <v>1.85</v>
+      </c>
+      <c r="W142">
+        <v>1.4</v>
+      </c>
+      <c r="X142">
+        <v>-1</v>
+      </c>
+      <c r="Y142">
+        <v>-1</v>
+      </c>
+      <c r="Z142">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="AA142">
+        <v>-1</v>
+      </c>
+      <c r="AB142">
         <v>1</v>
       </c>
-      <c r="I142">
-        <v>2</v>
-      </c>
-      <c r="J142" t="s">
-        <v>49</v>
-      </c>
-      <c r="K142">
-        <v>1.222</v>
-      </c>
-      <c r="L142">
-        <v>5.75</v>
-      </c>
-      <c r="M142">
-        <v>11</v>
-      </c>
-      <c r="N142">
-        <v>1.142</v>
-      </c>
-      <c r="O142">
-        <v>7.5</v>
-      </c>
-      <c r="P142">
-        <v>15</v>
-      </c>
-      <c r="Q142">
-        <v>-2.25</v>
-      </c>
-      <c r="R142">
-        <v>1.975</v>
-      </c>
-      <c r="S142">
-        <v>1.875</v>
-      </c>
-      <c r="T142">
-        <v>3.5</v>
-      </c>
-      <c r="U142">
-        <v>1.95</v>
-      </c>
-      <c r="V142">
-        <v>1.9</v>
-      </c>
-      <c r="W142">
-        <v>-1</v>
-      </c>
-      <c r="X142">
-        <v>-1</v>
-      </c>
-      <c r="Y142">
-        <v>14</v>
-      </c>
-      <c r="Z142">
-        <v>-1</v>
-      </c>
-      <c r="AA142">
-        <v>0.875</v>
-      </c>
-      <c r="AB142">
-        <v>-1</v>
-      </c>
       <c r="AC142">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="143" spans="1:29">
@@ -13174,7 +13174,7 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>6390066</v>
+        <v>6390442</v>
       </c>
       <c r="C143" t="s">
         <v>28</v>
@@ -13186,73 +13186,73 @@
         <v>45039.5625</v>
       </c>
       <c r="F143" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G143" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H143">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I143">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J143" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K143">
-        <v>3</v>
+        <v>1.333</v>
       </c>
       <c r="L143">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="M143">
-        <v>2.15</v>
+        <v>8</v>
       </c>
       <c r="N143">
-        <v>2.8</v>
+        <v>1.3</v>
       </c>
       <c r="O143">
-        <v>3.6</v>
+        <v>5.25</v>
       </c>
       <c r="P143">
-        <v>2.25</v>
+        <v>8.5</v>
       </c>
       <c r="Q143">
-        <v>0.25</v>
+        <v>-1.75</v>
       </c>
       <c r="R143">
+        <v>1.975</v>
+      </c>
+      <c r="S143">
+        <v>1.875</v>
+      </c>
+      <c r="T143">
+        <v>3.75</v>
+      </c>
+      <c r="U143">
+        <v>2.025</v>
+      </c>
+      <c r="V143">
         <v>1.825</v>
       </c>
-      <c r="S143">
-        <v>2.025</v>
-      </c>
-      <c r="T143">
-        <v>3</v>
-      </c>
-      <c r="U143">
-        <v>1.8</v>
-      </c>
-      <c r="V143">
-        <v>2.05</v>
-      </c>
       <c r="W143">
-        <v>-1</v>
+        <v>0.3</v>
       </c>
       <c r="X143">
         <v>-1</v>
       </c>
       <c r="Y143">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="Z143">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA143">
+        <v>-1</v>
+      </c>
+      <c r="AB143">
         <v>1.025</v>
-      </c>
-      <c r="AB143">
-        <v>0.8</v>
       </c>
       <c r="AC143">
         <v>-1</v>
@@ -13263,7 +13263,7 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>6390442</v>
+        <v>6389865</v>
       </c>
       <c r="C144" t="s">
         <v>28</v>
@@ -13275,73 +13275,73 @@
         <v>45039.5625</v>
       </c>
       <c r="F144" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G144" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H144">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I144">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J144" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K144">
-        <v>1.333</v>
+        <v>3.5</v>
       </c>
       <c r="L144">
-        <v>5</v>
+        <v>3.6</v>
       </c>
       <c r="M144">
-        <v>8</v>
+        <v>1.95</v>
       </c>
       <c r="N144">
-        <v>1.3</v>
+        <v>2.8</v>
       </c>
       <c r="O144">
-        <v>5.25</v>
+        <v>3.5</v>
       </c>
       <c r="P144">
-        <v>8.5</v>
+        <v>2.3</v>
       </c>
       <c r="Q144">
-        <v>-1.75</v>
+        <v>0.25</v>
       </c>
       <c r="R144">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="S144">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="T144">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="U144">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="V144">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="W144">
-        <v>0.3</v>
+        <v>-1</v>
       </c>
       <c r="X144">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y144">
         <v>-1</v>
       </c>
       <c r="Z144">
-        <v>0.9750000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="AA144">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB144">
-        <v>1.025</v>
+        <v>0.95</v>
       </c>
       <c r="AC144">
         <v>-1</v>
@@ -13352,7 +13352,7 @@
         <v>143</v>
       </c>
       <c r="B145">
-        <v>6390693</v>
+        <v>6389819</v>
       </c>
       <c r="C145" t="s">
         <v>28</v>
@@ -13364,40 +13364,40 @@
         <v>45039.5625</v>
       </c>
       <c r="F145" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G145" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="H145">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I145">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J145" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K145">
-        <v>2.5</v>
+        <v>5.25</v>
       </c>
       <c r="L145">
-        <v>3.6</v>
+        <v>4.2</v>
       </c>
       <c r="M145">
-        <v>2.45</v>
+        <v>1.533</v>
       </c>
       <c r="N145">
-        <v>2.4</v>
+        <v>6.5</v>
       </c>
       <c r="O145">
-        <v>3.8</v>
+        <v>4.75</v>
       </c>
       <c r="P145">
-        <v>2.45</v>
+        <v>1.4</v>
       </c>
       <c r="Q145">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="R145">
         <v>1.9</v>
@@ -13415,19 +13415,19 @@
         <v>1.85</v>
       </c>
       <c r="W145">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X145">
         <v>-1</v>
       </c>
       <c r="Y145">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="Z145">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA145">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB145">
         <v>1</v>
@@ -13542,7 +13542,7 @@
         <v>45045.55208333334</v>
       </c>
       <c r="F147" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G147" t="s">
         <v>29</v>
@@ -13990,7 +13990,7 @@
         <v>38</v>
       </c>
       <c r="G152" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H152">
         <v>3</v>
@@ -14165,7 +14165,7 @@
         <v>45059.55208333334</v>
       </c>
       <c r="F154" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G154" t="s">
         <v>42</v>
@@ -14613,7 +14613,7 @@
         <v>42</v>
       </c>
       <c r="G159" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H159">
         <v>2</v>
@@ -14969,7 +14969,7 @@
         <v>29</v>
       </c>
       <c r="G163" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H163">
         <v>0</v>
@@ -15233,7 +15233,7 @@
         <v>45080.64583333334</v>
       </c>
       <c r="F166" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G166" t="s">
         <v>38</v>
@@ -15948,7 +15948,7 @@
         <v>33</v>
       </c>
       <c r="G174" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H174">
         <v>1</v>
@@ -16479,7 +16479,7 @@
         <v>45143.55208333334</v>
       </c>
       <c r="F180" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G180" t="s">
         <v>44</v>
@@ -17357,7 +17357,7 @@
         <v>188</v>
       </c>
       <c r="B190">
-        <v>6810007</v>
+        <v>7030334</v>
       </c>
       <c r="C190" t="s">
         <v>28</v>
@@ -17369,55 +17369,55 @@
         <v>45151.45833333334</v>
       </c>
       <c r="F190" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G190" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H190">
         <v>0</v>
       </c>
       <c r="I190">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J190" t="s">
         <v>49</v>
       </c>
       <c r="K190">
-        <v>4.75</v>
+        <v>2.75</v>
       </c>
       <c r="L190">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="M190">
-        <v>1.571</v>
+        <v>2.25</v>
       </c>
       <c r="N190">
-        <v>7</v>
+        <v>2.4</v>
       </c>
       <c r="O190">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="P190">
-        <v>1.333</v>
+        <v>2.55</v>
       </c>
       <c r="Q190">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="R190">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="S190">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="T190">
         <v>3</v>
       </c>
       <c r="U190">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V190">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W190">
         <v>-1</v>
@@ -17426,19 +17426,19 @@
         <v>-1</v>
       </c>
       <c r="Y190">
-        <v>0.333</v>
+        <v>1.55</v>
       </c>
       <c r="Z190">
         <v>-1</v>
       </c>
       <c r="AA190">
-        <v>0.9750000000000001</v>
+        <v>1</v>
       </c>
       <c r="AB190">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC190">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="191" spans="1:29">
@@ -17446,7 +17446,7 @@
         <v>189</v>
       </c>
       <c r="B191">
-        <v>7030334</v>
+        <v>6810007</v>
       </c>
       <c r="C191" t="s">
         <v>28</v>
@@ -17458,55 +17458,55 @@
         <v>45151.45833333334</v>
       </c>
       <c r="F191" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G191" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H191">
         <v>0</v>
       </c>
       <c r="I191">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J191" t="s">
         <v>49</v>
       </c>
       <c r="K191">
-        <v>2.75</v>
+        <v>4.75</v>
       </c>
       <c r="L191">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="M191">
-        <v>2.25</v>
+        <v>1.571</v>
       </c>
       <c r="N191">
-        <v>2.4</v>
+        <v>7</v>
       </c>
       <c r="O191">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="P191">
-        <v>2.55</v>
+        <v>1.333</v>
       </c>
       <c r="Q191">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="R191">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="S191">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="T191">
         <v>3</v>
       </c>
       <c r="U191">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V191">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W191">
         <v>-1</v>
@@ -17515,19 +17515,19 @@
         <v>-1</v>
       </c>
       <c r="Y191">
-        <v>1.55</v>
+        <v>0.333</v>
       </c>
       <c r="Z191">
         <v>-1</v>
       </c>
       <c r="AA191">
-        <v>1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB191">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AC191">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="192" spans="1:29">
@@ -17817,7 +17817,7 @@
         <v>29</v>
       </c>
       <c r="G195" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H195">
         <v>0</v>
@@ -18707,7 +18707,7 @@
         <v>46</v>
       </c>
       <c r="G205" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H205">
         <v>0</v>
@@ -18971,7 +18971,7 @@
         <v>45171.45833333334</v>
       </c>
       <c r="F208" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G208" t="s">
         <v>38</v>
@@ -19686,7 +19686,7 @@
         <v>47</v>
       </c>
       <c r="G216" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H216">
         <v>2</v>
@@ -20751,7 +20751,7 @@
         <v>45193.45833333334</v>
       </c>
       <c r="F228" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G228" t="s">
         <v>43</v>
@@ -21288,7 +21288,7 @@
         <v>45</v>
       </c>
       <c r="G234" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H234">
         <v>2</v>
@@ -22086,7 +22086,7 @@
         <v>45206.45833333334</v>
       </c>
       <c r="F243" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G243" t="s">
         <v>37</v>
@@ -23154,7 +23154,7 @@
         <v>45221.45833333334</v>
       </c>
       <c r="F255" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G255" t="s">
         <v>42</v>
@@ -23513,7 +23513,7 @@
         <v>40</v>
       </c>
       <c r="G259" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H259">
         <v>0</v>
@@ -24489,7 +24489,7 @@
         <v>45235.39583333334</v>
       </c>
       <c r="F270" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G270" t="s">
         <v>36</v>
@@ -25204,7 +25204,7 @@
         <v>41</v>
       </c>
       <c r="G278" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H278">
         <v>0</v>
@@ -25646,7 +25646,7 @@
         <v>45255.5</v>
       </c>
       <c r="F283" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G283" t="s">
         <v>30</v>
@@ -26895,7 +26895,7 @@
         <v>43</v>
       </c>
       <c r="G297" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H297">
         <v>2</v>
@@ -27070,7 +27070,7 @@
         <v>45269.5</v>
       </c>
       <c r="F299" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G299" t="s">
         <v>33</v>
@@ -27785,7 +27785,7 @@
         <v>37</v>
       </c>
       <c r="G307" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H307">
         <v>1</v>
@@ -28405,7 +28405,7 @@
         <v>45280.60416666666</v>
       </c>
       <c r="F314" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G314" t="s">
         <v>45</v>
@@ -29194,7 +29194,7 @@
         <v>321</v>
       </c>
       <c r="B323">
-        <v>6810142</v>
+        <v>6810145</v>
       </c>
       <c r="C323" t="s">
         <v>28</v>
@@ -29206,76 +29206,76 @@
         <v>45286.5</v>
       </c>
       <c r="F323" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G323" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="H323">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I323">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J323" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K323">
-        <v>1.75</v>
+        <v>7</v>
       </c>
       <c r="L323">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M323">
-        <v>4</v>
+        <v>1.4</v>
       </c>
       <c r="N323">
+        <v>8.5</v>
+      </c>
+      <c r="O323">
+        <v>5.75</v>
+      </c>
+      <c r="P323">
+        <v>1.285</v>
+      </c>
+      <c r="Q323">
+        <v>1.5</v>
+      </c>
+      <c r="R323">
+        <v>2.025</v>
+      </c>
+      <c r="S323">
+        <v>1.825</v>
+      </c>
+      <c r="T323">
+        <v>3.25</v>
+      </c>
+      <c r="U323">
+        <v>2.05</v>
+      </c>
+      <c r="V323">
         <v>1.8</v>
       </c>
-      <c r="O323">
-        <v>3.8</v>
-      </c>
-      <c r="P323">
-        <v>3.8</v>
-      </c>
-      <c r="Q323">
-        <v>-0.5</v>
-      </c>
-      <c r="R323">
-        <v>1.825</v>
-      </c>
-      <c r="S323">
-        <v>2.025</v>
-      </c>
-      <c r="T323">
-        <v>3</v>
-      </c>
-      <c r="U323">
-        <v>1.975</v>
-      </c>
-      <c r="V323">
-        <v>1.875</v>
-      </c>
       <c r="W323">
+        <v>-1</v>
+      </c>
+      <c r="X323">
+        <v>-1</v>
+      </c>
+      <c r="Y323">
+        <v>0.2849999999999999</v>
+      </c>
+      <c r="Z323">
+        <v>-1</v>
+      </c>
+      <c r="AA323">
+        <v>0.825</v>
+      </c>
+      <c r="AB323">
+        <v>-1</v>
+      </c>
+      <c r="AC323">
         <v>0.8</v>
-      </c>
-      <c r="X323">
-        <v>-1</v>
-      </c>
-      <c r="Y323">
-        <v>-1</v>
-      </c>
-      <c r="Z323">
-        <v>0.825</v>
-      </c>
-      <c r="AA323">
-        <v>-1</v>
-      </c>
-      <c r="AB323">
-        <v>0</v>
-      </c>
-      <c r="AC323">
-        <v>-0</v>
       </c>
     </row>
     <row r="324" spans="1:29">
@@ -29283,7 +29283,7 @@
         <v>322</v>
       </c>
       <c r="B324">
-        <v>6810145</v>
+        <v>6810142</v>
       </c>
       <c r="C324" t="s">
         <v>28</v>
@@ -29295,76 +29295,76 @@
         <v>45286.5</v>
       </c>
       <c r="F324" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G324" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="H324">
+        <v>3</v>
+      </c>
+      <c r="I324">
         <v>0</v>
       </c>
-      <c r="I324">
-        <v>2</v>
-      </c>
       <c r="J324" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K324">
-        <v>7</v>
+        <v>1.75</v>
       </c>
       <c r="L324">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M324">
-        <v>1.4</v>
+        <v>4</v>
       </c>
       <c r="N324">
-        <v>8.5</v>
+        <v>1.8</v>
       </c>
       <c r="O324">
-        <v>5.75</v>
+        <v>3.8</v>
       </c>
       <c r="P324">
-        <v>1.285</v>
+        <v>3.8</v>
       </c>
       <c r="Q324">
-        <v>1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="R324">
+        <v>1.825</v>
+      </c>
+      <c r="S324">
         <v>2.025</v>
       </c>
-      <c r="S324">
-        <v>1.825</v>
-      </c>
       <c r="T324">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U324">
-        <v>2.05</v>
+        <v>1.975</v>
       </c>
       <c r="V324">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="W324">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="X324">
         <v>-1</v>
       </c>
       <c r="Y324">
-        <v>0.2849999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z324">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AA324">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB324">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC324">
-        <v>0.8</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="325" spans="1:29">
@@ -29654,7 +29654,7 @@
         <v>36</v>
       </c>
       <c r="G328" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H328">
         <v>2</v>
@@ -29921,7 +29921,7 @@
         <v>34</v>
       </c>
       <c r="G331" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H331">
         <v>1</v>
@@ -30452,7 +30452,7 @@
         <v>45317.69791666666</v>
       </c>
       <c r="F337" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G337" t="s">
         <v>29</v>
@@ -31256,7 +31256,7 @@
         <v>38</v>
       </c>
       <c r="G346" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H346">
         <v>4</v>
@@ -31508,7 +31508,7 @@
         <v>347</v>
       </c>
       <c r="B349">
-        <v>6810162</v>
+        <v>6810164</v>
       </c>
       <c r="C349" t="s">
         <v>28</v>
@@ -31520,76 +31520,76 @@
         <v>45322.70833333334</v>
       </c>
       <c r="F349" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="G349" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="H349">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I349">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J349" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K349">
-        <v>4</v>
+        <v>1.2</v>
       </c>
       <c r="L349">
-        <v>3.6</v>
+        <v>7</v>
       </c>
       <c r="M349">
-        <v>1.85</v>
+        <v>12</v>
       </c>
       <c r="N349">
-        <v>3.1</v>
+        <v>1.142</v>
       </c>
       <c r="O349">
-        <v>3.2</v>
+        <v>8.5</v>
       </c>
       <c r="P349">
-        <v>2.3</v>
+        <v>15</v>
       </c>
       <c r="Q349">
-        <v>0.25</v>
+        <v>-2.25</v>
       </c>
       <c r="R349">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="S349">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="T349">
-        <v>2.25</v>
+        <v>3.5</v>
       </c>
       <c r="U349">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="V349">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="W349">
-        <v>-1</v>
+        <v>0.1419999999999999</v>
       </c>
       <c r="X349">
         <v>-1</v>
       </c>
       <c r="Y349">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="Z349">
         <v>-1</v>
       </c>
       <c r="AA349">
-        <v>1.05</v>
+        <v>0.925</v>
       </c>
       <c r="AB349">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AC349">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="350" spans="1:29">
@@ -31597,7 +31597,7 @@
         <v>348</v>
       </c>
       <c r="B350">
-        <v>6810164</v>
+        <v>6810162</v>
       </c>
       <c r="C350" t="s">
         <v>28</v>
@@ -31609,76 +31609,76 @@
         <v>45322.70833333334</v>
       </c>
       <c r="F350" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="G350" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="H350">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I350">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J350" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K350">
-        <v>1.2</v>
+        <v>4</v>
       </c>
       <c r="L350">
-        <v>7</v>
+        <v>3.6</v>
       </c>
       <c r="M350">
-        <v>12</v>
+        <v>1.85</v>
       </c>
       <c r="N350">
-        <v>1.142</v>
+        <v>3.1</v>
       </c>
       <c r="O350">
-        <v>8.5</v>
+        <v>3.2</v>
       </c>
       <c r="P350">
-        <v>15</v>
+        <v>2.3</v>
       </c>
       <c r="Q350">
-        <v>-2.25</v>
+        <v>0.25</v>
       </c>
       <c r="R350">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="S350">
-        <v>1.925</v>
+        <v>2.05</v>
       </c>
       <c r="T350">
-        <v>3.5</v>
+        <v>2.25</v>
       </c>
       <c r="U350">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="V350">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="W350">
-        <v>0.1419999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X350">
         <v>-1</v>
       </c>
       <c r="Y350">
-        <v>-1</v>
+        <v>1.3</v>
       </c>
       <c r="Z350">
         <v>-1</v>
       </c>
       <c r="AA350">
-        <v>0.925</v>
+        <v>1.05</v>
       </c>
       <c r="AB350">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AC350">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="351" spans="1:29">
@@ -31891,31 +31891,31 @@
         <v>2.2</v>
       </c>
       <c r="N353">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="O353">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="P353">
-        <v>2.25</v>
+        <v>2.3</v>
       </c>
       <c r="Q353">
         <v>0.25</v>
       </c>
       <c r="R353">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="S353">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="T353">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="U353">
+        <v>1.8</v>
+      </c>
+      <c r="V353">
         <v>2.05</v>
-      </c>
-      <c r="V353">
-        <v>1.8</v>
       </c>
       <c r="W353">
         <v>0</v>
@@ -31986,10 +31986,10 @@
         <v>2.5</v>
       </c>
       <c r="U354">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="V354">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="W354">
         <v>0</v>
@@ -32051,10 +32051,10 @@
         <v>-0.5</v>
       </c>
       <c r="R355">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="S355">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="T355">
         <v>2.75</v>
@@ -32086,7 +32086,7 @@
         <v>354</v>
       </c>
       <c r="B356">
-        <v>6810177</v>
+        <v>6810174</v>
       </c>
       <c r="C356" t="s">
         <v>28</v>
@@ -32095,49 +32095,49 @@
         <v>28</v>
       </c>
       <c r="E356" s="2">
-        <v>45325.69791666666</v>
+        <v>45325.59375</v>
       </c>
       <c r="F356" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G356" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="K356">
-        <v>2.8</v>
+        <v>1.909</v>
       </c>
       <c r="L356">
+        <v>3.75</v>
+      </c>
+      <c r="M356">
+        <v>3.5</v>
+      </c>
+      <c r="N356">
+        <v>2</v>
+      </c>
+      <c r="O356">
+        <v>3.6</v>
+      </c>
+      <c r="P356">
         <v>3.4</v>
       </c>
-      <c r="M356">
-        <v>2.375</v>
-      </c>
-      <c r="N356">
-        <v>2.8</v>
-      </c>
-      <c r="O356">
-        <v>3.4</v>
-      </c>
-      <c r="P356">
-        <v>2.375</v>
-      </c>
       <c r="Q356">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R356">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="S356">
-        <v>1.775</v>
+        <v>1.85</v>
       </c>
       <c r="T356">
         <v>2.75</v>
       </c>
       <c r="U356">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V356">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="W356">
         <v>0</v>
@@ -32160,7 +32160,7 @@
         <v>355</v>
       </c>
       <c r="B357">
-        <v>6810178</v>
+        <v>6810177</v>
       </c>
       <c r="C357" t="s">
         <v>28</v>
@@ -32169,49 +32169,49 @@
         <v>28</v>
       </c>
       <c r="E357" s="2">
-        <v>45326.39583333334</v>
+        <v>45325.69791666666</v>
       </c>
       <c r="F357" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G357" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K357">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="L357">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M357">
-        <v>1.95</v>
+        <v>2.375</v>
       </c>
       <c r="N357">
-        <v>3.6</v>
+        <v>2.8</v>
       </c>
       <c r="O357">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="P357">
-        <v>1.909</v>
+        <v>2.375</v>
       </c>
       <c r="Q357">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R357">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="S357">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="T357">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U357">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="V357">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="W357">
         <v>0</v>
@@ -32234,7 +32234,7 @@
         <v>356</v>
       </c>
       <c r="B358">
-        <v>6810172</v>
+        <v>6810178</v>
       </c>
       <c r="C358" t="s">
         <v>28</v>
@@ -32243,40 +32243,40 @@
         <v>28</v>
       </c>
       <c r="E358" s="2">
-        <v>45326.5</v>
+        <v>45326.39583333334</v>
       </c>
       <c r="F358" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G358" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K358">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="L358">
         <v>3.5</v>
       </c>
       <c r="M358">
-        <v>2.1</v>
+        <v>1.95</v>
       </c>
       <c r="N358">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="O358">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P358">
-        <v>2.25</v>
+        <v>1.909</v>
       </c>
       <c r="Q358">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R358">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="S358">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="T358">
         <v>2.5</v>
@@ -32308,7 +32308,7 @@
         <v>357</v>
       </c>
       <c r="B359">
-        <v>6810173</v>
+        <v>6810172</v>
       </c>
       <c r="C359" t="s">
         <v>28</v>
@@ -32317,40 +32317,40 @@
         <v>28</v>
       </c>
       <c r="E359" s="2">
-        <v>45326.60416666666</v>
+        <v>45326.5</v>
       </c>
       <c r="F359" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G359" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K359">
-        <v>2.375</v>
+        <v>3.2</v>
       </c>
       <c r="L359">
+        <v>3.5</v>
+      </c>
+      <c r="M359">
+        <v>2.1</v>
+      </c>
+      <c r="N359">
+        <v>3</v>
+      </c>
+      <c r="O359">
         <v>3.4</v>
       </c>
-      <c r="M359">
-        <v>2.8</v>
-      </c>
-      <c r="N359">
-        <v>2.2</v>
-      </c>
-      <c r="O359">
-        <v>3.5</v>
-      </c>
       <c r="P359">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="Q359">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R359">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="S359">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="T359">
         <v>2.5</v>
@@ -32382,7 +32382,7 @@
         <v>358</v>
       </c>
       <c r="B360">
-        <v>6810170</v>
+        <v>6810173</v>
       </c>
       <c r="C360" t="s">
         <v>28</v>
@@ -32391,49 +32391,49 @@
         <v>28</v>
       </c>
       <c r="E360" s="2">
-        <v>45326.63541666666</v>
+        <v>45326.60416666666</v>
       </c>
       <c r="F360" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G360" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K360">
-        <v>1.833</v>
+        <v>2.375</v>
       </c>
       <c r="L360">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="M360">
-        <v>3.8</v>
+        <v>2.8</v>
       </c>
       <c r="N360">
-        <v>1.8</v>
+        <v>2.2</v>
       </c>
       <c r="O360">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="P360">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q360">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R360">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="S360">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="T360">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U360">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="V360">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="W360">
         <v>0</v>
@@ -32448,6 +32448,80 @@
         <v>0</v>
       </c>
       <c r="AA360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:27">
+      <c r="A361" s="1">
+        <v>359</v>
+      </c>
+      <c r="B361">
+        <v>6810170</v>
+      </c>
+      <c r="C361" t="s">
+        <v>28</v>
+      </c>
+      <c r="D361" t="s">
+        <v>28</v>
+      </c>
+      <c r="E361" s="2">
+        <v>45326.63541666666</v>
+      </c>
+      <c r="F361" t="s">
+        <v>31</v>
+      </c>
+      <c r="G361" t="s">
+        <v>46</v>
+      </c>
+      <c r="K361">
+        <v>1.833</v>
+      </c>
+      <c r="L361">
+        <v>3.75</v>
+      </c>
+      <c r="M361">
+        <v>3.8</v>
+      </c>
+      <c r="N361">
+        <v>1.85</v>
+      </c>
+      <c r="O361">
+        <v>3.6</v>
+      </c>
+      <c r="P361">
+        <v>3.8</v>
+      </c>
+      <c r="Q361">
+        <v>-0.5</v>
+      </c>
+      <c r="R361">
+        <v>1.875</v>
+      </c>
+      <c r="S361">
+        <v>1.975</v>
+      </c>
+      <c r="T361">
+        <v>2.75</v>
+      </c>
+      <c r="U361">
+        <v>1.975</v>
+      </c>
+      <c r="V361">
+        <v>1.875</v>
+      </c>
+      <c r="W361">
+        <v>0</v>
+      </c>
+      <c r="X361">
+        <v>0</v>
+      </c>
+      <c r="Y361">
+        <v>0</v>
+      </c>
+      <c r="Z361">
+        <v>0</v>
+      </c>
+      <c r="AA361">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-02-11 às 04:25
</commit_message>
<xml_diff>
--- a/Belgium First Division A/Belgium First Division A.xlsx
+++ b/Belgium First Division A/Belgium First Division A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -528,7 +528,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC368"/>
+  <dimension ref="A1:AC365"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1604,7 +1604,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>6114951</v>
+        <v>5208566</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
@@ -1616,76 +1616,76 @@
         <v>44940.59375</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K13">
+        <v>1.75</v>
+      </c>
+      <c r="L13">
+        <v>3.8</v>
+      </c>
+      <c r="M13">
+        <v>4.2</v>
+      </c>
+      <c r="N13">
+        <v>1.666</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>4.5</v>
+      </c>
+      <c r="Q13">
+        <v>-0.75</v>
+      </c>
+      <c r="R13">
+        <v>1.875</v>
+      </c>
+      <c r="S13">
+        <v>1.975</v>
+      </c>
+      <c r="T13">
         <v>2.75</v>
       </c>
-      <c r="L13">
-        <v>3.4</v>
-      </c>
-      <c r="M13">
-        <v>2.45</v>
-      </c>
-      <c r="N13">
-        <v>2.8</v>
-      </c>
-      <c r="O13">
-        <v>3.3</v>
-      </c>
-      <c r="P13">
-        <v>2.45</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>2.05</v>
-      </c>
-      <c r="S13">
-        <v>1.8</v>
-      </c>
-      <c r="T13">
-        <v>2.5</v>
-      </c>
       <c r="U13">
+        <v>1.825</v>
+      </c>
+      <c r="V13">
         <v>2.025</v>
       </c>
-      <c r="V13">
-        <v>1.825</v>
-      </c>
       <c r="W13">
-        <v>-1</v>
+        <v>0.6659999999999999</v>
       </c>
       <c r="X13">
         <v>-1</v>
       </c>
       <c r="Y13">
-        <v>1.45</v>
+        <v>-1</v>
       </c>
       <c r="Z13">
-        <v>-1</v>
+        <v>0.4375</v>
       </c>
       <c r="AA13">
-        <v>0.8</v>
+        <v>-0.5</v>
       </c>
       <c r="AB13">
-        <v>-1</v>
+        <v>0.4125</v>
       </c>
       <c r="AC13">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="14" spans="1:29">
@@ -1693,7 +1693,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>5208566</v>
+        <v>6114951</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
@@ -1705,76 +1705,76 @@
         <v>44940.59375</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="H14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K14">
-        <v>1.75</v>
+        <v>2.75</v>
       </c>
       <c r="L14">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="M14">
-        <v>4.2</v>
+        <v>2.45</v>
       </c>
       <c r="N14">
-        <v>1.666</v>
+        <v>2.8</v>
       </c>
       <c r="O14">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="P14">
-        <v>4.5</v>
+        <v>2.45</v>
       </c>
       <c r="Q14">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="R14">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="S14">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="T14">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U14">
+        <v>2.025</v>
+      </c>
+      <c r="V14">
         <v>1.825</v>
       </c>
-      <c r="V14">
-        <v>2.025</v>
-      </c>
       <c r="W14">
-        <v>0.6659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X14">
         <v>-1</v>
       </c>
       <c r="Y14">
-        <v>-1</v>
+        <v>1.45</v>
       </c>
       <c r="Z14">
-        <v>0.4375</v>
+        <v>-1</v>
       </c>
       <c r="AA14">
-        <v>-0.5</v>
+        <v>0.8</v>
       </c>
       <c r="AB14">
-        <v>0.4125</v>
+        <v>-1</v>
       </c>
       <c r="AC14">
-        <v>-0.5</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="15" spans="1:29">
@@ -2494,7 +2494,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>5208571</v>
+        <v>5208701</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
@@ -2506,76 +2506,76 @@
         <v>44944.60416666666</v>
       </c>
       <c r="F23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G23" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K23">
-        <v>4.2</v>
+        <v>3.3</v>
       </c>
       <c r="L23">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="M23">
-        <v>1.75</v>
+        <v>2.05</v>
       </c>
       <c r="N23">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="O23">
-        <v>3.8</v>
+        <v>3.3</v>
       </c>
       <c r="P23">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="Q23">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="R23">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="S23">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="T23">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U23">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="V23">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="W23">
         <v>-1</v>
       </c>
       <c r="X23">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Y23">
-        <v>0.7</v>
+        <v>-1</v>
       </c>
       <c r="Z23">
-        <v>-1</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AA23">
-        <v>0.875</v>
+        <v>-0.5</v>
       </c>
       <c r="AB23">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="AC23">
-        <v>-0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="24" spans="1:29">
@@ -2583,7 +2583,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>5208701</v>
+        <v>5208571</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
@@ -2595,76 +2595,76 @@
         <v>44944.60416666666</v>
       </c>
       <c r="F24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G24" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K24">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
       <c r="L24">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="M24">
-        <v>2.05</v>
+        <v>1.75</v>
       </c>
       <c r="N24">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="O24">
-        <v>3.3</v>
+        <v>3.8</v>
       </c>
       <c r="P24">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="Q24">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="R24">
-        <v>2.05</v>
+        <v>1.975</v>
       </c>
       <c r="S24">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="T24">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U24">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="V24">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="W24">
         <v>-1</v>
       </c>
       <c r="X24">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Y24">
-        <v>-1</v>
+        <v>0.7</v>
       </c>
       <c r="Z24">
-        <v>0.5249999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA24">
+        <v>0.875</v>
+      </c>
+      <c r="AB24">
+        <v>0.5</v>
+      </c>
+      <c r="AC24">
         <v>-0.5</v>
-      </c>
-      <c r="AB24">
-        <v>-1</v>
-      </c>
-      <c r="AC24">
-        <v>0.8</v>
       </c>
     </row>
     <row r="25" spans="1:29">
@@ -3117,7 +3117,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>5208575</v>
+        <v>5208577</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
@@ -3129,40 +3129,40 @@
         <v>44947.59375</v>
       </c>
       <c r="F30" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G30" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="H30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I30">
         <v>2</v>
       </c>
       <c r="J30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K30">
-        <v>1.95</v>
+        <v>2.625</v>
       </c>
       <c r="L30">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M30">
+        <v>2.4</v>
+      </c>
+      <c r="N30">
+        <v>3.2</v>
+      </c>
+      <c r="O30">
         <v>3.4</v>
       </c>
-      <c r="N30">
-        <v>1.75</v>
-      </c>
-      <c r="O30">
-        <v>3.6</v>
-      </c>
       <c r="P30">
-        <v>4</v>
+        <v>2.05</v>
       </c>
       <c r="Q30">
-        <v>-0.75</v>
+        <v>0.25</v>
       </c>
       <c r="R30">
         <v>2.025</v>
@@ -3171,34 +3171,34 @@
         <v>1.825</v>
       </c>
       <c r="T30">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U30">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="V30">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="W30">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="X30">
         <v>-1</v>
       </c>
       <c r="Y30">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z30">
-        <v>0.5125</v>
+        <v>-1</v>
       </c>
       <c r="AA30">
+        <v>0.825</v>
+      </c>
+      <c r="AB30">
+        <v>0.475</v>
+      </c>
+      <c r="AC30">
         <v>-0.5</v>
-      </c>
-      <c r="AB30">
-        <v>1</v>
-      </c>
-      <c r="AC30">
-        <v>-1</v>
       </c>
     </row>
     <row r="31" spans="1:29">
@@ -3206,7 +3206,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>5208577</v>
+        <v>5208575</v>
       </c>
       <c r="C31" t="s">
         <v>28</v>
@@ -3218,40 +3218,40 @@
         <v>44947.59375</v>
       </c>
       <c r="F31" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G31" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I31">
         <v>2</v>
       </c>
       <c r="J31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K31">
-        <v>2.625</v>
+        <v>1.95</v>
       </c>
       <c r="L31">
+        <v>3.5</v>
+      </c>
+      <c r="M31">
         <v>3.4</v>
       </c>
-      <c r="M31">
-        <v>2.4</v>
-      </c>
       <c r="N31">
-        <v>3.2</v>
+        <v>1.75</v>
       </c>
       <c r="O31">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="P31">
-        <v>2.05</v>
+        <v>4</v>
       </c>
       <c r="Q31">
-        <v>0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R31">
         <v>2.025</v>
@@ -3260,34 +3260,34 @@
         <v>1.825</v>
       </c>
       <c r="T31">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U31">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="V31">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="W31">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="X31">
         <v>-1</v>
       </c>
       <c r="Y31">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z31">
-        <v>-1</v>
+        <v>0.5125</v>
       </c>
       <c r="AA31">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
       <c r="AB31">
-        <v>0.475</v>
+        <v>1</v>
       </c>
       <c r="AC31">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="32" spans="1:29">
@@ -4808,7 +4808,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>6192614</v>
+        <v>6192613</v>
       </c>
       <c r="C49" t="s">
         <v>28</v>
@@ -4820,76 +4820,76 @@
         <v>44961.59375</v>
       </c>
       <c r="F49" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I49">
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K49">
-        <v>2.55</v>
+        <v>3.25</v>
       </c>
       <c r="L49">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M49">
-        <v>2.45</v>
+        <v>2.05</v>
       </c>
       <c r="N49">
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="O49">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="P49">
-        <v>1.909</v>
+        <v>1.75</v>
       </c>
       <c r="Q49">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="R49">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="S49">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="T49">
         <v>2.5</v>
       </c>
       <c r="U49">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="V49">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="W49">
-        <v>-1</v>
+        <v>3.5</v>
       </c>
       <c r="X49">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y49">
         <v>-1</v>
       </c>
       <c r="Z49">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AA49">
+        <v>-1</v>
+      </c>
+      <c r="AB49">
         <v>0.8999999999999999</v>
       </c>
-      <c r="AA49">
-        <v>-1</v>
-      </c>
-      <c r="AB49">
-        <v>-1</v>
-      </c>
       <c r="AC49">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="50" spans="1:29">
@@ -4897,7 +4897,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>6192613</v>
+        <v>6192614</v>
       </c>
       <c r="C50" t="s">
         <v>28</v>
@@ -4909,76 +4909,76 @@
         <v>44961.59375</v>
       </c>
       <c r="F50" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I50">
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K50">
-        <v>3.25</v>
+        <v>2.55</v>
       </c>
       <c r="L50">
+        <v>3.4</v>
+      </c>
+      <c r="M50">
+        <v>2.45</v>
+      </c>
+      <c r="N50">
+        <v>3.6</v>
+      </c>
+      <c r="O50">
         <v>3.5</v>
       </c>
-      <c r="M50">
-        <v>2.05</v>
-      </c>
-      <c r="N50">
-        <v>4.5</v>
-      </c>
-      <c r="O50">
-        <v>3.75</v>
-      </c>
       <c r="P50">
-        <v>1.75</v>
+        <v>1.909</v>
       </c>
       <c r="Q50">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="R50">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="S50">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="T50">
         <v>2.5</v>
       </c>
       <c r="U50">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="V50">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="W50">
-        <v>3.5</v>
+        <v>-1</v>
       </c>
       <c r="X50">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y50">
         <v>-1</v>
       </c>
       <c r="Z50">
-        <v>0.8500000000000001</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA50">
         <v>-1</v>
       </c>
       <c r="AB50">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC50">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:29">
@@ -5520,7 +5520,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>5208587</v>
+        <v>5208718</v>
       </c>
       <c r="C57" t="s">
         <v>28</v>
@@ -5532,76 +5532,76 @@
         <v>44967.69791666666</v>
       </c>
       <c r="F57" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G57" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I57">
         <v>1</v>
       </c>
       <c r="J57" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K57">
-        <v>2.3</v>
+        <v>2.55</v>
       </c>
       <c r="L57">
         <v>3.4</v>
       </c>
       <c r="M57">
-        <v>2.9</v>
+        <v>2.45</v>
       </c>
       <c r="N57">
+        <v>2.55</v>
+      </c>
+      <c r="O57">
+        <v>3.4</v>
+      </c>
+      <c r="P57">
         <v>2.5</v>
-      </c>
-      <c r="O57">
-        <v>3.2</v>
-      </c>
-      <c r="P57">
-        <v>2.8</v>
       </c>
       <c r="Q57">
         <v>0</v>
       </c>
       <c r="R57">
+        <v>1.95</v>
+      </c>
+      <c r="S57">
+        <v>1.9</v>
+      </c>
+      <c r="T57">
+        <v>2.75</v>
+      </c>
+      <c r="U57">
+        <v>1.975</v>
+      </c>
+      <c r="V57">
         <v>1.875</v>
       </c>
-      <c r="S57">
-        <v>1.975</v>
-      </c>
-      <c r="T57">
-        <v>2.25</v>
-      </c>
-      <c r="U57">
-        <v>1.8</v>
-      </c>
-      <c r="V57">
-        <v>2.05</v>
-      </c>
       <c r="W57">
-        <v>-1</v>
+        <v>1.55</v>
       </c>
       <c r="X57">
-        <v>2.2</v>
+        <v>-1</v>
       </c>
       <c r="Y57">
         <v>-1</v>
       </c>
       <c r="Z57">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AA57">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="AB57">
+        <v>0.4875</v>
+      </c>
+      <c r="AC57">
         <v>-0.5</v>
-      </c>
-      <c r="AC57">
-        <v>0.5249999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:29">
@@ -5609,7 +5609,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>5208718</v>
+        <v>5208587</v>
       </c>
       <c r="C58" t="s">
         <v>28</v>
@@ -5621,76 +5621,76 @@
         <v>44967.69791666666</v>
       </c>
       <c r="F58" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G58" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I58">
         <v>1</v>
       </c>
       <c r="J58" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K58">
-        <v>2.55</v>
+        <v>2.3</v>
       </c>
       <c r="L58">
         <v>3.4</v>
       </c>
       <c r="M58">
-        <v>2.45</v>
+        <v>2.9</v>
       </c>
       <c r="N58">
-        <v>2.55</v>
+        <v>2.5</v>
       </c>
       <c r="O58">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="P58">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="Q58">
         <v>0</v>
       </c>
       <c r="R58">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="S58">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="T58">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="U58">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="V58">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="W58">
-        <v>1.55</v>
+        <v>-1</v>
       </c>
       <c r="X58">
-        <v>-1</v>
+        <v>2.2</v>
       </c>
       <c r="Y58">
         <v>-1</v>
       </c>
       <c r="Z58">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="AA58">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="AB58">
-        <v>0.4875</v>
+        <v>-0.5</v>
       </c>
       <c r="AC58">
-        <v>-0.5</v>
+        <v>0.5249999999999999</v>
       </c>
     </row>
     <row r="59" spans="1:29">
@@ -9614,7 +9614,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>5208612</v>
+        <v>5208613</v>
       </c>
       <c r="C103" t="s">
         <v>28</v>
@@ -9626,76 +9626,76 @@
         <v>45003.59375</v>
       </c>
       <c r="F103" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G103" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H103">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I103">
+        <v>2</v>
+      </c>
+      <c r="J103" t="s">
+        <v>49</v>
+      </c>
+      <c r="K103">
+        <v>3.3</v>
+      </c>
+      <c r="L103">
+        <v>3.3</v>
+      </c>
+      <c r="M103">
+        <v>2.05</v>
+      </c>
+      <c r="N103">
+        <v>2.8</v>
+      </c>
+      <c r="O103">
+        <v>3.3</v>
+      </c>
+      <c r="P103">
+        <v>2.3</v>
+      </c>
+      <c r="Q103">
+        <v>0.25</v>
+      </c>
+      <c r="R103">
+        <v>1.85</v>
+      </c>
+      <c r="S103">
+        <v>2</v>
+      </c>
+      <c r="T103">
+        <v>2.75</v>
+      </c>
+      <c r="U103">
+        <v>1.9</v>
+      </c>
+      <c r="V103">
+        <v>1.95</v>
+      </c>
+      <c r="W103">
+        <v>-1</v>
+      </c>
+      <c r="X103">
+        <v>-1</v>
+      </c>
+      <c r="Y103">
+        <v>1.3</v>
+      </c>
+      <c r="Z103">
+        <v>-1</v>
+      </c>
+      <c r="AA103">
         <v>1</v>
       </c>
-      <c r="J103" t="s">
-        <v>50</v>
-      </c>
-      <c r="K103">
-        <v>1.45</v>
-      </c>
-      <c r="L103">
-        <v>4</v>
-      </c>
-      <c r="M103">
-        <v>6</v>
-      </c>
-      <c r="N103">
-        <v>1.5</v>
-      </c>
-      <c r="O103">
-        <v>3.75</v>
-      </c>
-      <c r="P103">
-        <v>6.5</v>
-      </c>
-      <c r="Q103">
-        <v>-1</v>
-      </c>
-      <c r="R103">
-        <v>2</v>
-      </c>
-      <c r="S103">
-        <v>1.85</v>
-      </c>
-      <c r="T103">
-        <v>2.25</v>
-      </c>
-      <c r="U103">
-        <v>2.025</v>
-      </c>
-      <c r="V103">
-        <v>1.825</v>
-      </c>
-      <c r="W103">
-        <v>0.5</v>
-      </c>
-      <c r="X103">
-        <v>-1</v>
-      </c>
-      <c r="Y103">
-        <v>-1</v>
-      </c>
-      <c r="Z103">
-        <v>0</v>
-      </c>
-      <c r="AA103">
-        <v>-0</v>
-      </c>
       <c r="AB103">
-        <v>1.025</v>
+        <v>0.45</v>
       </c>
       <c r="AC103">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="104" spans="1:29">
@@ -9703,7 +9703,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>5208613</v>
+        <v>5208612</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9715,76 +9715,76 @@
         <v>45003.59375</v>
       </c>
       <c r="F104" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="G104" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H104">
+        <v>2</v>
+      </c>
+      <c r="I104">
         <v>1</v>
       </c>
-      <c r="I104">
-        <v>2</v>
-      </c>
       <c r="J104" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K104">
-        <v>3.3</v>
+        <v>1.45</v>
       </c>
       <c r="L104">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="M104">
-        <v>2.05</v>
+        <v>6</v>
       </c>
       <c r="N104">
-        <v>2.8</v>
+        <v>1.5</v>
       </c>
       <c r="O104">
-        <v>3.3</v>
+        <v>3.75</v>
       </c>
       <c r="P104">
-        <v>2.3</v>
+        <v>6.5</v>
       </c>
       <c r="Q104">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="R104">
+        <v>2</v>
+      </c>
+      <c r="S104">
         <v>1.85</v>
       </c>
-      <c r="S104">
-        <v>2</v>
-      </c>
       <c r="T104">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="U104">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="V104">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="W104">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA104">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="AB104">
-        <v>0.45</v>
+        <v>1.025</v>
       </c>
       <c r="AC104">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -12818,7 +12818,7 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>6390693</v>
+        <v>6390442</v>
       </c>
       <c r="C139" t="s">
         <v>28</v>
@@ -12830,58 +12830,58 @@
         <v>45039.5625</v>
       </c>
       <c r="F139" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G139" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H139">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I139">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J139" t="s">
         <v>50</v>
       </c>
       <c r="K139">
-        <v>2.5</v>
+        <v>1.333</v>
       </c>
       <c r="L139">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="M139">
-        <v>2.45</v>
+        <v>8</v>
       </c>
       <c r="N139">
-        <v>2.4</v>
+        <v>1.3</v>
       </c>
       <c r="O139">
-        <v>3.8</v>
+        <v>5.25</v>
       </c>
       <c r="P139">
-        <v>2.45</v>
+        <v>8.5</v>
       </c>
       <c r="Q139">
-        <v>0</v>
+        <v>-1.75</v>
       </c>
       <c r="R139">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="S139">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="T139">
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="U139">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="V139">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="W139">
-        <v>1.4</v>
+        <v>0.3</v>
       </c>
       <c r="X139">
         <v>-1</v>
@@ -12890,13 +12890,13 @@
         <v>-1</v>
       </c>
       <c r="Z139">
-        <v>0.8999999999999999</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA139">
         <v>-1</v>
       </c>
       <c r="AB139">
-        <v>1</v>
+        <v>1.025</v>
       </c>
       <c r="AC139">
         <v>-1</v>
@@ -12907,7 +12907,7 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>6390066</v>
+        <v>6385540</v>
       </c>
       <c r="C140" t="s">
         <v>28</v>
@@ -12919,10 +12919,10 @@
         <v>45039.5625</v>
       </c>
       <c r="F140" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G140" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="H140">
         <v>2</v>
@@ -12934,40 +12934,40 @@
         <v>49</v>
       </c>
       <c r="K140">
-        <v>3</v>
+        <v>1.363</v>
       </c>
       <c r="L140">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="M140">
-        <v>2.15</v>
+        <v>7</v>
       </c>
       <c r="N140">
-        <v>2.8</v>
+        <v>1.55</v>
       </c>
       <c r="O140">
-        <v>3.6</v>
+        <v>4.2</v>
       </c>
       <c r="P140">
-        <v>2.25</v>
+        <v>5</v>
       </c>
       <c r="Q140">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="R140">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="S140">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="T140">
         <v>3</v>
       </c>
       <c r="U140">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="V140">
-        <v>2.05</v>
+        <v>1.975</v>
       </c>
       <c r="W140">
         <v>-1</v>
@@ -12976,16 +12976,16 @@
         <v>-1</v>
       </c>
       <c r="Y140">
-        <v>1.25</v>
+        <v>4</v>
       </c>
       <c r="Z140">
         <v>-1</v>
       </c>
       <c r="AA140">
-        <v>1.025</v>
+        <v>0.925</v>
       </c>
       <c r="AB140">
-        <v>0.8</v>
+        <v>0.875</v>
       </c>
       <c r="AC140">
         <v>-1</v>
@@ -12996,7 +12996,7 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>6389819</v>
+        <v>6390043</v>
       </c>
       <c r="C141" t="s">
         <v>28</v>
@@ -13008,56 +13008,56 @@
         <v>45039.5625</v>
       </c>
       <c r="F141" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G141" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="H141">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I141">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J141" t="s">
         <v>49</v>
       </c>
       <c r="K141">
-        <v>5.25</v>
+        <v>1.222</v>
       </c>
       <c r="L141">
-        <v>4.2</v>
+        <v>5.75</v>
       </c>
       <c r="M141">
-        <v>1.533</v>
+        <v>11</v>
       </c>
       <c r="N141">
-        <v>6.5</v>
+        <v>1.142</v>
       </c>
       <c r="O141">
-        <v>4.75</v>
+        <v>7.5</v>
       </c>
       <c r="P141">
-        <v>1.4</v>
+        <v>15</v>
       </c>
       <c r="Q141">
-        <v>1.25</v>
+        <v>-2.25</v>
       </c>
       <c r="R141">
+        <v>1.975</v>
+      </c>
+      <c r="S141">
+        <v>1.875</v>
+      </c>
+      <c r="T141">
+        <v>3.5</v>
+      </c>
+      <c r="U141">
+        <v>1.95</v>
+      </c>
+      <c r="V141">
         <v>1.9</v>
       </c>
-      <c r="S141">
-        <v>1.95</v>
-      </c>
-      <c r="T141">
-        <v>3.25</v>
-      </c>
-      <c r="U141">
-        <v>2</v>
-      </c>
-      <c r="V141">
-        <v>1.85</v>
-      </c>
       <c r="W141">
         <v>-1</v>
       </c>
@@ -13065,19 +13065,19 @@
         <v>-1</v>
       </c>
       <c r="Y141">
-        <v>0.3999999999999999</v>
+        <v>14</v>
       </c>
       <c r="Z141">
         <v>-1</v>
       </c>
       <c r="AA141">
-        <v>0.95</v>
+        <v>0.875</v>
       </c>
       <c r="AB141">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC141">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="142" spans="1:29">
@@ -13085,7 +13085,7 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>6389865</v>
+        <v>6390066</v>
       </c>
       <c r="C142" t="s">
         <v>28</v>
@@ -13097,73 +13097,73 @@
         <v>45039.5625</v>
       </c>
       <c r="F142" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="G142" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H142">
         <v>2</v>
       </c>
       <c r="I142">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J142" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K142">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="L142">
         <v>3.6</v>
       </c>
       <c r="M142">
-        <v>1.95</v>
+        <v>2.15</v>
       </c>
       <c r="N142">
         <v>2.8</v>
       </c>
       <c r="O142">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="P142">
-        <v>2.3</v>
+        <v>2.25</v>
       </c>
       <c r="Q142">
         <v>0.25</v>
       </c>
       <c r="R142">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="S142">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="T142">
         <v>3</v>
       </c>
       <c r="U142">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="V142">
-        <v>1.9</v>
+        <v>2.05</v>
       </c>
       <c r="W142">
         <v>-1</v>
       </c>
       <c r="X142">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y142">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="Z142">
-        <v>0.4</v>
+        <v>-1</v>
       </c>
       <c r="AA142">
-        <v>-0.5</v>
+        <v>1.025</v>
       </c>
       <c r="AB142">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="AC142">
         <v>-1</v>
@@ -13174,7 +13174,7 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>6390043</v>
+        <v>6389865</v>
       </c>
       <c r="C143" t="s">
         <v>28</v>
@@ -13186,49 +13186,49 @@
         <v>45039.5625</v>
       </c>
       <c r="F143" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G143" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H143">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I143">
         <v>2</v>
       </c>
       <c r="J143" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K143">
-        <v>1.222</v>
+        <v>3.5</v>
       </c>
       <c r="L143">
-        <v>5.75</v>
+        <v>3.6</v>
       </c>
       <c r="M143">
-        <v>11</v>
+        <v>1.95</v>
       </c>
       <c r="N143">
-        <v>1.142</v>
+        <v>2.8</v>
       </c>
       <c r="O143">
-        <v>7.5</v>
+        <v>3.5</v>
       </c>
       <c r="P143">
-        <v>15</v>
+        <v>2.3</v>
       </c>
       <c r="Q143">
-        <v>-2.25</v>
+        <v>0.25</v>
       </c>
       <c r="R143">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="S143">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="T143">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="U143">
         <v>1.95</v>
@@ -13240,22 +13240,22 @@
         <v>-1</v>
       </c>
       <c r="X143">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y143">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="Z143">
-        <v>-1</v>
+        <v>0.4</v>
       </c>
       <c r="AA143">
-        <v>0.875</v>
+        <v>-0.5</v>
       </c>
       <c r="AB143">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AC143">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="144" spans="1:29">
@@ -13263,7 +13263,7 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>6385540</v>
+        <v>6390693</v>
       </c>
       <c r="C144" t="s">
         <v>28</v>
@@ -13275,73 +13275,73 @@
         <v>45039.5625</v>
       </c>
       <c r="F144" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G144" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H144">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I144">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J144" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K144">
-        <v>1.363</v>
+        <v>2.5</v>
       </c>
       <c r="L144">
-        <v>5</v>
+        <v>3.6</v>
       </c>
       <c r="M144">
-        <v>7</v>
+        <v>2.45</v>
       </c>
       <c r="N144">
-        <v>1.55</v>
+        <v>2.4</v>
       </c>
       <c r="O144">
-        <v>4.2</v>
+        <v>3.8</v>
       </c>
       <c r="P144">
-        <v>5</v>
+        <v>2.45</v>
       </c>
       <c r="Q144">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="R144">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="S144">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="T144">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U144">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="V144">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="W144">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X144">
         <v>-1</v>
       </c>
       <c r="Y144">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="Z144">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA144">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AB144">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="AC144">
         <v>-1</v>
@@ -13352,7 +13352,7 @@
         <v>143</v>
       </c>
       <c r="B145">
-        <v>6390442</v>
+        <v>6389819</v>
       </c>
       <c r="C145" t="s">
         <v>28</v>
@@ -13364,73 +13364,73 @@
         <v>45039.5625</v>
       </c>
       <c r="F145" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G145" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="H145">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I145">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J145" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K145">
-        <v>1.333</v>
+        <v>5.25</v>
       </c>
       <c r="L145">
-        <v>5</v>
+        <v>4.2</v>
       </c>
       <c r="M145">
-        <v>8</v>
+        <v>1.533</v>
       </c>
       <c r="N145">
-        <v>1.3</v>
+        <v>6.5</v>
       </c>
       <c r="O145">
-        <v>5.25</v>
+        <v>4.75</v>
       </c>
       <c r="P145">
-        <v>8.5</v>
+        <v>1.4</v>
       </c>
       <c r="Q145">
-        <v>-1.75</v>
+        <v>1.25</v>
       </c>
       <c r="R145">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="S145">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="T145">
-        <v>3.75</v>
+        <v>3.25</v>
       </c>
       <c r="U145">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="V145">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="W145">
-        <v>0.3</v>
+        <v>-1</v>
       </c>
       <c r="X145">
         <v>-1</v>
       </c>
       <c r="Y145">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="Z145">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA145">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB145">
-        <v>1.025</v>
+        <v>1</v>
       </c>
       <c r="AC145">
         <v>-1</v>
@@ -15221,7 +15221,7 @@
         <v>164</v>
       </c>
       <c r="B166">
-        <v>6576986</v>
+        <v>6576985</v>
       </c>
       <c r="C166" t="s">
         <v>28</v>
@@ -15233,58 +15233,58 @@
         <v>45080.64583333334</v>
       </c>
       <c r="F166" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="G166" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H166">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I166">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J166" t="s">
         <v>50</v>
       </c>
       <c r="K166">
-        <v>1.5</v>
+        <v>1.727</v>
       </c>
       <c r="L166">
-        <v>4.75</v>
+        <v>4.2</v>
       </c>
       <c r="M166">
-        <v>5.5</v>
+        <v>4.2</v>
       </c>
       <c r="N166">
-        <v>1.363</v>
+        <v>1.45</v>
       </c>
       <c r="O166">
+        <v>5</v>
+      </c>
+      <c r="P166">
         <v>5.75</v>
       </c>
-      <c r="P166">
-        <v>6.5</v>
-      </c>
       <c r="Q166">
-        <v>-1.5</v>
+        <v>-1.25</v>
       </c>
       <c r="R166">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="S166">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="T166">
         <v>3.5</v>
       </c>
       <c r="U166">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V166">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W166">
-        <v>0.363</v>
+        <v>0.45</v>
       </c>
       <c r="X166">
         <v>-1</v>
@@ -15293,16 +15293,16 @@
         <v>-1</v>
       </c>
       <c r="Z166">
-        <v>0.925</v>
+        <v>0.95</v>
       </c>
       <c r="AA166">
         <v>-1</v>
       </c>
       <c r="AB166">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC166">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="167" spans="1:29">
@@ -15310,7 +15310,7 @@
         <v>165</v>
       </c>
       <c r="B167">
-        <v>6576985</v>
+        <v>6576986</v>
       </c>
       <c r="C167" t="s">
         <v>28</v>
@@ -15322,58 +15322,58 @@
         <v>45080.64583333334</v>
       </c>
       <c r="F167" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G167" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H167">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I167">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J167" t="s">
         <v>50</v>
       </c>
       <c r="K167">
-        <v>1.727</v>
+        <v>1.5</v>
       </c>
       <c r="L167">
-        <v>4.2</v>
+        <v>4.75</v>
       </c>
       <c r="M167">
-        <v>4.2</v>
+        <v>5.5</v>
       </c>
       <c r="N167">
-        <v>1.45</v>
+        <v>1.363</v>
       </c>
       <c r="O167">
-        <v>5</v>
+        <v>5.75</v>
       </c>
       <c r="P167">
-        <v>5.75</v>
+        <v>6.5</v>
       </c>
       <c r="Q167">
-        <v>-1.25</v>
+        <v>-1.5</v>
       </c>
       <c r="R167">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="S167">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="T167">
         <v>3.5</v>
       </c>
       <c r="U167">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V167">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W167">
-        <v>0.45</v>
+        <v>0.363</v>
       </c>
       <c r="X167">
         <v>-1</v>
@@ -15382,16 +15382,16 @@
         <v>-1</v>
       </c>
       <c r="Z167">
-        <v>0.95</v>
+        <v>0.925</v>
       </c>
       <c r="AA167">
         <v>-1</v>
       </c>
       <c r="AB167">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AC167">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="168" spans="1:29">
@@ -17357,7 +17357,7 @@
         <v>188</v>
       </c>
       <c r="B190">
-        <v>6810007</v>
+        <v>7030334</v>
       </c>
       <c r="C190" t="s">
         <v>28</v>
@@ -17369,55 +17369,55 @@
         <v>45151.45833333334</v>
       </c>
       <c r="F190" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G190" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H190">
         <v>0</v>
       </c>
       <c r="I190">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J190" t="s">
         <v>49</v>
       </c>
       <c r="K190">
-        <v>4.75</v>
+        <v>2.75</v>
       </c>
       <c r="L190">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="M190">
-        <v>1.571</v>
+        <v>2.25</v>
       </c>
       <c r="N190">
-        <v>7</v>
+        <v>2.4</v>
       </c>
       <c r="O190">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="P190">
-        <v>1.333</v>
+        <v>2.55</v>
       </c>
       <c r="Q190">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="R190">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="S190">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="T190">
         <v>3</v>
       </c>
       <c r="U190">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V190">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W190">
         <v>-1</v>
@@ -17426,19 +17426,19 @@
         <v>-1</v>
       </c>
       <c r="Y190">
-        <v>0.333</v>
+        <v>1.55</v>
       </c>
       <c r="Z190">
         <v>-1</v>
       </c>
       <c r="AA190">
-        <v>0.9750000000000001</v>
+        <v>1</v>
       </c>
       <c r="AB190">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC190">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="191" spans="1:29">
@@ -17446,7 +17446,7 @@
         <v>189</v>
       </c>
       <c r="B191">
-        <v>7030334</v>
+        <v>6810007</v>
       </c>
       <c r="C191" t="s">
         <v>28</v>
@@ -17458,55 +17458,55 @@
         <v>45151.45833333334</v>
       </c>
       <c r="F191" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G191" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H191">
         <v>0</v>
       </c>
       <c r="I191">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J191" t="s">
         <v>49</v>
       </c>
       <c r="K191">
-        <v>2.75</v>
+        <v>4.75</v>
       </c>
       <c r="L191">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="M191">
-        <v>2.25</v>
+        <v>1.571</v>
       </c>
       <c r="N191">
-        <v>2.4</v>
+        <v>7</v>
       </c>
       <c r="O191">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="P191">
-        <v>2.55</v>
+        <v>1.333</v>
       </c>
       <c r="Q191">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="R191">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="S191">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="T191">
         <v>3</v>
       </c>
       <c r="U191">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V191">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W191">
         <v>-1</v>
@@ -17515,19 +17515,19 @@
         <v>-1</v>
       </c>
       <c r="Y191">
-        <v>1.55</v>
+        <v>0.333</v>
       </c>
       <c r="Z191">
         <v>-1</v>
       </c>
       <c r="AA191">
-        <v>1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB191">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AC191">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="192" spans="1:29">
@@ -18069,7 +18069,7 @@
         <v>196</v>
       </c>
       <c r="B198">
-        <v>6810012</v>
+        <v>6810015</v>
       </c>
       <c r="C198" t="s">
         <v>28</v>
@@ -18081,61 +18081,61 @@
         <v>45158.45833333334</v>
       </c>
       <c r="F198" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="G198" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H198">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I198">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J198" t="s">
         <v>48</v>
       </c>
       <c r="K198">
+        <v>1.45</v>
+      </c>
+      <c r="L198">
+        <v>4.5</v>
+      </c>
+      <c r="M198">
+        <v>7</v>
+      </c>
+      <c r="N198">
         <v>1.533</v>
       </c>
-      <c r="L198">
+      <c r="O198">
         <v>4.2</v>
       </c>
-      <c r="M198">
-        <v>5.5</v>
-      </c>
-      <c r="N198">
-        <v>1.6</v>
-      </c>
-      <c r="O198">
-        <v>4</v>
-      </c>
       <c r="P198">
-        <v>5.25</v>
+        <v>6</v>
       </c>
       <c r="Q198">
         <v>-1</v>
       </c>
       <c r="R198">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="S198">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="T198">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="U198">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="V198">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="W198">
         <v>-1</v>
       </c>
       <c r="X198">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="Y198">
         <v>-1</v>
@@ -18144,13 +18144,13 @@
         <v>-1</v>
       </c>
       <c r="AA198">
-        <v>0.875</v>
+        <v>0.95</v>
       </c>
       <c r="AB198">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AC198">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="199" spans="1:29">
@@ -18158,7 +18158,7 @@
         <v>197</v>
       </c>
       <c r="B199">
-        <v>6810015</v>
+        <v>6810012</v>
       </c>
       <c r="C199" t="s">
         <v>28</v>
@@ -18170,61 +18170,61 @@
         <v>45158.45833333334</v>
       </c>
       <c r="F199" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="G199" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H199">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I199">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J199" t="s">
         <v>48</v>
       </c>
       <c r="K199">
-        <v>1.45</v>
+        <v>1.533</v>
       </c>
       <c r="L199">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="M199">
-        <v>7</v>
+        <v>5.5</v>
       </c>
       <c r="N199">
-        <v>1.533</v>
+        <v>1.6</v>
       </c>
       <c r="O199">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="P199">
-        <v>6</v>
+        <v>5.25</v>
       </c>
       <c r="Q199">
         <v>-1</v>
       </c>
       <c r="R199">
+        <v>1.975</v>
+      </c>
+      <c r="S199">
+        <v>1.875</v>
+      </c>
+      <c r="T199">
+        <v>3</v>
+      </c>
+      <c r="U199">
         <v>1.9</v>
       </c>
-      <c r="S199">
+      <c r="V199">
         <v>1.95</v>
       </c>
-      <c r="T199">
-        <v>2.5</v>
-      </c>
-      <c r="U199">
-        <v>1.8</v>
-      </c>
-      <c r="V199">
-        <v>2.05</v>
-      </c>
       <c r="W199">
         <v>-1</v>
       </c>
       <c r="X199">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Y199">
         <v>-1</v>
@@ -18233,13 +18233,13 @@
         <v>-1</v>
       </c>
       <c r="AA199">
+        <v>0.875</v>
+      </c>
+      <c r="AB199">
+        <v>-1</v>
+      </c>
+      <c r="AC199">
         <v>0.95</v>
-      </c>
-      <c r="AB199">
-        <v>0.8</v>
-      </c>
-      <c r="AC199">
-        <v>-1</v>
       </c>
     </row>
     <row r="200" spans="1:29">
@@ -30618,7 +30618,7 @@
         <v>337</v>
       </c>
       <c r="B339">
-        <v>6810159</v>
+        <v>6810158</v>
       </c>
       <c r="C339" t="s">
         <v>28</v>
@@ -30630,73 +30630,73 @@
         <v>45318.69791666666</v>
       </c>
       <c r="F339" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G339" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H339">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I339">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J339" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K339">
-        <v>5.5</v>
+        <v>1.363</v>
       </c>
       <c r="L339">
-        <v>4.2</v>
+        <v>5</v>
       </c>
       <c r="M339">
-        <v>1.5</v>
+        <v>6.5</v>
       </c>
       <c r="N339">
-        <v>6</v>
+        <v>1.444</v>
       </c>
       <c r="O339">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="P339">
-        <v>1.45</v>
+        <v>5.75</v>
       </c>
       <c r="Q339">
-        <v>1.25</v>
+        <v>-1.25</v>
       </c>
       <c r="R339">
+        <v>2</v>
+      </c>
+      <c r="S339">
+        <v>1.85</v>
+      </c>
+      <c r="T339">
+        <v>3</v>
+      </c>
+      <c r="U339">
+        <v>2.025</v>
+      </c>
+      <c r="V339">
         <v>1.825</v>
       </c>
-      <c r="S339">
-        <v>2.025</v>
-      </c>
-      <c r="T339">
-        <v>2.75</v>
-      </c>
-      <c r="U339">
-        <v>1.95</v>
-      </c>
-      <c r="V339">
-        <v>1.9</v>
-      </c>
       <c r="W339">
         <v>-1</v>
       </c>
       <c r="X339">
-        <v>-1</v>
+        <v>3.5</v>
       </c>
       <c r="Y339">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
       <c r="Z339">
         <v>-1</v>
       </c>
       <c r="AA339">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AB339">
         <v>1.025</v>
-      </c>
-      <c r="AB339">
-        <v>0.95</v>
       </c>
       <c r="AC339">
         <v>-1</v>
@@ -30707,7 +30707,7 @@
         <v>338</v>
       </c>
       <c r="B340">
-        <v>6810158</v>
+        <v>6810159</v>
       </c>
       <c r="C340" t="s">
         <v>28</v>
@@ -30719,73 +30719,73 @@
         <v>45318.69791666666</v>
       </c>
       <c r="F340" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G340" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H340">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I340">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J340" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K340">
-        <v>1.363</v>
+        <v>5.5</v>
       </c>
       <c r="L340">
-        <v>5</v>
+        <v>4.2</v>
       </c>
       <c r="M340">
-        <v>6.5</v>
+        <v>1.5</v>
       </c>
       <c r="N340">
-        <v>1.444</v>
+        <v>6</v>
       </c>
       <c r="O340">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="P340">
-        <v>5.75</v>
+        <v>1.45</v>
       </c>
       <c r="Q340">
-        <v>-1.25</v>
+        <v>1.25</v>
       </c>
       <c r="R340">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="S340">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="T340">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U340">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="V340">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="W340">
         <v>-1</v>
       </c>
       <c r="X340">
-        <v>3.5</v>
+        <v>-1</v>
       </c>
       <c r="Y340">
-        <v>-1</v>
+        <v>0.45</v>
       </c>
       <c r="Z340">
         <v>-1</v>
       </c>
       <c r="AA340">
-        <v>0.8500000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="AB340">
-        <v>1.025</v>
+        <v>0.95</v>
       </c>
       <c r="AC340">
         <v>-1</v>
@@ -31152,7 +31152,7 @@
         <v>343</v>
       </c>
       <c r="B345">
-        <v>6810167</v>
+        <v>6810169</v>
       </c>
       <c r="C345" t="s">
         <v>28</v>
@@ -31164,73 +31164,73 @@
         <v>45321.6875</v>
       </c>
       <c r="F345" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G345" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="H345">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I345">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J345" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K345">
-        <v>1.125</v>
+        <v>3.4</v>
       </c>
       <c r="L345">
-        <v>8.5</v>
+        <v>3.8</v>
       </c>
       <c r="M345">
-        <v>17</v>
+        <v>1.95</v>
       </c>
       <c r="N345">
-        <v>1.125</v>
+        <v>3.3</v>
       </c>
       <c r="O345">
-        <v>8.5</v>
+        <v>3.6</v>
       </c>
       <c r="P345">
-        <v>17</v>
+        <v>2.05</v>
       </c>
       <c r="Q345">
-        <v>-2.25</v>
+        <v>0.25</v>
       </c>
       <c r="R345">
+        <v>2</v>
+      </c>
+      <c r="S345">
         <v>1.85</v>
       </c>
-      <c r="S345">
-        <v>2</v>
-      </c>
       <c r="T345">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U345">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V345">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W345">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="X345">
-        <v>7.5</v>
+        <v>-1</v>
       </c>
       <c r="Y345">
         <v>-1</v>
       </c>
       <c r="Z345">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AA345">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB345">
-        <v>0.8999999999999999</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC345">
         <v>-1</v>
@@ -31241,7 +31241,7 @@
         <v>344</v>
       </c>
       <c r="B346">
-        <v>6810169</v>
+        <v>6810167</v>
       </c>
       <c r="C346" t="s">
         <v>28</v>
@@ -31253,73 +31253,73 @@
         <v>45321.6875</v>
       </c>
       <c r="F346" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G346" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H346">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I346">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J346" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K346">
-        <v>3.4</v>
+        <v>1.125</v>
       </c>
       <c r="L346">
-        <v>3.8</v>
+        <v>8.5</v>
       </c>
       <c r="M346">
+        <v>17</v>
+      </c>
+      <c r="N346">
+        <v>1.125</v>
+      </c>
+      <c r="O346">
+        <v>8.5</v>
+      </c>
+      <c r="P346">
+        <v>17</v>
+      </c>
+      <c r="Q346">
+        <v>-2.25</v>
+      </c>
+      <c r="R346">
+        <v>1.85</v>
+      </c>
+      <c r="S346">
+        <v>2</v>
+      </c>
+      <c r="T346">
+        <v>3.5</v>
+      </c>
+      <c r="U346">
+        <v>1.9</v>
+      </c>
+      <c r="V346">
         <v>1.95</v>
       </c>
-      <c r="N346">
-        <v>3.3</v>
-      </c>
-      <c r="O346">
-        <v>3.6</v>
-      </c>
-      <c r="P346">
-        <v>2.05</v>
-      </c>
-      <c r="Q346">
-        <v>0.25</v>
-      </c>
-      <c r="R346">
-        <v>2</v>
-      </c>
-      <c r="S346">
-        <v>1.85</v>
-      </c>
-      <c r="T346">
-        <v>2.75</v>
-      </c>
-      <c r="U346">
-        <v>1.975</v>
-      </c>
-      <c r="V346">
-        <v>1.875</v>
-      </c>
       <c r="W346">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="X346">
-        <v>-1</v>
+        <v>7.5</v>
       </c>
       <c r="Y346">
         <v>-1</v>
       </c>
       <c r="Z346">
+        <v>-1</v>
+      </c>
+      <c r="AA346">
         <v>1</v>
       </c>
-      <c r="AA346">
-        <v>-1</v>
-      </c>
       <c r="AB346">
-        <v>0.9750000000000001</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC346">
         <v>-1</v>
@@ -31330,7 +31330,7 @@
         <v>345</v>
       </c>
       <c r="B347">
-        <v>6810168</v>
+        <v>6810165</v>
       </c>
       <c r="C347" t="s">
         <v>28</v>
@@ -31342,58 +31342,58 @@
         <v>45322.61458333334</v>
       </c>
       <c r="F347" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G347" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H347">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I347">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J347" t="s">
         <v>50</v>
       </c>
       <c r="K347">
-        <v>4.5</v>
+        <v>1.6</v>
       </c>
       <c r="L347">
+        <v>4</v>
+      </c>
+      <c r="M347">
+        <v>5</v>
+      </c>
+      <c r="N347">
+        <v>1.8</v>
+      </c>
+      <c r="O347">
+        <v>3.75</v>
+      </c>
+      <c r="P347">
         <v>4.2</v>
       </c>
-      <c r="M347">
-        <v>1.666</v>
-      </c>
-      <c r="N347">
-        <v>4.333</v>
-      </c>
-      <c r="O347">
-        <v>4</v>
-      </c>
-      <c r="P347">
-        <v>1.7</v>
-      </c>
       <c r="Q347">
-        <v>0.75</v>
+        <v>-0.75</v>
       </c>
       <c r="R347">
+        <v>2.05</v>
+      </c>
+      <c r="S347">
+        <v>1.8</v>
+      </c>
+      <c r="T347">
+        <v>2.75</v>
+      </c>
+      <c r="U347">
         <v>1.95</v>
       </c>
-      <c r="S347">
+      <c r="V347">
         <v>1.9</v>
       </c>
-      <c r="T347">
-        <v>3</v>
-      </c>
-      <c r="U347">
-        <v>1.975</v>
-      </c>
-      <c r="V347">
-        <v>1.875</v>
-      </c>
       <c r="W347">
-        <v>3.333</v>
+        <v>0.8</v>
       </c>
       <c r="X347">
         <v>-1</v>
@@ -31402,16 +31402,16 @@
         <v>-1</v>
       </c>
       <c r="Z347">
-        <v>0.95</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AA347">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB347">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC347">
-        <v>-0</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="348" spans="1:29">
@@ -31419,7 +31419,7 @@
         <v>346</v>
       </c>
       <c r="B348">
-        <v>6810165</v>
+        <v>6810168</v>
       </c>
       <c r="C348" t="s">
         <v>28</v>
@@ -31431,58 +31431,58 @@
         <v>45322.61458333334</v>
       </c>
       <c r="F348" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G348" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H348">
+        <v>2</v>
+      </c>
+      <c r="I348">
         <v>1</v>
-      </c>
-      <c r="I348">
-        <v>0</v>
       </c>
       <c r="J348" t="s">
         <v>50</v>
       </c>
       <c r="K348">
-        <v>1.6</v>
+        <v>4.5</v>
       </c>
       <c r="L348">
+        <v>4.2</v>
+      </c>
+      <c r="M348">
+        <v>1.666</v>
+      </c>
+      <c r="N348">
+        <v>4.333</v>
+      </c>
+      <c r="O348">
         <v>4</v>
       </c>
-      <c r="M348">
-        <v>5</v>
-      </c>
-      <c r="N348">
-        <v>1.8</v>
-      </c>
-      <c r="O348">
-        <v>3.75</v>
-      </c>
       <c r="P348">
-        <v>4.2</v>
+        <v>1.7</v>
       </c>
       <c r="Q348">
-        <v>-0.75</v>
+        <v>0.75</v>
       </c>
       <c r="R348">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="S348">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="T348">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U348">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="V348">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="W348">
-        <v>0.8</v>
+        <v>3.333</v>
       </c>
       <c r="X348">
         <v>-1</v>
@@ -31491,16 +31491,16 @@
         <v>-1</v>
       </c>
       <c r="Z348">
-        <v>0.5249999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="AA348">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB348">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC348">
-        <v>0.8999999999999999</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="349" spans="1:29">
@@ -31686,7 +31686,7 @@
         <v>349</v>
       </c>
       <c r="B351">
-        <v>6810163</v>
+        <v>6810166</v>
       </c>
       <c r="C351" t="s">
         <v>28</v>
@@ -31698,73 +31698,73 @@
         <v>45323.6875</v>
       </c>
       <c r="F351" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G351" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H351">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I351">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J351" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K351">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="L351">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M351">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="N351">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="O351">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P351">
-        <v>2.15</v>
+        <v>2.2</v>
       </c>
       <c r="Q351">
         <v>0.25</v>
       </c>
       <c r="R351">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="S351">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="T351">
         <v>2.5</v>
       </c>
       <c r="U351">
+        <v>1.875</v>
+      </c>
+      <c r="V351">
         <v>1.975</v>
       </c>
-      <c r="V351">
-        <v>1.875</v>
-      </c>
       <c r="W351">
-        <v>2.25</v>
+        <v>-1</v>
       </c>
       <c r="X351">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y351">
         <v>-1</v>
       </c>
       <c r="Z351">
-        <v>0.95</v>
+        <v>0.4625</v>
       </c>
       <c r="AA351">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB351">
-        <v>0.9750000000000001</v>
+        <v>0.875</v>
       </c>
       <c r="AC351">
         <v>-1</v>
@@ -31775,7 +31775,7 @@
         <v>350</v>
       </c>
       <c r="B352">
-        <v>6810166</v>
+        <v>6810163</v>
       </c>
       <c r="C352" t="s">
         <v>28</v>
@@ -31787,73 +31787,73 @@
         <v>45323.6875</v>
       </c>
       <c r="F352" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G352" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H352">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I352">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J352" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K352">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="L352">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M352">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="N352">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="O352">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="P352">
-        <v>2.2</v>
+        <v>2.15</v>
       </c>
       <c r="Q352">
         <v>0.25</v>
       </c>
       <c r="R352">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="S352">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="T352">
         <v>2.5</v>
       </c>
       <c r="U352">
+        <v>1.975</v>
+      </c>
+      <c r="V352">
         <v>1.875</v>
       </c>
-      <c r="V352">
-        <v>1.975</v>
-      </c>
       <c r="W352">
-        <v>-1</v>
+        <v>2.25</v>
       </c>
       <c r="X352">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y352">
         <v>-1</v>
       </c>
       <c r="Z352">
-        <v>0.4625</v>
+        <v>0.95</v>
       </c>
       <c r="AA352">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB352">
-        <v>0.875</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC352">
         <v>-1</v>
@@ -32593,6 +32593,15 @@
       <c r="G361" t="s">
         <v>45</v>
       </c>
+      <c r="H361">
+        <v>1</v>
+      </c>
+      <c r="I361">
+        <v>0</v>
+      </c>
+      <c r="J361" t="s">
+        <v>50</v>
+      </c>
       <c r="K361">
         <v>1.5</v>
       </c>
@@ -32603,46 +32612,52 @@
         <v>5.75</v>
       </c>
       <c r="N361">
-        <v>1.5</v>
+        <v>1.533</v>
       </c>
       <c r="O361">
         <v>4.333</v>
       </c>
       <c r="P361">
-        <v>6</v>
+        <v>5.75</v>
       </c>
       <c r="Q361">
         <v>-1</v>
       </c>
       <c r="R361">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="S361">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="T361">
         <v>2.75</v>
       </c>
       <c r="U361">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="V361">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="W361">
-        <v>0</v>
+        <v>0.5329999999999999</v>
       </c>
       <c r="X361">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y361">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z361">
         <v>0</v>
       </c>
       <c r="AA361">
-        <v>0</v>
+        <v>-0</v>
+      </c>
+      <c r="AB361">
+        <v>-1</v>
+      </c>
+      <c r="AC361">
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="362" spans="1:29">
@@ -32650,7 +32665,7 @@
         <v>360</v>
       </c>
       <c r="B362">
-        <v>6810184</v>
+        <v>6810179</v>
       </c>
       <c r="C362" t="s">
         <v>28</v>
@@ -32659,49 +32674,49 @@
         <v>28</v>
       </c>
       <c r="E362" s="2">
-        <v>45332.5</v>
+        <v>45333.39583333334</v>
       </c>
       <c r="F362" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="G362" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K362">
-        <v>1.833</v>
+        <v>5.25</v>
       </c>
       <c r="L362">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M362">
-        <v>3.75</v>
+        <v>1.55</v>
       </c>
       <c r="N362">
-        <v>1.833</v>
+        <v>5</v>
       </c>
       <c r="O362">
-        <v>3.75</v>
+        <v>4.2</v>
       </c>
       <c r="P362">
-        <v>4</v>
+        <v>1.615</v>
       </c>
       <c r="Q362">
-        <v>-0.5</v>
+        <v>0.75</v>
       </c>
       <c r="R362">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="S362">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="T362">
         <v>2.75</v>
       </c>
       <c r="U362">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="V362">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="W362">
         <v>0</v>
@@ -32724,7 +32739,7 @@
         <v>361</v>
       </c>
       <c r="B363">
-        <v>6810186</v>
+        <v>6810182</v>
       </c>
       <c r="C363" t="s">
         <v>28</v>
@@ -32733,34 +32748,34 @@
         <v>28</v>
       </c>
       <c r="E363" s="2">
-        <v>45332.59375</v>
+        <v>45333.5</v>
       </c>
       <c r="F363" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G363" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K363">
-        <v>1.285</v>
+        <v>3.8</v>
       </c>
       <c r="L363">
-        <v>5.5</v>
+        <v>3.6</v>
       </c>
       <c r="M363">
-        <v>8.5</v>
+        <v>1.85</v>
       </c>
       <c r="N363">
-        <v>1.3</v>
+        <v>3.5</v>
       </c>
       <c r="O363">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="P363">
-        <v>8.5</v>
+        <v>2</v>
       </c>
       <c r="Q363">
-        <v>-1.5</v>
+        <v>0.5</v>
       </c>
       <c r="R363">
         <v>1.825</v>
@@ -32769,13 +32784,13 @@
         <v>2.025</v>
       </c>
       <c r="T363">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U363">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="V363">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="W363">
         <v>0</v>
@@ -32798,7 +32813,7 @@
         <v>362</v>
       </c>
       <c r="B364">
-        <v>6810185</v>
+        <v>6810180</v>
       </c>
       <c r="C364" t="s">
         <v>28</v>
@@ -32807,34 +32822,34 @@
         <v>28</v>
       </c>
       <c r="E364" s="2">
-        <v>45332.69791666666</v>
+        <v>45333.60416666666</v>
       </c>
       <c r="F364" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G364" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="K364">
-        <v>1.2</v>
+        <v>3.6</v>
       </c>
       <c r="L364">
-        <v>6.5</v>
+        <v>3.4</v>
       </c>
       <c r="M364">
-        <v>9.5</v>
+        <v>2</v>
       </c>
       <c r="N364">
-        <v>1.222</v>
+        <v>3.75</v>
       </c>
       <c r="O364">
-        <v>7</v>
+        <v>3.4</v>
       </c>
       <c r="P364">
-        <v>9.5</v>
+        <v>2</v>
       </c>
       <c r="Q364">
-        <v>-1.75</v>
+        <v>0.5</v>
       </c>
       <c r="R364">
         <v>1.825</v>
@@ -32843,13 +32858,13 @@
         <v>2.025</v>
       </c>
       <c r="T364">
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
       <c r="U364">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="V364">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="W364">
         <v>0</v>
@@ -32872,7 +32887,7 @@
         <v>363</v>
       </c>
       <c r="B365">
-        <v>6810179</v>
+        <v>6810181</v>
       </c>
       <c r="C365" t="s">
         <v>28</v>
@@ -32881,49 +32896,49 @@
         <v>28</v>
       </c>
       <c r="E365" s="2">
-        <v>45333.39583333334</v>
+        <v>45333.63541666666</v>
       </c>
       <c r="F365" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G365" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K365">
-        <v>5.25</v>
+        <v>2.05</v>
       </c>
       <c r="L365">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M365">
-        <v>1.55</v>
+        <v>3.2</v>
       </c>
       <c r="N365">
-        <v>5</v>
+        <v>2.15</v>
       </c>
       <c r="O365">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P365">
-        <v>1.615</v>
+        <v>3.1</v>
       </c>
       <c r="Q365">
-        <v>1</v>
+        <v>-0.25</v>
       </c>
       <c r="R365">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="S365">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="T365">
         <v>2.75</v>
       </c>
       <c r="U365">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="V365">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="W365">
         <v>0</v>
@@ -32938,228 +32953,6 @@
         <v>0</v>
       </c>
       <c r="AA365">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="366" spans="1:29">
-      <c r="A366" s="1">
-        <v>364</v>
-      </c>
-      <c r="B366">
-        <v>6810182</v>
-      </c>
-      <c r="C366" t="s">
-        <v>28</v>
-      </c>
-      <c r="D366" t="s">
-        <v>28</v>
-      </c>
-      <c r="E366" s="2">
-        <v>45333.5</v>
-      </c>
-      <c r="F366" t="s">
-        <v>40</v>
-      </c>
-      <c r="G366" t="s">
-        <v>34</v>
-      </c>
-      <c r="K366">
-        <v>3.8</v>
-      </c>
-      <c r="L366">
-        <v>3.6</v>
-      </c>
-      <c r="M366">
-        <v>1.85</v>
-      </c>
-      <c r="N366">
-        <v>3.75</v>
-      </c>
-      <c r="O366">
-        <v>3.6</v>
-      </c>
-      <c r="P366">
-        <v>1.909</v>
-      </c>
-      <c r="Q366">
-        <v>0.5</v>
-      </c>
-      <c r="R366">
-        <v>1.9</v>
-      </c>
-      <c r="S366">
-        <v>1.95</v>
-      </c>
-      <c r="T366">
-        <v>2.75</v>
-      </c>
-      <c r="U366">
-        <v>1.95</v>
-      </c>
-      <c r="V366">
-        <v>1.9</v>
-      </c>
-      <c r="W366">
-        <v>0</v>
-      </c>
-      <c r="X366">
-        <v>0</v>
-      </c>
-      <c r="Y366">
-        <v>0</v>
-      </c>
-      <c r="Z366">
-        <v>0</v>
-      </c>
-      <c r="AA366">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="367" spans="1:29">
-      <c r="A367" s="1">
-        <v>365</v>
-      </c>
-      <c r="B367">
-        <v>6810180</v>
-      </c>
-      <c r="C367" t="s">
-        <v>28</v>
-      </c>
-      <c r="D367" t="s">
-        <v>28</v>
-      </c>
-      <c r="E367" s="2">
-        <v>45333.60416666666</v>
-      </c>
-      <c r="F367" t="s">
-        <v>44</v>
-      </c>
-      <c r="G367" t="s">
-        <v>36</v>
-      </c>
-      <c r="K367">
-        <v>3.6</v>
-      </c>
-      <c r="L367">
-        <v>3.4</v>
-      </c>
-      <c r="M367">
-        <v>2</v>
-      </c>
-      <c r="N367">
-        <v>3.75</v>
-      </c>
-      <c r="O367">
-        <v>3.4</v>
-      </c>
-      <c r="P367">
-        <v>2</v>
-      </c>
-      <c r="Q367">
-        <v>0.5</v>
-      </c>
-      <c r="R367">
-        <v>1.8</v>
-      </c>
-      <c r="S367">
-        <v>2.05</v>
-      </c>
-      <c r="T367">
-        <v>2.5</v>
-      </c>
-      <c r="U367">
-        <v>1.9</v>
-      </c>
-      <c r="V367">
-        <v>1.95</v>
-      </c>
-      <c r="W367">
-        <v>0</v>
-      </c>
-      <c r="X367">
-        <v>0</v>
-      </c>
-      <c r="Y367">
-        <v>0</v>
-      </c>
-      <c r="Z367">
-        <v>0</v>
-      </c>
-      <c r="AA367">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="368" spans="1:29">
-      <c r="A368" s="1">
-        <v>366</v>
-      </c>
-      <c r="B368">
-        <v>6810181</v>
-      </c>
-      <c r="C368" t="s">
-        <v>28</v>
-      </c>
-      <c r="D368" t="s">
-        <v>28</v>
-      </c>
-      <c r="E368" s="2">
-        <v>45333.63541666666</v>
-      </c>
-      <c r="F368" t="s">
-        <v>42</v>
-      </c>
-      <c r="G368" t="s">
-        <v>31</v>
-      </c>
-      <c r="K368">
-        <v>2.05</v>
-      </c>
-      <c r="L368">
-        <v>3.6</v>
-      </c>
-      <c r="M368">
-        <v>3.2</v>
-      </c>
-      <c r="N368">
-        <v>2.05</v>
-      </c>
-      <c r="O368">
-        <v>3.75</v>
-      </c>
-      <c r="P368">
-        <v>3.25</v>
-      </c>
-      <c r="Q368">
-        <v>-0.25</v>
-      </c>
-      <c r="R368">
-        <v>1.85</v>
-      </c>
-      <c r="S368">
-        <v>2</v>
-      </c>
-      <c r="T368">
-        <v>2.75</v>
-      </c>
-      <c r="U368">
-        <v>1.925</v>
-      </c>
-      <c r="V368">
-        <v>1.925</v>
-      </c>
-      <c r="W368">
-        <v>0</v>
-      </c>
-      <c r="X368">
-        <v>0</v>
-      </c>
-      <c r="Y368">
-        <v>0</v>
-      </c>
-      <c r="Z368">
-        <v>0</v>
-      </c>
-      <c r="AA368">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-02-15 às 19:43
</commit_message>
<xml_diff>
--- a/Belgium First Division A/Belgium First Division A.xlsx
+++ b/Belgium First Division A/Belgium First Division A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -528,7 +528,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC365"/>
+  <dimension ref="A1:AC376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2316,7 +2316,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>5208702</v>
+        <v>5208698</v>
       </c>
       <c r="C21" t="s">
         <v>28</v>
@@ -2328,76 +2328,76 @@
         <v>44943.69791666666</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G21" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H21">
         <v>2</v>
       </c>
       <c r="I21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K21">
-        <v>4.2</v>
+        <v>2</v>
       </c>
       <c r="L21">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="M21">
-        <v>1.75</v>
+        <v>3.5</v>
       </c>
       <c r="N21">
-        <v>3</v>
+        <v>2.05</v>
       </c>
       <c r="O21">
         <v>3.6</v>
       </c>
       <c r="P21">
-        <v>2.2</v>
+        <v>3.4</v>
       </c>
       <c r="Q21">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R21">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="S21">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="T21">
         <v>2.75</v>
       </c>
       <c r="U21">
+        <v>2.025</v>
+      </c>
+      <c r="V21">
         <v>1.825</v>
       </c>
-      <c r="V21">
-        <v>2.025</v>
-      </c>
       <c r="W21">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="X21">
         <v>-1</v>
       </c>
       <c r="Y21">
-        <v>1.2</v>
+        <v>-1</v>
       </c>
       <c r="Z21">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA21">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AB21">
+        <v>-1</v>
+      </c>
+      <c r="AC21">
         <v>0.825</v>
-      </c>
-      <c r="AC21">
-        <v>-1</v>
       </c>
     </row>
     <row r="22" spans="1:29">
@@ -2405,7 +2405,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>5208698</v>
+        <v>5208702</v>
       </c>
       <c r="C22" t="s">
         <v>28</v>
@@ -2417,76 +2417,76 @@
         <v>44943.69791666666</v>
       </c>
       <c r="F22" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="G22" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H22">
         <v>2</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K22">
-        <v>2</v>
+        <v>4.2</v>
       </c>
       <c r="L22">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="M22">
-        <v>3.5</v>
+        <v>1.75</v>
       </c>
       <c r="N22">
-        <v>2.05</v>
+        <v>3</v>
       </c>
       <c r="O22">
         <v>3.6</v>
       </c>
       <c r="P22">
-        <v>3.4</v>
+        <v>2.2</v>
       </c>
       <c r="Q22">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R22">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="S22">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="T22">
         <v>2.75</v>
       </c>
       <c r="U22">
+        <v>1.825</v>
+      </c>
+      <c r="V22">
         <v>2.025</v>
       </c>
-      <c r="V22">
-        <v>1.825</v>
-      </c>
       <c r="W22">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="X22">
         <v>-1</v>
       </c>
       <c r="Y22">
-        <v>-1</v>
+        <v>1.2</v>
       </c>
       <c r="Z22">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA22">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AB22">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AC22">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="23" spans="1:29">
@@ -3117,7 +3117,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>5208577</v>
+        <v>5208575</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
@@ -3129,40 +3129,40 @@
         <v>44947.59375</v>
       </c>
       <c r="F30" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G30" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I30">
         <v>2</v>
       </c>
       <c r="J30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K30">
-        <v>2.625</v>
+        <v>1.95</v>
       </c>
       <c r="L30">
+        <v>3.5</v>
+      </c>
+      <c r="M30">
         <v>3.4</v>
       </c>
-      <c r="M30">
-        <v>2.4</v>
-      </c>
       <c r="N30">
-        <v>3.2</v>
+        <v>1.75</v>
       </c>
       <c r="O30">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="P30">
-        <v>2.05</v>
+        <v>4</v>
       </c>
       <c r="Q30">
-        <v>0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R30">
         <v>2.025</v>
@@ -3171,34 +3171,34 @@
         <v>1.825</v>
       </c>
       <c r="T30">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U30">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="V30">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="W30">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="X30">
         <v>-1</v>
       </c>
       <c r="Y30">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z30">
-        <v>-1</v>
+        <v>0.5125</v>
       </c>
       <c r="AA30">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
       <c r="AB30">
-        <v>0.475</v>
+        <v>1</v>
       </c>
       <c r="AC30">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="31" spans="1:29">
@@ -3206,7 +3206,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>5208575</v>
+        <v>5208577</v>
       </c>
       <c r="C31" t="s">
         <v>28</v>
@@ -3218,40 +3218,40 @@
         <v>44947.59375</v>
       </c>
       <c r="F31" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G31" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="H31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <v>2</v>
       </c>
       <c r="J31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K31">
-        <v>1.95</v>
+        <v>2.625</v>
       </c>
       <c r="L31">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M31">
+        <v>2.4</v>
+      </c>
+      <c r="N31">
+        <v>3.2</v>
+      </c>
+      <c r="O31">
         <v>3.4</v>
       </c>
-      <c r="N31">
-        <v>1.75</v>
-      </c>
-      <c r="O31">
-        <v>3.6</v>
-      </c>
       <c r="P31">
-        <v>4</v>
+        <v>2.05</v>
       </c>
       <c r="Q31">
-        <v>-0.75</v>
+        <v>0.25</v>
       </c>
       <c r="R31">
         <v>2.025</v>
@@ -3260,34 +3260,34 @@
         <v>1.825</v>
       </c>
       <c r="T31">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U31">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="V31">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="W31">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="X31">
         <v>-1</v>
       </c>
       <c r="Y31">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z31">
-        <v>0.5125</v>
+        <v>-1</v>
       </c>
       <c r="AA31">
+        <v>0.825</v>
+      </c>
+      <c r="AB31">
+        <v>0.475</v>
+      </c>
+      <c r="AC31">
         <v>-0.5</v>
-      </c>
-      <c r="AB31">
-        <v>1</v>
-      </c>
-      <c r="AC31">
-        <v>-1</v>
       </c>
     </row>
     <row r="32" spans="1:29">
@@ -6410,7 +6410,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>5208596</v>
+        <v>5208593</v>
       </c>
       <c r="C67" t="s">
         <v>28</v>
@@ -6422,55 +6422,55 @@
         <v>44975.59375</v>
       </c>
       <c r="F67" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G67" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J67" t="s">
         <v>48</v>
       </c>
       <c r="K67">
-        <v>3.2</v>
+        <v>2.7</v>
       </c>
       <c r="L67">
         <v>3.4</v>
       </c>
       <c r="M67">
-        <v>2.2</v>
+        <v>2.5</v>
       </c>
       <c r="N67">
-        <v>3.1</v>
+        <v>3.8</v>
       </c>
       <c r="O67">
         <v>3.4</v>
       </c>
       <c r="P67">
-        <v>2.2</v>
+        <v>1.95</v>
       </c>
       <c r="Q67">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R67">
+        <v>1.875</v>
+      </c>
+      <c r="S67">
         <v>1.975</v>
       </c>
-      <c r="S67">
-        <v>1.875</v>
-      </c>
       <c r="T67">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U67">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="V67">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="W67">
         <v>-1</v>
@@ -6482,16 +6482,16 @@
         <v>-1</v>
       </c>
       <c r="Z67">
-        <v>0.4875</v>
+        <v>0.875</v>
       </c>
       <c r="AA67">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB67">
         <v>-1</v>
       </c>
       <c r="AC67">
-        <v>0.9750000000000001</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="68" spans="1:29">
@@ -6499,7 +6499,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>5208593</v>
+        <v>5208596</v>
       </c>
       <c r="C68" t="s">
         <v>28</v>
@@ -6511,55 +6511,55 @@
         <v>44975.59375</v>
       </c>
       <c r="F68" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G68" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J68" t="s">
         <v>48</v>
       </c>
       <c r="K68">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
       <c r="L68">
         <v>3.4</v>
       </c>
       <c r="M68">
-        <v>2.5</v>
+        <v>2.2</v>
       </c>
       <c r="N68">
-        <v>3.8</v>
+        <v>3.1</v>
       </c>
       <c r="O68">
         <v>3.4</v>
       </c>
       <c r="P68">
-        <v>1.95</v>
+        <v>2.2</v>
       </c>
       <c r="Q68">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R68">
+        <v>1.975</v>
+      </c>
+      <c r="S68">
         <v>1.875</v>
       </c>
-      <c r="S68">
+      <c r="T68">
+        <v>2.75</v>
+      </c>
+      <c r="U68">
+        <v>1.875</v>
+      </c>
+      <c r="V68">
         <v>1.975</v>
-      </c>
-      <c r="T68">
-        <v>2.5</v>
-      </c>
-      <c r="U68">
-        <v>1.925</v>
-      </c>
-      <c r="V68">
-        <v>1.925</v>
       </c>
       <c r="W68">
         <v>-1</v>
@@ -6571,16 +6571,16 @@
         <v>-1</v>
       </c>
       <c r="Z68">
-        <v>0.875</v>
+        <v>0.4875</v>
       </c>
       <c r="AA68">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB68">
         <v>-1</v>
       </c>
       <c r="AC68">
-        <v>0.925</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="69" spans="1:29">
@@ -8813,7 +8813,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>5208610</v>
+        <v>5208609</v>
       </c>
       <c r="C94" t="s">
         <v>28</v>
@@ -8825,73 +8825,73 @@
         <v>44996.59375</v>
       </c>
       <c r="F94" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G94" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="H94">
+        <v>3</v>
+      </c>
+      <c r="I94">
+        <v>1</v>
+      </c>
+      <c r="J94" t="s">
+        <v>50</v>
+      </c>
+      <c r="K94">
+        <v>1.615</v>
+      </c>
+      <c r="L94">
         <v>4</v>
       </c>
-      <c r="I94">
+      <c r="M94">
+        <v>4.75</v>
+      </c>
+      <c r="N94">
+        <v>1.615</v>
+      </c>
+      <c r="O94">
         <v>4</v>
       </c>
-      <c r="J94" t="s">
-        <v>48</v>
-      </c>
-      <c r="K94">
-        <v>2.25</v>
-      </c>
-      <c r="L94">
-        <v>3.4</v>
-      </c>
-      <c r="M94">
-        <v>2.9</v>
-      </c>
-      <c r="N94">
-        <v>2.5</v>
-      </c>
-      <c r="O94">
-        <v>3.4</v>
-      </c>
       <c r="P94">
-        <v>2.6</v>
+        <v>4.5</v>
       </c>
       <c r="Q94">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="R94">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="S94">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="T94">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U94">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="V94">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="W94">
-        <v>-1</v>
+        <v>0.615</v>
       </c>
       <c r="X94">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Y94">
         <v>-1</v>
       </c>
       <c r="Z94">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="AA94">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="AB94">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="AC94">
         <v>-1</v>
@@ -8902,7 +8902,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>5208609</v>
+        <v>5208610</v>
       </c>
       <c r="C95" t="s">
         <v>28</v>
@@ -8914,73 +8914,73 @@
         <v>44996.59375</v>
       </c>
       <c r="F95" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G95" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="H95">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I95">
+        <v>4</v>
+      </c>
+      <c r="J95" t="s">
+        <v>48</v>
+      </c>
+      <c r="K95">
+        <v>2.25</v>
+      </c>
+      <c r="L95">
+        <v>3.4</v>
+      </c>
+      <c r="M95">
+        <v>2.9</v>
+      </c>
+      <c r="N95">
+        <v>2.5</v>
+      </c>
+      <c r="O95">
+        <v>3.4</v>
+      </c>
+      <c r="P95">
+        <v>2.6</v>
+      </c>
+      <c r="Q95">
+        <v>0</v>
+      </c>
+      <c r="R95">
+        <v>1.875</v>
+      </c>
+      <c r="S95">
+        <v>1.975</v>
+      </c>
+      <c r="T95">
+        <v>2.75</v>
+      </c>
+      <c r="U95">
+        <v>2</v>
+      </c>
+      <c r="V95">
+        <v>1.85</v>
+      </c>
+      <c r="W95">
+        <v>-1</v>
+      </c>
+      <c r="X95">
+        <v>2.4</v>
+      </c>
+      <c r="Y95">
+        <v>-1</v>
+      </c>
+      <c r="Z95">
+        <v>0</v>
+      </c>
+      <c r="AA95">
+        <v>-0</v>
+      </c>
+      <c r="AB95">
         <v>1</v>
-      </c>
-      <c r="J95" t="s">
-        <v>50</v>
-      </c>
-      <c r="K95">
-        <v>1.615</v>
-      </c>
-      <c r="L95">
-        <v>4</v>
-      </c>
-      <c r="M95">
-        <v>4.75</v>
-      </c>
-      <c r="N95">
-        <v>1.615</v>
-      </c>
-      <c r="O95">
-        <v>4</v>
-      </c>
-      <c r="P95">
-        <v>4.5</v>
-      </c>
-      <c r="Q95">
-        <v>-1</v>
-      </c>
-      <c r="R95">
-        <v>2.05</v>
-      </c>
-      <c r="S95">
-        <v>1.8</v>
-      </c>
-      <c r="T95">
-        <v>3</v>
-      </c>
-      <c r="U95">
-        <v>1.95</v>
-      </c>
-      <c r="V95">
-        <v>1.9</v>
-      </c>
-      <c r="W95">
-        <v>0.615</v>
-      </c>
-      <c r="X95">
-        <v>-1</v>
-      </c>
-      <c r="Y95">
-        <v>-1</v>
-      </c>
-      <c r="Z95">
-        <v>1.05</v>
-      </c>
-      <c r="AA95">
-        <v>-1</v>
-      </c>
-      <c r="AB95">
-        <v>0.95</v>
       </c>
       <c r="AC95">
         <v>-1</v>
@@ -9614,7 +9614,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>5208613</v>
+        <v>5208612</v>
       </c>
       <c r="C103" t="s">
         <v>28</v>
@@ -9626,76 +9626,76 @@
         <v>45003.59375</v>
       </c>
       <c r="F103" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="G103" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H103">
+        <v>2</v>
+      </c>
+      <c r="I103">
         <v>1</v>
       </c>
-      <c r="I103">
-        <v>2</v>
-      </c>
       <c r="J103" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K103">
-        <v>3.3</v>
+        <v>1.45</v>
       </c>
       <c r="L103">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="M103">
-        <v>2.05</v>
+        <v>6</v>
       </c>
       <c r="N103">
-        <v>2.8</v>
+        <v>1.5</v>
       </c>
       <c r="O103">
-        <v>3.3</v>
+        <v>3.75</v>
       </c>
       <c r="P103">
-        <v>2.3</v>
+        <v>6.5</v>
       </c>
       <c r="Q103">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="R103">
+        <v>2</v>
+      </c>
+      <c r="S103">
         <v>1.85</v>
       </c>
-      <c r="S103">
-        <v>2</v>
-      </c>
       <c r="T103">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="U103">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="V103">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="W103">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="X103">
         <v>-1</v>
       </c>
       <c r="Y103">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="Z103">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA103">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="AB103">
-        <v>0.45</v>
+        <v>1.025</v>
       </c>
       <c r="AC103">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="104" spans="1:29">
@@ -9703,7 +9703,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>5208612</v>
+        <v>5208613</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9715,76 +9715,76 @@
         <v>45003.59375</v>
       </c>
       <c r="F104" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G104" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I104">
+        <v>2</v>
+      </c>
+      <c r="J104" t="s">
+        <v>49</v>
+      </c>
+      <c r="K104">
+        <v>3.3</v>
+      </c>
+      <c r="L104">
+        <v>3.3</v>
+      </c>
+      <c r="M104">
+        <v>2.05</v>
+      </c>
+      <c r="N104">
+        <v>2.8</v>
+      </c>
+      <c r="O104">
+        <v>3.3</v>
+      </c>
+      <c r="P104">
+        <v>2.3</v>
+      </c>
+      <c r="Q104">
+        <v>0.25</v>
+      </c>
+      <c r="R104">
+        <v>1.85</v>
+      </c>
+      <c r="S104">
+        <v>2</v>
+      </c>
+      <c r="T104">
+        <v>2.75</v>
+      </c>
+      <c r="U104">
+        <v>1.9</v>
+      </c>
+      <c r="V104">
+        <v>1.95</v>
+      </c>
+      <c r="W104">
+        <v>-1</v>
+      </c>
+      <c r="X104">
+        <v>-1</v>
+      </c>
+      <c r="Y104">
+        <v>1.3</v>
+      </c>
+      <c r="Z104">
+        <v>-1</v>
+      </c>
+      <c r="AA104">
         <v>1</v>
       </c>
-      <c r="J104" t="s">
-        <v>50</v>
-      </c>
-      <c r="K104">
-        <v>1.45</v>
-      </c>
-      <c r="L104">
-        <v>4</v>
-      </c>
-      <c r="M104">
-        <v>6</v>
-      </c>
-      <c r="N104">
-        <v>1.5</v>
-      </c>
-      <c r="O104">
-        <v>3.75</v>
-      </c>
-      <c r="P104">
-        <v>6.5</v>
-      </c>
-      <c r="Q104">
-        <v>-1</v>
-      </c>
-      <c r="R104">
-        <v>2</v>
-      </c>
-      <c r="S104">
-        <v>1.85</v>
-      </c>
-      <c r="T104">
-        <v>2.25</v>
-      </c>
-      <c r="U104">
-        <v>2.025</v>
-      </c>
-      <c r="V104">
-        <v>1.825</v>
-      </c>
-      <c r="W104">
-        <v>0.5</v>
-      </c>
-      <c r="X104">
-        <v>-1</v>
-      </c>
-      <c r="Y104">
-        <v>-1</v>
-      </c>
-      <c r="Z104">
-        <v>0</v>
-      </c>
-      <c r="AA104">
-        <v>-0</v>
-      </c>
       <c r="AB104">
-        <v>1.025</v>
+        <v>0.45</v>
       </c>
       <c r="AC104">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -10415,7 +10415,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>5351637</v>
+        <v>5356593</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10427,55 +10427,55 @@
         <v>45017.55208333334</v>
       </c>
       <c r="F112" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G112" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I112">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J112" t="s">
         <v>49</v>
       </c>
       <c r="K112">
-        <v>6.5</v>
+        <v>2</v>
       </c>
       <c r="L112">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="M112">
-        <v>1.444</v>
+        <v>3.25</v>
       </c>
       <c r="N112">
-        <v>9.5</v>
+        <v>2.1</v>
       </c>
       <c r="O112">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="P112">
-        <v>1.285</v>
+        <v>3.1</v>
       </c>
       <c r="Q112">
-        <v>1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R112">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="S112">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="T112">
         <v>2.75</v>
       </c>
       <c r="U112">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V112">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W112">
         <v>-1</v>
@@ -10484,16 +10484,16 @@
         <v>-1</v>
       </c>
       <c r="Y112">
-        <v>0.2849999999999999</v>
+        <v>2.1</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
-        <v>0.8999999999999999</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB112">
-        <v>0.875</v>
+        <v>0.95</v>
       </c>
       <c r="AC112">
         <v>-1</v>
@@ -10504,7 +10504,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>5356593</v>
+        <v>5351637</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10516,55 +10516,55 @@
         <v>45017.55208333334</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G113" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I113">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J113" t="s">
         <v>49</v>
       </c>
       <c r="K113">
-        <v>2</v>
+        <v>6.5</v>
       </c>
       <c r="L113">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="M113">
-        <v>3.25</v>
+        <v>1.444</v>
       </c>
       <c r="N113">
-        <v>2.1</v>
+        <v>9.5</v>
       </c>
       <c r="O113">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="P113">
-        <v>3.1</v>
+        <v>1.285</v>
       </c>
       <c r="Q113">
-        <v>-0.25</v>
+        <v>1.5</v>
       </c>
       <c r="R113">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="S113">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="T113">
         <v>2.75</v>
       </c>
       <c r="U113">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V113">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="W113">
         <v>-1</v>
@@ -10573,16 +10573,16 @@
         <v>-1</v>
       </c>
       <c r="Y113">
-        <v>2.1</v>
+        <v>0.2849999999999999</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
-        <v>0.9750000000000001</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB113">
-        <v>0.95</v>
+        <v>0.875</v>
       </c>
       <c r="AC113">
         <v>-1</v>
@@ -12907,7 +12907,7 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>6385540</v>
+        <v>6390066</v>
       </c>
       <c r="C140" t="s">
         <v>28</v>
@@ -12919,10 +12919,10 @@
         <v>45039.5625</v>
       </c>
       <c r="F140" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G140" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="H140">
         <v>2</v>
@@ -12934,40 +12934,40 @@
         <v>49</v>
       </c>
       <c r="K140">
-        <v>1.363</v>
+        <v>3</v>
       </c>
       <c r="L140">
-        <v>5</v>
+        <v>3.6</v>
       </c>
       <c r="M140">
-        <v>7</v>
+        <v>2.15</v>
       </c>
       <c r="N140">
-        <v>1.55</v>
+        <v>2.8</v>
       </c>
       <c r="O140">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P140">
-        <v>5</v>
+        <v>2.25</v>
       </c>
       <c r="Q140">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R140">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="S140">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="T140">
         <v>3</v>
       </c>
       <c r="U140">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="V140">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="W140">
         <v>-1</v>
@@ -12976,16 +12976,16 @@
         <v>-1</v>
       </c>
       <c r="Y140">
-        <v>4</v>
+        <v>1.25</v>
       </c>
       <c r="Z140">
         <v>-1</v>
       </c>
       <c r="AA140">
-        <v>0.925</v>
+        <v>1.025</v>
       </c>
       <c r="AB140">
-        <v>0.875</v>
+        <v>0.8</v>
       </c>
       <c r="AC140">
         <v>-1</v>
@@ -13085,7 +13085,7 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>6390066</v>
+        <v>6389865</v>
       </c>
       <c r="C142" t="s">
         <v>28</v>
@@ -13097,73 +13097,73 @@
         <v>45039.5625</v>
       </c>
       <c r="F142" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="G142" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H142">
         <v>2</v>
       </c>
       <c r="I142">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J142" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K142">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="L142">
         <v>3.6</v>
       </c>
       <c r="M142">
-        <v>2.15</v>
+        <v>1.95</v>
       </c>
       <c r="N142">
         <v>2.8</v>
       </c>
       <c r="O142">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="P142">
-        <v>2.25</v>
+        <v>2.3</v>
       </c>
       <c r="Q142">
         <v>0.25</v>
       </c>
       <c r="R142">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="S142">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="T142">
         <v>3</v>
       </c>
       <c r="U142">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="V142">
-        <v>2.05</v>
+        <v>1.9</v>
       </c>
       <c r="W142">
         <v>-1</v>
       </c>
       <c r="X142">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y142">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="Z142">
-        <v>-1</v>
+        <v>0.4</v>
       </c>
       <c r="AA142">
-        <v>1.025</v>
+        <v>-0.5</v>
       </c>
       <c r="AB142">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="AC142">
         <v>-1</v>
@@ -13174,7 +13174,7 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>6389865</v>
+        <v>6385540</v>
       </c>
       <c r="C143" t="s">
         <v>28</v>
@@ -13186,73 +13186,73 @@
         <v>45039.5625</v>
       </c>
       <c r="F143" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G143" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H143">
         <v>2</v>
       </c>
       <c r="I143">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J143" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K143">
-        <v>3.5</v>
+        <v>1.363</v>
       </c>
       <c r="L143">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="M143">
-        <v>1.95</v>
+        <v>7</v>
       </c>
       <c r="N143">
-        <v>2.8</v>
+        <v>1.55</v>
       </c>
       <c r="O143">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="P143">
-        <v>2.3</v>
+        <v>5</v>
       </c>
       <c r="Q143">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="R143">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="S143">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="T143">
         <v>3</v>
       </c>
       <c r="U143">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V143">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="W143">
         <v>-1</v>
       </c>
       <c r="X143">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y143">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="Z143">
-        <v>0.4</v>
+        <v>-1</v>
       </c>
       <c r="AA143">
-        <v>-0.5</v>
+        <v>0.925</v>
       </c>
       <c r="AB143">
-        <v>0.95</v>
+        <v>0.875</v>
       </c>
       <c r="AC143">
         <v>-1</v>
@@ -15399,7 +15399,7 @@
         <v>166</v>
       </c>
       <c r="B168">
-        <v>6576988</v>
+        <v>6576065</v>
       </c>
       <c r="C168" t="s">
         <v>28</v>
@@ -15411,73 +15411,73 @@
         <v>45081.5625</v>
       </c>
       <c r="F168" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G168" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H168">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I168">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J168" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K168">
-        <v>2.4</v>
+        <v>1.75</v>
       </c>
       <c r="L168">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="M168">
-        <v>2.7</v>
+        <v>4.2</v>
       </c>
       <c r="N168">
-        <v>2.4</v>
+        <v>1.55</v>
       </c>
       <c r="O168">
-        <v>3.6</v>
+        <v>4.333</v>
       </c>
       <c r="P168">
-        <v>2.7</v>
+        <v>4.75</v>
       </c>
       <c r="Q168">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="R168">
-        <v>2.05</v>
+        <v>1.975</v>
       </c>
       <c r="S168">
-        <v>1.75</v>
+        <v>1.875</v>
       </c>
       <c r="T168">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U168">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="V168">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="W168">
         <v>-1</v>
       </c>
       <c r="X168">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Y168">
-        <v>-1</v>
+        <v>3.75</v>
       </c>
       <c r="Z168">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AA168">
-        <v>0.375</v>
+        <v>0.875</v>
       </c>
       <c r="AB168">
-        <v>0.95</v>
+        <v>1.025</v>
       </c>
       <c r="AC168">
         <v>-1</v>
@@ -15488,7 +15488,7 @@
         <v>167</v>
       </c>
       <c r="B169">
-        <v>6576065</v>
+        <v>6576988</v>
       </c>
       <c r="C169" t="s">
         <v>28</v>
@@ -15500,73 +15500,73 @@
         <v>45081.5625</v>
       </c>
       <c r="F169" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G169" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H169">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I169">
+        <v>2</v>
+      </c>
+      <c r="J169" t="s">
+        <v>48</v>
+      </c>
+      <c r="K169">
+        <v>2.4</v>
+      </c>
+      <c r="L169">
+        <v>3.6</v>
+      </c>
+      <c r="M169">
+        <v>2.7</v>
+      </c>
+      <c r="N169">
+        <v>2.4</v>
+      </c>
+      <c r="O169">
+        <v>3.6</v>
+      </c>
+      <c r="P169">
+        <v>2.7</v>
+      </c>
+      <c r="Q169">
+        <v>-0.25</v>
+      </c>
+      <c r="R169">
+        <v>2.05</v>
+      </c>
+      <c r="S169">
+        <v>1.75</v>
+      </c>
+      <c r="T169">
         <v>3</v>
       </c>
-      <c r="J169" t="s">
-        <v>49</v>
-      </c>
-      <c r="K169">
-        <v>1.75</v>
-      </c>
-      <c r="L169">
-        <v>3.8</v>
-      </c>
-      <c r="M169">
-        <v>4.2</v>
-      </c>
-      <c r="N169">
-        <v>1.55</v>
-      </c>
-      <c r="O169">
-        <v>4.333</v>
-      </c>
-      <c r="P169">
-        <v>4.75</v>
-      </c>
-      <c r="Q169">
-        <v>-1</v>
-      </c>
-      <c r="R169">
-        <v>1.975</v>
-      </c>
-      <c r="S169">
-        <v>1.875</v>
-      </c>
-      <c r="T169">
-        <v>3.25</v>
-      </c>
       <c r="U169">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="V169">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="W169">
         <v>-1</v>
       </c>
       <c r="X169">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Y169">
-        <v>3.75</v>
+        <v>-1</v>
       </c>
       <c r="Z169">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AA169">
-        <v>0.875</v>
+        <v>0.375</v>
       </c>
       <c r="AB169">
-        <v>1.025</v>
+        <v>0.95</v>
       </c>
       <c r="AC169">
         <v>-1</v>
@@ -18069,7 +18069,7 @@
         <v>196</v>
       </c>
       <c r="B198">
-        <v>6810015</v>
+        <v>6810012</v>
       </c>
       <c r="C198" t="s">
         <v>28</v>
@@ -18081,61 +18081,61 @@
         <v>45158.45833333334</v>
       </c>
       <c r="F198" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="G198" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H198">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I198">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J198" t="s">
         <v>48</v>
       </c>
       <c r="K198">
-        <v>1.45</v>
+        <v>1.533</v>
       </c>
       <c r="L198">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="M198">
-        <v>7</v>
+        <v>5.5</v>
       </c>
       <c r="N198">
-        <v>1.533</v>
+        <v>1.6</v>
       </c>
       <c r="O198">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="P198">
-        <v>6</v>
+        <v>5.25</v>
       </c>
       <c r="Q198">
         <v>-1</v>
       </c>
       <c r="R198">
+        <v>1.975</v>
+      </c>
+      <c r="S198">
+        <v>1.875</v>
+      </c>
+      <c r="T198">
+        <v>3</v>
+      </c>
+      <c r="U198">
         <v>1.9</v>
       </c>
-      <c r="S198">
+      <c r="V198">
         <v>1.95</v>
       </c>
-      <c r="T198">
-        <v>2.5</v>
-      </c>
-      <c r="U198">
-        <v>1.8</v>
-      </c>
-      <c r="V198">
-        <v>2.05</v>
-      </c>
       <c r="W198">
         <v>-1</v>
       </c>
       <c r="X198">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Y198">
         <v>-1</v>
@@ -18144,13 +18144,13 @@
         <v>-1</v>
       </c>
       <c r="AA198">
+        <v>0.875</v>
+      </c>
+      <c r="AB198">
+        <v>-1</v>
+      </c>
+      <c r="AC198">
         <v>0.95</v>
-      </c>
-      <c r="AB198">
-        <v>0.8</v>
-      </c>
-      <c r="AC198">
-        <v>-1</v>
       </c>
     </row>
     <row r="199" spans="1:29">
@@ -18158,7 +18158,7 @@
         <v>197</v>
       </c>
       <c r="B199">
-        <v>6810012</v>
+        <v>6810015</v>
       </c>
       <c r="C199" t="s">
         <v>28</v>
@@ -18170,61 +18170,61 @@
         <v>45158.45833333334</v>
       </c>
       <c r="F199" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="G199" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H199">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I199">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J199" t="s">
         <v>48</v>
       </c>
       <c r="K199">
+        <v>1.45</v>
+      </c>
+      <c r="L199">
+        <v>4.5</v>
+      </c>
+      <c r="M199">
+        <v>7</v>
+      </c>
+      <c r="N199">
         <v>1.533</v>
       </c>
-      <c r="L199">
+      <c r="O199">
         <v>4.2</v>
       </c>
-      <c r="M199">
-        <v>5.5</v>
-      </c>
-      <c r="N199">
-        <v>1.6</v>
-      </c>
-      <c r="O199">
-        <v>4</v>
-      </c>
       <c r="P199">
-        <v>5.25</v>
+        <v>6</v>
       </c>
       <c r="Q199">
         <v>-1</v>
       </c>
       <c r="R199">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="S199">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="T199">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="U199">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="V199">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="W199">
         <v>-1</v>
       </c>
       <c r="X199">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="Y199">
         <v>-1</v>
@@ -18233,13 +18233,13 @@
         <v>-1</v>
       </c>
       <c r="AA199">
-        <v>0.875</v>
+        <v>0.95</v>
       </c>
       <c r="AB199">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AC199">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="200" spans="1:29">
@@ -28838,7 +28838,7 @@
         <v>317</v>
       </c>
       <c r="B319">
-        <v>6810132</v>
+        <v>6810130</v>
       </c>
       <c r="C319" t="s">
         <v>28</v>
@@ -28850,76 +28850,76 @@
         <v>45283.59375</v>
       </c>
       <c r="F319" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="G319" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H319">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I319">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J319" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K319">
-        <v>2.2</v>
+        <v>1.363</v>
       </c>
       <c r="L319">
-        <v>3.4</v>
+        <v>5</v>
       </c>
       <c r="M319">
-        <v>3.2</v>
+        <v>7.5</v>
       </c>
       <c r="N319">
-        <v>2.3</v>
+        <v>1.333</v>
       </c>
       <c r="O319">
-        <v>3.3</v>
+        <v>5.25</v>
       </c>
       <c r="P319">
+        <v>8</v>
+      </c>
+      <c r="Q319">
+        <v>-1.5</v>
+      </c>
+      <c r="R319">
+        <v>1.9</v>
+      </c>
+      <c r="S319">
+        <v>1.95</v>
+      </c>
+      <c r="T319">
         <v>3</v>
       </c>
-      <c r="Q319">
-        <v>-0.25</v>
-      </c>
-      <c r="R319">
-        <v>2</v>
-      </c>
-      <c r="S319">
-        <v>1.85</v>
-      </c>
-      <c r="T319">
-        <v>2.25</v>
-      </c>
       <c r="U319">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="V319">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="W319">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="X319">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y319">
         <v>-1</v>
       </c>
       <c r="Z319">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AA319">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB319">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AC319">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="320" spans="1:29">
@@ -28927,7 +28927,7 @@
         <v>318</v>
       </c>
       <c r="B320">
-        <v>6810130</v>
+        <v>6810132</v>
       </c>
       <c r="C320" t="s">
         <v>28</v>
@@ -28939,76 +28939,76 @@
         <v>45283.59375</v>
       </c>
       <c r="F320" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="G320" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="H320">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I320">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J320" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K320">
-        <v>1.363</v>
+        <v>2.2</v>
       </c>
       <c r="L320">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="M320">
-        <v>7.5</v>
+        <v>3.2</v>
       </c>
       <c r="N320">
-        <v>1.333</v>
+        <v>2.3</v>
       </c>
       <c r="O320">
-        <v>5.25</v>
+        <v>3.3</v>
       </c>
       <c r="P320">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="Q320">
-        <v>-1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R320">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="S320">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="T320">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="U320">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="V320">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="W320">
-        <v>-1</v>
+        <v>1.3</v>
       </c>
       <c r="X320">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y320">
         <v>-1</v>
       </c>
       <c r="Z320">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AA320">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB320">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AC320">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321" spans="1:29">
@@ -29194,7 +29194,7 @@
         <v>321</v>
       </c>
       <c r="B323">
-        <v>6810145</v>
+        <v>6810142</v>
       </c>
       <c r="C323" t="s">
         <v>28</v>
@@ -29206,76 +29206,76 @@
         <v>45286.5</v>
       </c>
       <c r="F323" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G323" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="H323">
+        <v>3</v>
+      </c>
+      <c r="I323">
         <v>0</v>
       </c>
-      <c r="I323">
-        <v>2</v>
-      </c>
       <c r="J323" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K323">
-        <v>7</v>
+        <v>1.75</v>
       </c>
       <c r="L323">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M323">
-        <v>1.4</v>
+        <v>4</v>
       </c>
       <c r="N323">
-        <v>8.5</v>
+        <v>1.8</v>
       </c>
       <c r="O323">
-        <v>5.75</v>
+        <v>3.8</v>
       </c>
       <c r="P323">
-        <v>1.285</v>
+        <v>3.8</v>
       </c>
       <c r="Q323">
-        <v>1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="R323">
+        <v>1.825</v>
+      </c>
+      <c r="S323">
         <v>2.025</v>
       </c>
-      <c r="S323">
-        <v>1.825</v>
-      </c>
       <c r="T323">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U323">
-        <v>2.05</v>
+        <v>1.975</v>
       </c>
       <c r="V323">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="W323">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="X323">
         <v>-1</v>
       </c>
       <c r="Y323">
-        <v>0.2849999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z323">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AA323">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB323">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC323">
-        <v>0.8</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="324" spans="1:29">
@@ -29283,7 +29283,7 @@
         <v>322</v>
       </c>
       <c r="B324">
-        <v>6810142</v>
+        <v>6810145</v>
       </c>
       <c r="C324" t="s">
         <v>28</v>
@@ -29295,76 +29295,76 @@
         <v>45286.5</v>
       </c>
       <c r="F324" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G324" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="H324">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I324">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J324" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K324">
-        <v>1.75</v>
+        <v>7</v>
       </c>
       <c r="L324">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M324">
-        <v>4</v>
+        <v>1.4</v>
       </c>
       <c r="N324">
+        <v>8.5</v>
+      </c>
+      <c r="O324">
+        <v>5.75</v>
+      </c>
+      <c r="P324">
+        <v>1.285</v>
+      </c>
+      <c r="Q324">
+        <v>1.5</v>
+      </c>
+      <c r="R324">
+        <v>2.025</v>
+      </c>
+      <c r="S324">
+        <v>1.825</v>
+      </c>
+      <c r="T324">
+        <v>3.25</v>
+      </c>
+      <c r="U324">
+        <v>2.05</v>
+      </c>
+      <c r="V324">
         <v>1.8</v>
       </c>
-      <c r="O324">
-        <v>3.8</v>
-      </c>
-      <c r="P324">
-        <v>3.8</v>
-      </c>
-      <c r="Q324">
-        <v>-0.5</v>
-      </c>
-      <c r="R324">
-        <v>1.825</v>
-      </c>
-      <c r="S324">
-        <v>2.025</v>
-      </c>
-      <c r="T324">
-        <v>3</v>
-      </c>
-      <c r="U324">
-        <v>1.975</v>
-      </c>
-      <c r="V324">
-        <v>1.875</v>
-      </c>
       <c r="W324">
+        <v>-1</v>
+      </c>
+      <c r="X324">
+        <v>-1</v>
+      </c>
+      <c r="Y324">
+        <v>0.2849999999999999</v>
+      </c>
+      <c r="Z324">
+        <v>-1</v>
+      </c>
+      <c r="AA324">
+        <v>0.825</v>
+      </c>
+      <c r="AB324">
+        <v>-1</v>
+      </c>
+      <c r="AC324">
         <v>0.8</v>
-      </c>
-      <c r="X324">
-        <v>-1</v>
-      </c>
-      <c r="Y324">
-        <v>-1</v>
-      </c>
-      <c r="Z324">
-        <v>0.825</v>
-      </c>
-      <c r="AA324">
-        <v>-1</v>
-      </c>
-      <c r="AB324">
-        <v>0</v>
-      </c>
-      <c r="AC324">
-        <v>-0</v>
       </c>
     </row>
     <row r="325" spans="1:29">
@@ -29639,7 +29639,7 @@
         <v>326</v>
       </c>
       <c r="B328">
-        <v>6810143</v>
+        <v>6810139</v>
       </c>
       <c r="C328" t="s">
         <v>28</v>
@@ -29651,58 +29651,58 @@
         <v>45287.69791666666</v>
       </c>
       <c r="F328" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G328" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="H328">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I328">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J328" t="s">
         <v>50</v>
       </c>
       <c r="K328">
+        <v>1.869</v>
+      </c>
+      <c r="L328">
+        <v>3.7</v>
+      </c>
+      <c r="M328">
+        <v>3.8</v>
+      </c>
+      <c r="N328">
         <v>2.05</v>
       </c>
-      <c r="L328">
-        <v>3.4</v>
-      </c>
-      <c r="M328">
-        <v>3.5</v>
-      </c>
-      <c r="N328">
-        <v>2.375</v>
-      </c>
       <c r="O328">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="P328">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="Q328">
         <v>-0.25</v>
       </c>
       <c r="R328">
+        <v>1.825</v>
+      </c>
+      <c r="S328">
         <v>2.025</v>
       </c>
-      <c r="S328">
-        <v>1.825</v>
-      </c>
       <c r="T328">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="U328">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="V328">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="W328">
-        <v>1.375</v>
+        <v>1.05</v>
       </c>
       <c r="X328">
         <v>-1</v>
@@ -29711,16 +29711,16 @@
         <v>-1</v>
       </c>
       <c r="Z328">
-        <v>1.025</v>
+        <v>0.825</v>
       </c>
       <c r="AA328">
         <v>-1</v>
       </c>
       <c r="AB328">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AC328">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="329" spans="1:29">
@@ -29728,7 +29728,7 @@
         <v>327</v>
       </c>
       <c r="B329">
-        <v>6810139</v>
+        <v>6810143</v>
       </c>
       <c r="C329" t="s">
         <v>28</v>
@@ -29740,58 +29740,58 @@
         <v>45287.69791666666</v>
       </c>
       <c r="F329" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="G329" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="H329">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I329">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J329" t="s">
         <v>50</v>
       </c>
       <c r="K329">
-        <v>1.869</v>
+        <v>2.05</v>
       </c>
       <c r="L329">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="M329">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="N329">
-        <v>2.05</v>
+        <v>2.375</v>
       </c>
       <c r="O329">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="P329">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="Q329">
         <v>-0.25</v>
       </c>
       <c r="R329">
+        <v>2.025</v>
+      </c>
+      <c r="S329">
         <v>1.825</v>
       </c>
-      <c r="S329">
+      <c r="T329">
+        <v>2.25</v>
+      </c>
+      <c r="U329">
         <v>2.025</v>
       </c>
-      <c r="T329">
-        <v>2.75</v>
-      </c>
-      <c r="U329">
-        <v>1.9</v>
-      </c>
       <c r="V329">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="W329">
-        <v>1.05</v>
+        <v>1.375</v>
       </c>
       <c r="X329">
         <v>-1</v>
@@ -29800,16 +29800,16 @@
         <v>-1</v>
       </c>
       <c r="Z329">
-        <v>0.825</v>
+        <v>1.025</v>
       </c>
       <c r="AA329">
         <v>-1</v>
       </c>
       <c r="AB329">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AC329">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="330" spans="1:29">
@@ -31330,7 +31330,7 @@
         <v>345</v>
       </c>
       <c r="B347">
-        <v>6810165</v>
+        <v>6810168</v>
       </c>
       <c r="C347" t="s">
         <v>28</v>
@@ -31342,58 +31342,58 @@
         <v>45322.61458333334</v>
       </c>
       <c r="F347" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G347" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H347">
+        <v>2</v>
+      </c>
+      <c r="I347">
         <v>1</v>
-      </c>
-      <c r="I347">
-        <v>0</v>
       </c>
       <c r="J347" t="s">
         <v>50</v>
       </c>
       <c r="K347">
-        <v>1.6</v>
+        <v>4.5</v>
       </c>
       <c r="L347">
+        <v>4.2</v>
+      </c>
+      <c r="M347">
+        <v>1.666</v>
+      </c>
+      <c r="N347">
+        <v>4.333</v>
+      </c>
+      <c r="O347">
         <v>4</v>
       </c>
-      <c r="M347">
-        <v>5</v>
-      </c>
-      <c r="N347">
-        <v>1.8</v>
-      </c>
-      <c r="O347">
-        <v>3.75</v>
-      </c>
       <c r="P347">
-        <v>4.2</v>
+        <v>1.7</v>
       </c>
       <c r="Q347">
-        <v>-0.75</v>
+        <v>0.75</v>
       </c>
       <c r="R347">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="S347">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="T347">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U347">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="V347">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="W347">
-        <v>0.8</v>
+        <v>3.333</v>
       </c>
       <c r="X347">
         <v>-1</v>
@@ -31402,16 +31402,16 @@
         <v>-1</v>
       </c>
       <c r="Z347">
-        <v>0.5249999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="AA347">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB347">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC347">
-        <v>0.8999999999999999</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="348" spans="1:29">
@@ -31419,7 +31419,7 @@
         <v>346</v>
       </c>
       <c r="B348">
-        <v>6810168</v>
+        <v>6810165</v>
       </c>
       <c r="C348" t="s">
         <v>28</v>
@@ -31431,58 +31431,58 @@
         <v>45322.61458333334</v>
       </c>
       <c r="F348" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G348" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H348">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I348">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J348" t="s">
         <v>50</v>
       </c>
       <c r="K348">
-        <v>4.5</v>
+        <v>1.6</v>
       </c>
       <c r="L348">
+        <v>4</v>
+      </c>
+      <c r="M348">
+        <v>5</v>
+      </c>
+      <c r="N348">
+        <v>1.8</v>
+      </c>
+      <c r="O348">
+        <v>3.75</v>
+      </c>
+      <c r="P348">
         <v>4.2</v>
       </c>
-      <c r="M348">
-        <v>1.666</v>
-      </c>
-      <c r="N348">
-        <v>4.333</v>
-      </c>
-      <c r="O348">
-        <v>4</v>
-      </c>
-      <c r="P348">
-        <v>1.7</v>
-      </c>
       <c r="Q348">
-        <v>0.75</v>
+        <v>-0.75</v>
       </c>
       <c r="R348">
+        <v>2.05</v>
+      </c>
+      <c r="S348">
+        <v>1.8</v>
+      </c>
+      <c r="T348">
+        <v>2.75</v>
+      </c>
+      <c r="U348">
         <v>1.95</v>
       </c>
-      <c r="S348">
+      <c r="V348">
         <v>1.9</v>
       </c>
-      <c r="T348">
-        <v>3</v>
-      </c>
-      <c r="U348">
-        <v>1.975</v>
-      </c>
-      <c r="V348">
-        <v>1.875</v>
-      </c>
       <c r="W348">
-        <v>3.333</v>
+        <v>0.8</v>
       </c>
       <c r="X348">
         <v>-1</v>
@@ -31491,16 +31491,16 @@
         <v>-1</v>
       </c>
       <c r="Z348">
-        <v>0.95</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AA348">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB348">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC348">
-        <v>-0</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="349" spans="1:29">
@@ -31686,7 +31686,7 @@
         <v>349</v>
       </c>
       <c r="B351">
-        <v>6810166</v>
+        <v>6810163</v>
       </c>
       <c r="C351" t="s">
         <v>28</v>
@@ -31698,73 +31698,73 @@
         <v>45323.6875</v>
       </c>
       <c r="F351" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G351" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H351">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I351">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J351" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K351">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="L351">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M351">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="N351">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="O351">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="P351">
-        <v>2.2</v>
+        <v>2.15</v>
       </c>
       <c r="Q351">
         <v>0.25</v>
       </c>
       <c r="R351">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="S351">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="T351">
         <v>2.5</v>
       </c>
       <c r="U351">
+        <v>1.975</v>
+      </c>
+      <c r="V351">
         <v>1.875</v>
       </c>
-      <c r="V351">
-        <v>1.975</v>
-      </c>
       <c r="W351">
-        <v>-1</v>
+        <v>2.25</v>
       </c>
       <c r="X351">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y351">
         <v>-1</v>
       </c>
       <c r="Z351">
-        <v>0.4625</v>
+        <v>0.95</v>
       </c>
       <c r="AA351">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB351">
-        <v>0.875</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC351">
         <v>-1</v>
@@ -31775,7 +31775,7 @@
         <v>350</v>
       </c>
       <c r="B352">
-        <v>6810163</v>
+        <v>6810166</v>
       </c>
       <c r="C352" t="s">
         <v>28</v>
@@ -31787,73 +31787,73 @@
         <v>45323.6875</v>
       </c>
       <c r="F352" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G352" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H352">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I352">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J352" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K352">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="L352">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M352">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="N352">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="O352">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P352">
-        <v>2.15</v>
+        <v>2.2</v>
       </c>
       <c r="Q352">
         <v>0.25</v>
       </c>
       <c r="R352">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="S352">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="T352">
         <v>2.5</v>
       </c>
       <c r="U352">
+        <v>1.875</v>
+      </c>
+      <c r="V352">
         <v>1.975</v>
       </c>
-      <c r="V352">
-        <v>1.875</v>
-      </c>
       <c r="W352">
-        <v>2.25</v>
+        <v>-1</v>
       </c>
       <c r="X352">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y352">
         <v>-1</v>
       </c>
       <c r="Z352">
-        <v>0.95</v>
+        <v>0.4625</v>
       </c>
       <c r="AA352">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB352">
-        <v>0.9750000000000001</v>
+        <v>0.875</v>
       </c>
       <c r="AC352">
         <v>-1</v>
@@ -32665,7 +32665,7 @@
         <v>360</v>
       </c>
       <c r="B362">
-        <v>6810179</v>
+        <v>6810184</v>
       </c>
       <c r="C362" t="s">
         <v>28</v>
@@ -32674,43 +32674,52 @@
         <v>28</v>
       </c>
       <c r="E362" s="2">
-        <v>45333.39583333334</v>
+        <v>45332.5</v>
       </c>
       <c r="F362" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="G362" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="H362">
+        <v>1</v>
+      </c>
+      <c r="I362">
+        <v>0</v>
+      </c>
+      <c r="J362" t="s">
+        <v>50</v>
       </c>
       <c r="K362">
-        <v>5.25</v>
+        <v>1.833</v>
       </c>
       <c r="L362">
+        <v>3.6</v>
+      </c>
+      <c r="M362">
+        <v>3.75</v>
+      </c>
+      <c r="N362">
+        <v>1.909</v>
+      </c>
+      <c r="O362">
+        <v>3.5</v>
+      </c>
+      <c r="P362">
         <v>4</v>
       </c>
-      <c r="M362">
-        <v>1.55</v>
-      </c>
-      <c r="N362">
-        <v>5</v>
-      </c>
-      <c r="O362">
-        <v>4.2</v>
-      </c>
-      <c r="P362">
-        <v>1.615</v>
-      </c>
       <c r="Q362">
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="R362">
-        <v>2.05</v>
+        <v>1.85</v>
       </c>
       <c r="S362">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="T362">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U362">
         <v>1.975</v>
@@ -32719,19 +32728,25 @@
         <v>1.875</v>
       </c>
       <c r="W362">
-        <v>0</v>
+        <v>0.909</v>
       </c>
       <c r="X362">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y362">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z362">
-        <v>0</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA362">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB362">
+        <v>-1</v>
+      </c>
+      <c r="AC362">
+        <v>0.875</v>
       </c>
     </row>
     <row r="363" spans="1:29">
@@ -32739,7 +32754,7 @@
         <v>361</v>
       </c>
       <c r="B363">
-        <v>6810182</v>
+        <v>6810186</v>
       </c>
       <c r="C363" t="s">
         <v>28</v>
@@ -32748,64 +32763,79 @@
         <v>28</v>
       </c>
       <c r="E363" s="2">
-        <v>45333.5</v>
+        <v>45332.59375</v>
       </c>
       <c r="F363" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G363" t="s">
-        <v>34</v>
+        <v>38</v>
+      </c>
+      <c r="H363">
+        <v>2</v>
+      </c>
+      <c r="I363">
+        <v>2</v>
+      </c>
+      <c r="J363" t="s">
+        <v>48</v>
       </c>
       <c r="K363">
-        <v>3.8</v>
+        <v>1.285</v>
       </c>
       <c r="L363">
-        <v>3.6</v>
+        <v>5.5</v>
       </c>
       <c r="M363">
+        <v>8.5</v>
+      </c>
+      <c r="N363">
+        <v>1.285</v>
+      </c>
+      <c r="O363">
+        <v>6</v>
+      </c>
+      <c r="P363">
+        <v>9</v>
+      </c>
+      <c r="Q363">
+        <v>-1.75</v>
+      </c>
+      <c r="R363">
+        <v>2.025</v>
+      </c>
+      <c r="S363">
+        <v>1.825</v>
+      </c>
+      <c r="T363">
+        <v>3</v>
+      </c>
+      <c r="U363">
         <v>1.85</v>
       </c>
-      <c r="N363">
-        <v>3.5</v>
-      </c>
-      <c r="O363">
-        <v>3.5</v>
-      </c>
-      <c r="P363">
-        <v>2</v>
-      </c>
-      <c r="Q363">
-        <v>0.5</v>
-      </c>
-      <c r="R363">
-        <v>1.825</v>
-      </c>
-      <c r="S363">
-        <v>2.025</v>
-      </c>
-      <c r="T363">
-        <v>2.75</v>
-      </c>
-      <c r="U363">
-        <v>2.025</v>
-      </c>
       <c r="V363">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="W363">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X363">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y363">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z363">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA363">
-        <v>0</v>
+        <v>0.825</v>
+      </c>
+      <c r="AB363">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AC363">
+        <v>-1</v>
       </c>
     </row>
     <row r="364" spans="1:29">
@@ -32813,7 +32843,7 @@
         <v>362</v>
       </c>
       <c r="B364">
-        <v>6810180</v>
+        <v>6810185</v>
       </c>
       <c r="C364" t="s">
         <v>28</v>
@@ -32822,64 +32852,79 @@
         <v>28</v>
       </c>
       <c r="E364" s="2">
-        <v>45333.60416666666</v>
+        <v>45332.69791666666</v>
       </c>
       <c r="F364" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G364" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="H364">
+        <v>4</v>
+      </c>
+      <c r="I364">
+        <v>0</v>
+      </c>
+      <c r="J364" t="s">
+        <v>50</v>
       </c>
       <c r="K364">
-        <v>3.6</v>
+        <v>1.2</v>
       </c>
       <c r="L364">
-        <v>3.4</v>
+        <v>6.5</v>
       </c>
       <c r="M364">
-        <v>2</v>
+        <v>9.5</v>
       </c>
       <c r="N364">
-        <v>3.75</v>
+        <v>1.222</v>
       </c>
       <c r="O364">
-        <v>3.4</v>
+        <v>6.5</v>
       </c>
       <c r="P364">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="Q364">
-        <v>0.5</v>
+        <v>-1.75</v>
       </c>
       <c r="R364">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="S364">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="T364">
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="U364">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V364">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="W364">
-        <v>0</v>
+        <v>0.222</v>
       </c>
       <c r="X364">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y364">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z364">
-        <v>0</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA364">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB364">
+        <v>1</v>
+      </c>
+      <c r="AC364">
+        <v>-1</v>
       </c>
     </row>
     <row r="365" spans="1:29">
@@ -32887,7 +32932,7 @@
         <v>363</v>
       </c>
       <c r="B365">
-        <v>6810181</v>
+        <v>6810179</v>
       </c>
       <c r="C365" t="s">
         <v>28</v>
@@ -32896,63 +32941,937 @@
         <v>28</v>
       </c>
       <c r="E365" s="2">
-        <v>45333.63541666666</v>
+        <v>45333.39583333334</v>
       </c>
       <c r="F365" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G365" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="H365">
+        <v>0</v>
+      </c>
+      <c r="I365">
+        <v>4</v>
+      </c>
+      <c r="J365" t="s">
+        <v>49</v>
       </c>
       <c r="K365">
-        <v>2.05</v>
+        <v>5.25</v>
       </c>
       <c r="L365">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M365">
-        <v>3.2</v>
+        <v>1.55</v>
       </c>
       <c r="N365">
-        <v>2.15</v>
+        <v>4.75</v>
       </c>
       <c r="O365">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="P365">
-        <v>3.1</v>
+        <v>1.666</v>
       </c>
       <c r="Q365">
-        <v>-0.25</v>
+        <v>0.75</v>
       </c>
       <c r="R365">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="S365">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="T365">
         <v>2.75</v>
       </c>
       <c r="U365">
+        <v>2.025</v>
+      </c>
+      <c r="V365">
+        <v>1.825</v>
+      </c>
+      <c r="W365">
+        <v>-1</v>
+      </c>
+      <c r="X365">
+        <v>-1</v>
+      </c>
+      <c r="Y365">
+        <v>0.6659999999999999</v>
+      </c>
+      <c r="Z365">
+        <v>-1</v>
+      </c>
+      <c r="AA365">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="AB365">
+        <v>1.025</v>
+      </c>
+      <c r="AC365">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="366" spans="1:29">
+      <c r="A366" s="1">
+        <v>364</v>
+      </c>
+      <c r="B366">
+        <v>6810182</v>
+      </c>
+      <c r="C366" t="s">
+        <v>28</v>
+      </c>
+      <c r="D366" t="s">
+        <v>28</v>
+      </c>
+      <c r="E366" s="2">
+        <v>45333.5</v>
+      </c>
+      <c r="F366" t="s">
+        <v>40</v>
+      </c>
+      <c r="G366" t="s">
+        <v>34</v>
+      </c>
+      <c r="H366">
+        <v>1</v>
+      </c>
+      <c r="I366">
+        <v>1</v>
+      </c>
+      <c r="J366" t="s">
+        <v>48</v>
+      </c>
+      <c r="K366">
+        <v>3.8</v>
+      </c>
+      <c r="L366">
+        <v>3.6</v>
+      </c>
+      <c r="M366">
+        <v>1.85</v>
+      </c>
+      <c r="N366">
+        <v>3.75</v>
+      </c>
+      <c r="O366">
+        <v>3.5</v>
+      </c>
+      <c r="P366">
+        <v>1.95</v>
+      </c>
+      <c r="Q366">
+        <v>0.5</v>
+      </c>
+      <c r="R366">
+        <v>1.9</v>
+      </c>
+      <c r="S366">
+        <v>1.95</v>
+      </c>
+      <c r="T366">
+        <v>2.5</v>
+      </c>
+      <c r="U366">
+        <v>1.825</v>
+      </c>
+      <c r="V366">
+        <v>2.025</v>
+      </c>
+      <c r="W366">
+        <v>-1</v>
+      </c>
+      <c r="X366">
+        <v>2.5</v>
+      </c>
+      <c r="Y366">
+        <v>-1</v>
+      </c>
+      <c r="Z366">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="AA366">
+        <v>-1</v>
+      </c>
+      <c r="AB366">
+        <v>-1</v>
+      </c>
+      <c r="AC366">
+        <v>1.025</v>
+      </c>
+    </row>
+    <row r="367" spans="1:29">
+      <c r="A367" s="1">
+        <v>365</v>
+      </c>
+      <c r="B367">
+        <v>6810180</v>
+      </c>
+      <c r="C367" t="s">
+        <v>28</v>
+      </c>
+      <c r="D367" t="s">
+        <v>28</v>
+      </c>
+      <c r="E367" s="2">
+        <v>45333.60416666666</v>
+      </c>
+      <c r="F367" t="s">
+        <v>44</v>
+      </c>
+      <c r="G367" t="s">
+        <v>36</v>
+      </c>
+      <c r="H367">
+        <v>1</v>
+      </c>
+      <c r="I367">
+        <v>3</v>
+      </c>
+      <c r="J367" t="s">
+        <v>49</v>
+      </c>
+      <c r="K367">
+        <v>3.6</v>
+      </c>
+      <c r="L367">
+        <v>3.4</v>
+      </c>
+      <c r="M367">
+        <v>2</v>
+      </c>
+      <c r="N367">
+        <v>3.6</v>
+      </c>
+      <c r="O367">
+        <v>3.4</v>
+      </c>
+      <c r="P367">
+        <v>2.05</v>
+      </c>
+      <c r="Q367">
+        <v>0.5</v>
+      </c>
+      <c r="R367">
+        <v>1.825</v>
+      </c>
+      <c r="S367">
+        <v>2.025</v>
+      </c>
+      <c r="T367">
+        <v>2.5</v>
+      </c>
+      <c r="U367">
+        <v>1.875</v>
+      </c>
+      <c r="V367">
         <v>1.975</v>
       </c>
-      <c r="V365">
+      <c r="W367">
+        <v>-1</v>
+      </c>
+      <c r="X367">
+        <v>-1</v>
+      </c>
+      <c r="Y367">
+        <v>1.05</v>
+      </c>
+      <c r="Z367">
+        <v>-1</v>
+      </c>
+      <c r="AA367">
+        <v>1.025</v>
+      </c>
+      <c r="AB367">
+        <v>0.875</v>
+      </c>
+      <c r="AC367">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="368" spans="1:29">
+      <c r="A368" s="1">
+        <v>366</v>
+      </c>
+      <c r="B368">
+        <v>6810181</v>
+      </c>
+      <c r="C368" t="s">
+        <v>28</v>
+      </c>
+      <c r="D368" t="s">
+        <v>28</v>
+      </c>
+      <c r="E368" s="2">
+        <v>45333.63541666666</v>
+      </c>
+      <c r="F368" t="s">
+        <v>42</v>
+      </c>
+      <c r="G368" t="s">
+        <v>31</v>
+      </c>
+      <c r="H368">
+        <v>1</v>
+      </c>
+      <c r="I368">
+        <v>2</v>
+      </c>
+      <c r="J368" t="s">
+        <v>49</v>
+      </c>
+      <c r="K368">
+        <v>2.05</v>
+      </c>
+      <c r="L368">
+        <v>3.6</v>
+      </c>
+      <c r="M368">
+        <v>3.2</v>
+      </c>
+      <c r="N368">
+        <v>2.45</v>
+      </c>
+      <c r="O368">
+        <v>3.6</v>
+      </c>
+      <c r="P368">
+        <v>2.7</v>
+      </c>
+      <c r="Q368">
+        <v>0</v>
+      </c>
+      <c r="R368">
+        <v>1.8</v>
+      </c>
+      <c r="S368">
+        <v>2.05</v>
+      </c>
+      <c r="T368">
+        <v>2.75</v>
+      </c>
+      <c r="U368">
+        <v>1.925</v>
+      </c>
+      <c r="V368">
+        <v>1.925</v>
+      </c>
+      <c r="W368">
+        <v>-1</v>
+      </c>
+      <c r="X368">
+        <v>-1</v>
+      </c>
+      <c r="Y368">
+        <v>1.7</v>
+      </c>
+      <c r="Z368">
+        <v>-1</v>
+      </c>
+      <c r="AA368">
+        <v>1.05</v>
+      </c>
+      <c r="AB368">
+        <v>0.4625</v>
+      </c>
+      <c r="AC368">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="369" spans="1:27">
+      <c r="A369" s="1">
+        <v>367</v>
+      </c>
+      <c r="B369">
+        <v>6810189</v>
+      </c>
+      <c r="C369" t="s">
+        <v>28</v>
+      </c>
+      <c r="D369" t="s">
+        <v>28</v>
+      </c>
+      <c r="E369" s="2">
+        <v>45338.69791666666</v>
+      </c>
+      <c r="F369" t="s">
+        <v>38</v>
+      </c>
+      <c r="G369" t="s">
+        <v>29</v>
+      </c>
+      <c r="K369">
+        <v>2.375</v>
+      </c>
+      <c r="L369">
+        <v>3.4</v>
+      </c>
+      <c r="M369">
+        <v>2.9</v>
+      </c>
+      <c r="N369">
+        <v>2.375</v>
+      </c>
+      <c r="O369">
+        <v>3.3</v>
+      </c>
+      <c r="P369">
+        <v>3</v>
+      </c>
+      <c r="Q369">
+        <v>-0.25</v>
+      </c>
+      <c r="R369">
+        <v>2.05</v>
+      </c>
+      <c r="S369">
+        <v>1.8</v>
+      </c>
+      <c r="T369">
+        <v>2.5</v>
+      </c>
+      <c r="U369">
+        <v>1.95</v>
+      </c>
+      <c r="V369">
+        <v>1.9</v>
+      </c>
+      <c r="W369">
+        <v>0</v>
+      </c>
+      <c r="X369">
+        <v>0</v>
+      </c>
+      <c r="Y369">
+        <v>0</v>
+      </c>
+      <c r="Z369">
+        <v>0</v>
+      </c>
+      <c r="AA369">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370" spans="1:27">
+      <c r="A370" s="1">
+        <v>368</v>
+      </c>
+      <c r="B370">
+        <v>6810193</v>
+      </c>
+      <c r="C370" t="s">
+        <v>28</v>
+      </c>
+      <c r="D370" t="s">
+        <v>28</v>
+      </c>
+      <c r="E370" s="2">
+        <v>45339.5</v>
+      </c>
+      <c r="F370" t="s">
+        <v>34</v>
+      </c>
+      <c r="G370" t="s">
+        <v>47</v>
+      </c>
+      <c r="K370">
+        <v>1.3</v>
+      </c>
+      <c r="L370">
+        <v>5.75</v>
+      </c>
+      <c r="M370">
+        <v>9</v>
+      </c>
+      <c r="N370">
+        <v>1.285</v>
+      </c>
+      <c r="O370">
+        <v>6</v>
+      </c>
+      <c r="P370">
+        <v>9.5</v>
+      </c>
+      <c r="Q370">
+        <v>-1.75</v>
+      </c>
+      <c r="R370">
+        <v>2.025</v>
+      </c>
+      <c r="S370">
+        <v>1.825</v>
+      </c>
+      <c r="T370">
+        <v>3</v>
+      </c>
+      <c r="U370">
+        <v>1.85</v>
+      </c>
+      <c r="V370">
+        <v>2</v>
+      </c>
+      <c r="W370">
+        <v>0</v>
+      </c>
+      <c r="X370">
+        <v>0</v>
+      </c>
+      <c r="Y370">
+        <v>0</v>
+      </c>
+      <c r="Z370">
+        <v>0</v>
+      </c>
+      <c r="AA370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:27">
+      <c r="A371" s="1">
+        <v>369</v>
+      </c>
+      <c r="B371">
+        <v>6810192</v>
+      </c>
+      <c r="C371" t="s">
+        <v>28</v>
+      </c>
+      <c r="D371" t="s">
+        <v>28</v>
+      </c>
+      <c r="E371" s="2">
+        <v>45339.59375</v>
+      </c>
+      <c r="F371" t="s">
+        <v>37</v>
+      </c>
+      <c r="G371" t="s">
+        <v>44</v>
+      </c>
+      <c r="K371">
+        <v>2.25</v>
+      </c>
+      <c r="L371">
+        <v>3.4</v>
+      </c>
+      <c r="M371">
+        <v>3.1</v>
+      </c>
+      <c r="N371">
+        <v>2.3</v>
+      </c>
+      <c r="O371">
+        <v>3.5</v>
+      </c>
+      <c r="P371">
+        <v>3</v>
+      </c>
+      <c r="Q371">
+        <v>-0.25</v>
+      </c>
+      <c r="R371">
+        <v>2.025</v>
+      </c>
+      <c r="S371">
+        <v>1.825</v>
+      </c>
+      <c r="T371">
+        <v>2.5</v>
+      </c>
+      <c r="U371">
         <v>1.875</v>
       </c>
-      <c r="W365">
+      <c r="V371">
+        <v>1.975</v>
+      </c>
+      <c r="W371">
         <v>0</v>
       </c>
-      <c r="X365">
+      <c r="X371">
         <v>0</v>
       </c>
-      <c r="Y365">
+      <c r="Y371">
         <v>0</v>
       </c>
-      <c r="Z365">
+      <c r="Z371">
         <v>0</v>
       </c>
-      <c r="AA365">
+      <c r="AA371">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="372" spans="1:27">
+      <c r="A372" s="1">
+        <v>370</v>
+      </c>
+      <c r="B372">
+        <v>6810188</v>
+      </c>
+      <c r="C372" t="s">
+        <v>28</v>
+      </c>
+      <c r="D372" t="s">
+        <v>28</v>
+      </c>
+      <c r="E372" s="2">
+        <v>45339.69791666666</v>
+      </c>
+      <c r="F372" t="s">
+        <v>33</v>
+      </c>
+      <c r="G372" t="s">
+        <v>40</v>
+      </c>
+      <c r="K372">
+        <v>1.533</v>
+      </c>
+      <c r="L372">
+        <v>4.2</v>
+      </c>
+      <c r="M372">
+        <v>6</v>
+      </c>
+      <c r="N372">
+        <v>1.571</v>
+      </c>
+      <c r="O372">
+        <v>4</v>
+      </c>
+      <c r="P372">
+        <v>5.75</v>
+      </c>
+      <c r="Q372">
+        <v>-1</v>
+      </c>
+      <c r="R372">
+        <v>2</v>
+      </c>
+      <c r="S372">
+        <v>1.85</v>
+      </c>
+      <c r="T372">
+        <v>2.75</v>
+      </c>
+      <c r="U372">
+        <v>2.025</v>
+      </c>
+      <c r="V372">
+        <v>1.825</v>
+      </c>
+      <c r="W372">
+        <v>0</v>
+      </c>
+      <c r="X372">
+        <v>0</v>
+      </c>
+      <c r="Y372">
+        <v>0</v>
+      </c>
+      <c r="Z372">
+        <v>0</v>
+      </c>
+      <c r="AA372">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="373" spans="1:27">
+      <c r="A373" s="1">
+        <v>371</v>
+      </c>
+      <c r="B373">
+        <v>6810194</v>
+      </c>
+      <c r="C373" t="s">
+        <v>28</v>
+      </c>
+      <c r="D373" t="s">
+        <v>28</v>
+      </c>
+      <c r="E373" s="2">
+        <v>45340.39583333334</v>
+      </c>
+      <c r="F373" t="s">
+        <v>31</v>
+      </c>
+      <c r="G373" t="s">
+        <v>41</v>
+      </c>
+      <c r="K373">
+        <v>3</v>
+      </c>
+      <c r="L373">
+        <v>3.6</v>
+      </c>
+      <c r="M373">
+        <v>2.25</v>
+      </c>
+      <c r="N373">
+        <v>3.4</v>
+      </c>
+      <c r="O373">
+        <v>3.75</v>
+      </c>
+      <c r="P373">
+        <v>2.05</v>
+      </c>
+      <c r="Q373">
+        <v>0.5</v>
+      </c>
+      <c r="R373">
+        <v>1.825</v>
+      </c>
+      <c r="S373">
+        <v>2.025</v>
+      </c>
+      <c r="T373">
+        <v>2.75</v>
+      </c>
+      <c r="U373">
+        <v>2</v>
+      </c>
+      <c r="V373">
+        <v>1.85</v>
+      </c>
+      <c r="W373">
+        <v>0</v>
+      </c>
+      <c r="X373">
+        <v>0</v>
+      </c>
+      <c r="Y373">
+        <v>0</v>
+      </c>
+      <c r="Z373">
+        <v>0</v>
+      </c>
+      <c r="AA373">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:27">
+      <c r="A374" s="1">
+        <v>372</v>
+      </c>
+      <c r="B374">
+        <v>6810190</v>
+      </c>
+      <c r="C374" t="s">
+        <v>28</v>
+      </c>
+      <c r="D374" t="s">
+        <v>28</v>
+      </c>
+      <c r="E374" s="2">
+        <v>45340.5</v>
+      </c>
+      <c r="F374" t="s">
+        <v>45</v>
+      </c>
+      <c r="G374" t="s">
+        <v>43</v>
+      </c>
+      <c r="K374">
+        <v>6</v>
+      </c>
+      <c r="L374">
+        <v>4.75</v>
+      </c>
+      <c r="M374">
+        <v>1.444</v>
+      </c>
+      <c r="N374">
+        <v>7.5</v>
+      </c>
+      <c r="O374">
+        <v>5.25</v>
+      </c>
+      <c r="P374">
+        <v>1.363</v>
+      </c>
+      <c r="Q374">
+        <v>1.5</v>
+      </c>
+      <c r="R374">
+        <v>1.825</v>
+      </c>
+      <c r="S374">
+        <v>2.025</v>
+      </c>
+      <c r="T374">
+        <v>3</v>
+      </c>
+      <c r="U374">
+        <v>1.95</v>
+      </c>
+      <c r="V374">
+        <v>1.9</v>
+      </c>
+      <c r="W374">
+        <v>0</v>
+      </c>
+      <c r="X374">
+        <v>0</v>
+      </c>
+      <c r="Y374">
+        <v>0</v>
+      </c>
+      <c r="Z374">
+        <v>0</v>
+      </c>
+      <c r="AA374">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="1:27">
+      <c r="A375" s="1">
+        <v>373</v>
+      </c>
+      <c r="B375">
+        <v>6810187</v>
+      </c>
+      <c r="C375" t="s">
+        <v>28</v>
+      </c>
+      <c r="D375" t="s">
+        <v>28</v>
+      </c>
+      <c r="E375" s="2">
+        <v>45340.60416666666</v>
+      </c>
+      <c r="F375" t="s">
+        <v>36</v>
+      </c>
+      <c r="G375" t="s">
+        <v>46</v>
+      </c>
+      <c r="K375">
+        <v>1.571</v>
+      </c>
+      <c r="L375">
+        <v>4</v>
+      </c>
+      <c r="M375">
+        <v>6</v>
+      </c>
+      <c r="N375">
+        <v>1.615</v>
+      </c>
+      <c r="O375">
+        <v>3.75</v>
+      </c>
+      <c r="P375">
+        <v>5.75</v>
+      </c>
+      <c r="Q375">
+        <v>-0.75</v>
+      </c>
+      <c r="R375">
+        <v>1.8</v>
+      </c>
+      <c r="S375">
+        <v>2.05</v>
+      </c>
+      <c r="T375">
+        <v>2.5</v>
+      </c>
+      <c r="U375">
+        <v>1.85</v>
+      </c>
+      <c r="V375">
+        <v>2</v>
+      </c>
+      <c r="W375">
+        <v>0</v>
+      </c>
+      <c r="X375">
+        <v>0</v>
+      </c>
+      <c r="Y375">
+        <v>0</v>
+      </c>
+      <c r="Z375">
+        <v>0</v>
+      </c>
+      <c r="AA375">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:27">
+      <c r="A376" s="1">
+        <v>374</v>
+      </c>
+      <c r="B376">
+        <v>6810191</v>
+      </c>
+      <c r="C376" t="s">
+        <v>28</v>
+      </c>
+      <c r="D376" t="s">
+        <v>28</v>
+      </c>
+      <c r="E376" s="2">
+        <v>45340.63541666666</v>
+      </c>
+      <c r="F376" t="s">
+        <v>30</v>
+      </c>
+      <c r="G376" t="s">
+        <v>42</v>
+      </c>
+      <c r="K376">
+        <v>5</v>
+      </c>
+      <c r="L376">
+        <v>4</v>
+      </c>
+      <c r="M376">
+        <v>1.65</v>
+      </c>
+      <c r="N376">
+        <v>5</v>
+      </c>
+      <c r="O376">
+        <v>4</v>
+      </c>
+      <c r="P376">
+        <v>1.666</v>
+      </c>
+      <c r="Q376">
+        <v>0.75</v>
+      </c>
+      <c r="R376">
+        <v>1.95</v>
+      </c>
+      <c r="S376">
+        <v>1.9</v>
+      </c>
+      <c r="T376">
+        <v>2.75</v>
+      </c>
+      <c r="U376">
+        <v>1.875</v>
+      </c>
+      <c r="V376">
+        <v>1.975</v>
+      </c>
+      <c r="W376">
+        <v>0</v>
+      </c>
+      <c r="X376">
+        <v>0</v>
+      </c>
+      <c r="Y376">
+        <v>0</v>
+      </c>
+      <c r="Z376">
+        <v>0</v>
+      </c>
+      <c r="AA376">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-02-16 às 20:23
</commit_message>
<xml_diff>
--- a/Belgium First Division A/Belgium First Division A.xlsx
+++ b/Belgium First Division A/Belgium First Division A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -1604,7 +1604,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>5208566</v>
+        <v>6114951</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
@@ -1616,76 +1616,76 @@
         <v>44940.59375</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K13">
-        <v>1.75</v>
+        <v>2.75</v>
       </c>
       <c r="L13">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="M13">
-        <v>4.2</v>
+        <v>2.45</v>
       </c>
       <c r="N13">
-        <v>1.666</v>
+        <v>2.8</v>
       </c>
       <c r="O13">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="P13">
-        <v>4.5</v>
+        <v>2.45</v>
       </c>
       <c r="Q13">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="S13">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="T13">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U13">
+        <v>2.025</v>
+      </c>
+      <c r="V13">
         <v>1.825</v>
       </c>
-      <c r="V13">
-        <v>2.025</v>
-      </c>
       <c r="W13">
-        <v>0.6659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X13">
         <v>-1</v>
       </c>
       <c r="Y13">
-        <v>-1</v>
+        <v>1.45</v>
       </c>
       <c r="Z13">
-        <v>0.4375</v>
+        <v>-1</v>
       </c>
       <c r="AA13">
-        <v>-0.5</v>
+        <v>0.8</v>
       </c>
       <c r="AB13">
-        <v>0.4125</v>
+        <v>-1</v>
       </c>
       <c r="AC13">
-        <v>-0.5</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="14" spans="1:29">
@@ -1693,7 +1693,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>6114951</v>
+        <v>5208566</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
@@ -1705,76 +1705,76 @@
         <v>44940.59375</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K14">
+        <v>1.75</v>
+      </c>
+      <c r="L14">
+        <v>3.8</v>
+      </c>
+      <c r="M14">
+        <v>4.2</v>
+      </c>
+      <c r="N14">
+        <v>1.666</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>4.5</v>
+      </c>
+      <c r="Q14">
+        <v>-0.75</v>
+      </c>
+      <c r="R14">
+        <v>1.875</v>
+      </c>
+      <c r="S14">
+        <v>1.975</v>
+      </c>
+      <c r="T14">
         <v>2.75</v>
       </c>
-      <c r="L14">
-        <v>3.4</v>
-      </c>
-      <c r="M14">
-        <v>2.45</v>
-      </c>
-      <c r="N14">
-        <v>2.8</v>
-      </c>
-      <c r="O14">
-        <v>3.3</v>
-      </c>
-      <c r="P14">
-        <v>2.45</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>2.05</v>
-      </c>
-      <c r="S14">
-        <v>1.8</v>
-      </c>
-      <c r="T14">
-        <v>2.5</v>
-      </c>
       <c r="U14">
+        <v>1.825</v>
+      </c>
+      <c r="V14">
         <v>2.025</v>
       </c>
-      <c r="V14">
-        <v>1.825</v>
-      </c>
       <c r="W14">
-        <v>-1</v>
+        <v>0.6659999999999999</v>
       </c>
       <c r="X14">
         <v>-1</v>
       </c>
       <c r="Y14">
-        <v>1.45</v>
+        <v>-1</v>
       </c>
       <c r="Z14">
-        <v>-1</v>
+        <v>0.4375</v>
       </c>
       <c r="AA14">
-        <v>0.8</v>
+        <v>-0.5</v>
       </c>
       <c r="AB14">
-        <v>-1</v>
+        <v>0.4125</v>
       </c>
       <c r="AC14">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="15" spans="1:29">
@@ -2494,7 +2494,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>5208701</v>
+        <v>5208571</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
@@ -2506,76 +2506,76 @@
         <v>44944.60416666666</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G23" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K23">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
       <c r="L23">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="M23">
-        <v>2.05</v>
+        <v>1.75</v>
       </c>
       <c r="N23">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="O23">
-        <v>3.3</v>
+        <v>3.8</v>
       </c>
       <c r="P23">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="Q23">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="R23">
-        <v>2.05</v>
+        <v>1.975</v>
       </c>
       <c r="S23">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="T23">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U23">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="V23">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="W23">
         <v>-1</v>
       </c>
       <c r="X23">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Y23">
-        <v>-1</v>
+        <v>0.7</v>
       </c>
       <c r="Z23">
-        <v>0.5249999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA23">
+        <v>0.875</v>
+      </c>
+      <c r="AB23">
+        <v>0.5</v>
+      </c>
+      <c r="AC23">
         <v>-0.5</v>
-      </c>
-      <c r="AB23">
-        <v>-1</v>
-      </c>
-      <c r="AC23">
-        <v>0.8</v>
       </c>
     </row>
     <row r="24" spans="1:29">
@@ -2583,7 +2583,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>5208571</v>
+        <v>5208701</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
@@ -2595,76 +2595,76 @@
         <v>44944.60416666666</v>
       </c>
       <c r="F24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G24" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K24">
-        <v>4.2</v>
+        <v>3.3</v>
       </c>
       <c r="L24">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="M24">
-        <v>1.75</v>
+        <v>2.05</v>
       </c>
       <c r="N24">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="O24">
-        <v>3.8</v>
+        <v>3.3</v>
       </c>
       <c r="P24">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="Q24">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="R24">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="S24">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="T24">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U24">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="V24">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="W24">
         <v>-1</v>
       </c>
       <c r="X24">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Y24">
-        <v>0.7</v>
+        <v>-1</v>
       </c>
       <c r="Z24">
-        <v>-1</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AA24">
-        <v>0.875</v>
+        <v>-0.5</v>
       </c>
       <c r="AB24">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="AC24">
-        <v>-0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="25" spans="1:29">
@@ -2672,7 +2672,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>5208568</v>
+        <v>5208569</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
@@ -2684,73 +2684,73 @@
         <v>44944.69791666666</v>
       </c>
       <c r="F25" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G25" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K25">
-        <v>1.4</v>
+        <v>1.85</v>
       </c>
       <c r="L25">
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="M25">
-        <v>6.5</v>
+        <v>3.8</v>
       </c>
       <c r="N25">
-        <v>1.7</v>
+        <v>1.666</v>
       </c>
       <c r="O25">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P25">
-        <v>4.333</v>
+        <v>4.75</v>
       </c>
       <c r="Q25">
         <v>-0.75</v>
       </c>
       <c r="R25">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="S25">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="T25">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U25">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="V25">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="W25">
-        <v>-1</v>
+        <v>0.6659999999999999</v>
       </c>
       <c r="X25">
         <v>-1</v>
       </c>
       <c r="Y25">
-        <v>3.333</v>
+        <v>-1</v>
       </c>
       <c r="Z25">
-        <v>-1</v>
+        <v>0.4375</v>
       </c>
       <c r="AA25">
-        <v>0.925</v>
+        <v>-0.5</v>
       </c>
       <c r="AB25">
-        <v>0.9750000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="AC25">
         <v>-1</v>
@@ -2761,7 +2761,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>5208569</v>
+        <v>5208568</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
@@ -2773,73 +2773,73 @@
         <v>44944.69791666666</v>
       </c>
       <c r="F26" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26">
         <v>3</v>
       </c>
-      <c r="I26">
-        <v>2</v>
-      </c>
       <c r="J26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K26">
-        <v>1.85</v>
+        <v>1.4</v>
       </c>
       <c r="L26">
-        <v>3.75</v>
+        <v>5</v>
       </c>
       <c r="M26">
-        <v>3.8</v>
+        <v>6.5</v>
       </c>
       <c r="N26">
-        <v>1.666</v>
+        <v>1.7</v>
       </c>
       <c r="O26">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P26">
-        <v>4.75</v>
+        <v>4.333</v>
       </c>
       <c r="Q26">
         <v>-0.75</v>
       </c>
       <c r="R26">
+        <v>1.925</v>
+      </c>
+      <c r="S26">
+        <v>1.925</v>
+      </c>
+      <c r="T26">
+        <v>2.75</v>
+      </c>
+      <c r="U26">
+        <v>1.975</v>
+      </c>
+      <c r="V26">
         <v>1.875</v>
       </c>
-      <c r="S26">
-        <v>1.975</v>
-      </c>
-      <c r="T26">
-        <v>2.5</v>
-      </c>
-      <c r="U26">
-        <v>1.95</v>
-      </c>
-      <c r="V26">
-        <v>1.9</v>
-      </c>
       <c r="W26">
-        <v>0.6659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X26">
         <v>-1</v>
       </c>
       <c r="Y26">
-        <v>-1</v>
+        <v>3.333</v>
       </c>
       <c r="Z26">
-        <v>0.4375</v>
+        <v>-1</v>
       </c>
       <c r="AA26">
-        <v>-0.5</v>
+        <v>0.925</v>
       </c>
       <c r="AB26">
-        <v>0.95</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC26">
         <v>-1</v>
@@ -3918,7 +3918,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>5208580</v>
+        <v>5208579</v>
       </c>
       <c r="C39" t="s">
         <v>28</v>
@@ -3930,34 +3930,34 @@
         <v>44954.59375</v>
       </c>
       <c r="F39" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G39" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="H39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J39" t="s">
         <v>48</v>
       </c>
       <c r="K39">
-        <v>2.05</v>
+        <v>2.15</v>
       </c>
       <c r="L39">
         <v>3.4</v>
       </c>
       <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="N39">
+        <v>2.2</v>
+      </c>
+      <c r="O39">
         <v>3.2</v>
-      </c>
-      <c r="N39">
-        <v>2.1</v>
-      </c>
-      <c r="O39">
-        <v>3.4</v>
       </c>
       <c r="P39">
         <v>3.1</v>
@@ -3966,25 +3966,25 @@
         <v>-0.25</v>
       </c>
       <c r="R39">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="S39">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="T39">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="U39">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="V39">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="W39">
         <v>-1</v>
       </c>
       <c r="X39">
-        <v>2.4</v>
+        <v>2.2</v>
       </c>
       <c r="Y39">
         <v>-1</v>
@@ -3993,13 +3993,13 @@
         <v>-0.5</v>
       </c>
       <c r="AA39">
-        <v>0.475</v>
+        <v>0.4375</v>
       </c>
       <c r="AB39">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
       <c r="AC39">
-        <v>-1</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="40" spans="1:29">
@@ -4007,7 +4007,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>5208579</v>
+        <v>5208580</v>
       </c>
       <c r="C40" t="s">
         <v>28</v>
@@ -4019,34 +4019,34 @@
         <v>44954.59375</v>
       </c>
       <c r="F40" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G40" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J40" t="s">
         <v>48</v>
       </c>
       <c r="K40">
-        <v>2.15</v>
+        <v>2.05</v>
       </c>
       <c r="L40">
         <v>3.4</v>
       </c>
       <c r="M40">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="N40">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="O40">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="P40">
         <v>3.1</v>
@@ -4055,25 +4055,25 @@
         <v>-0.25</v>
       </c>
       <c r="R40">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="S40">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="T40">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="U40">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="V40">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="W40">
         <v>-1</v>
       </c>
       <c r="X40">
-        <v>2.2</v>
+        <v>2.4</v>
       </c>
       <c r="Y40">
         <v>-1</v>
@@ -4082,13 +4082,13 @@
         <v>-0.5</v>
       </c>
       <c r="AA40">
-        <v>0.4375</v>
+        <v>0.475</v>
       </c>
       <c r="AB40">
-        <v>-0.5</v>
+        <v>0.825</v>
       </c>
       <c r="AC40">
-        <v>0.4375</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="41" spans="1:29">
@@ -9614,7 +9614,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>5208612</v>
+        <v>5208613</v>
       </c>
       <c r="C103" t="s">
         <v>28</v>
@@ -9626,76 +9626,76 @@
         <v>45003.59375</v>
       </c>
       <c r="F103" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G103" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H103">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I103">
+        <v>2</v>
+      </c>
+      <c r="J103" t="s">
+        <v>49</v>
+      </c>
+      <c r="K103">
+        <v>3.3</v>
+      </c>
+      <c r="L103">
+        <v>3.3</v>
+      </c>
+      <c r="M103">
+        <v>2.05</v>
+      </c>
+      <c r="N103">
+        <v>2.8</v>
+      </c>
+      <c r="O103">
+        <v>3.3</v>
+      </c>
+      <c r="P103">
+        <v>2.3</v>
+      </c>
+      <c r="Q103">
+        <v>0.25</v>
+      </c>
+      <c r="R103">
+        <v>1.85</v>
+      </c>
+      <c r="S103">
+        <v>2</v>
+      </c>
+      <c r="T103">
+        <v>2.75</v>
+      </c>
+      <c r="U103">
+        <v>1.9</v>
+      </c>
+      <c r="V103">
+        <v>1.95</v>
+      </c>
+      <c r="W103">
+        <v>-1</v>
+      </c>
+      <c r="X103">
+        <v>-1</v>
+      </c>
+      <c r="Y103">
+        <v>1.3</v>
+      </c>
+      <c r="Z103">
+        <v>-1</v>
+      </c>
+      <c r="AA103">
         <v>1</v>
       </c>
-      <c r="J103" t="s">
-        <v>50</v>
-      </c>
-      <c r="K103">
-        <v>1.45</v>
-      </c>
-      <c r="L103">
-        <v>4</v>
-      </c>
-      <c r="M103">
-        <v>6</v>
-      </c>
-      <c r="N103">
-        <v>1.5</v>
-      </c>
-      <c r="O103">
-        <v>3.75</v>
-      </c>
-      <c r="P103">
-        <v>6.5</v>
-      </c>
-      <c r="Q103">
-        <v>-1</v>
-      </c>
-      <c r="R103">
-        <v>2</v>
-      </c>
-      <c r="S103">
-        <v>1.85</v>
-      </c>
-      <c r="T103">
-        <v>2.25</v>
-      </c>
-      <c r="U103">
-        <v>2.025</v>
-      </c>
-      <c r="V103">
-        <v>1.825</v>
-      </c>
-      <c r="W103">
-        <v>0.5</v>
-      </c>
-      <c r="X103">
-        <v>-1</v>
-      </c>
-      <c r="Y103">
-        <v>-1</v>
-      </c>
-      <c r="Z103">
-        <v>0</v>
-      </c>
-      <c r="AA103">
-        <v>-0</v>
-      </c>
       <c r="AB103">
-        <v>1.025</v>
+        <v>0.45</v>
       </c>
       <c r="AC103">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="104" spans="1:29">
@@ -9703,7 +9703,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>5208613</v>
+        <v>5208612</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9715,76 +9715,76 @@
         <v>45003.59375</v>
       </c>
       <c r="F104" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="G104" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H104">
+        <v>2</v>
+      </c>
+      <c r="I104">
         <v>1</v>
       </c>
-      <c r="I104">
-        <v>2</v>
-      </c>
       <c r="J104" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K104">
-        <v>3.3</v>
+        <v>1.45</v>
       </c>
       <c r="L104">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="M104">
-        <v>2.05</v>
+        <v>6</v>
       </c>
       <c r="N104">
-        <v>2.8</v>
+        <v>1.5</v>
       </c>
       <c r="O104">
-        <v>3.3</v>
+        <v>3.75</v>
       </c>
       <c r="P104">
-        <v>2.3</v>
+        <v>6.5</v>
       </c>
       <c r="Q104">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="R104">
+        <v>2</v>
+      </c>
+      <c r="S104">
         <v>1.85</v>
       </c>
-      <c r="S104">
-        <v>2</v>
-      </c>
       <c r="T104">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="U104">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="V104">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="W104">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA104">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="AB104">
-        <v>0.45</v>
+        <v>1.025</v>
       </c>
       <c r="AC104">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -11127,7 +11127,7 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>5391100</v>
+        <v>5394553</v>
       </c>
       <c r="C120" t="s">
         <v>28</v>
@@ -11139,76 +11139,76 @@
         <v>45024.45833333334</v>
       </c>
       <c r="F120" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G120" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H120">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J120" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K120">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="L120">
         <v>3.5</v>
       </c>
       <c r="M120">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="N120">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="O120">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="P120">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="Q120">
+        <v>-0.25</v>
+      </c>
+      <c r="R120">
+        <v>1.95</v>
+      </c>
+      <c r="S120">
+        <v>1.9</v>
+      </c>
+      <c r="T120">
+        <v>2.75</v>
+      </c>
+      <c r="U120">
+        <v>1.875</v>
+      </c>
+      <c r="V120">
+        <v>1.975</v>
+      </c>
+      <c r="W120">
+        <v>-1</v>
+      </c>
+      <c r="X120">
+        <v>2.4</v>
+      </c>
+      <c r="Y120">
+        <v>-1</v>
+      </c>
+      <c r="Z120">
         <v>-0.5</v>
       </c>
-      <c r="R120">
-        <v>2.025</v>
-      </c>
-      <c r="S120">
-        <v>1.825</v>
-      </c>
-      <c r="T120">
-        <v>3</v>
-      </c>
-      <c r="U120">
-        <v>1.95</v>
-      </c>
-      <c r="V120">
-        <v>1.9</v>
-      </c>
-      <c r="W120">
-        <v>1</v>
-      </c>
-      <c r="X120">
-        <v>-1</v>
-      </c>
-      <c r="Y120">
-        <v>-1</v>
-      </c>
-      <c r="Z120">
-        <v>1.025</v>
-      </c>
       <c r="AA120">
-        <v>-1</v>
+        <v>0.45</v>
       </c>
       <c r="AB120">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC120">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="121" spans="1:29">
@@ -11216,7 +11216,7 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>5394553</v>
+        <v>5391100</v>
       </c>
       <c r="C121" t="s">
         <v>28</v>
@@ -11228,76 +11228,76 @@
         <v>45024.45833333334</v>
       </c>
       <c r="F121" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G121" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H121">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J121" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K121">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="L121">
         <v>3.5</v>
       </c>
       <c r="M121">
+        <v>3.3</v>
+      </c>
+      <c r="N121">
+        <v>2</v>
+      </c>
+      <c r="O121">
         <v>3.6</v>
       </c>
-      <c r="N121">
-        <v>2.25</v>
-      </c>
-      <c r="O121">
-        <v>3.4</v>
-      </c>
       <c r="P121">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="Q121">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R121">
+        <v>2.025</v>
+      </c>
+      <c r="S121">
+        <v>1.825</v>
+      </c>
+      <c r="T121">
+        <v>3</v>
+      </c>
+      <c r="U121">
         <v>1.95</v>
       </c>
-      <c r="S121">
+      <c r="V121">
         <v>1.9</v>
       </c>
-      <c r="T121">
-        <v>2.75</v>
-      </c>
-      <c r="U121">
-        <v>1.875</v>
-      </c>
-      <c r="V121">
-        <v>1.975</v>
-      </c>
       <c r="W121">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X121">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Y121">
         <v>-1</v>
       </c>
       <c r="Z121">
-        <v>-0.5</v>
+        <v>1.025</v>
       </c>
       <c r="AA121">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
       <c r="AB121">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AC121">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="122" spans="1:29">
@@ -12017,7 +12017,7 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>5424405</v>
+        <v>5424406</v>
       </c>
       <c r="C130" t="s">
         <v>28</v>
@@ -12029,73 +12029,73 @@
         <v>45031.55208333334</v>
       </c>
       <c r="F130" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G130" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H130">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I130">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J130" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K130">
-        <v>1.75</v>
+        <v>2.4</v>
       </c>
       <c r="L130">
         <v>3.5</v>
       </c>
       <c r="M130">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N130">
-        <v>1.65</v>
+        <v>2.4</v>
       </c>
       <c r="O130">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="P130">
-        <v>5.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q130">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="R130">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="S130">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="T130">
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="U130">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="V130">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="W130">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X130">
         <v>-1</v>
       </c>
       <c r="Y130">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z130">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA130">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB130">
-        <v>1</v>
+        <v>1.025</v>
       </c>
       <c r="AC130">
         <v>-1</v>
@@ -12106,7 +12106,7 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>5424406</v>
+        <v>5424405</v>
       </c>
       <c r="C131" t="s">
         <v>28</v>
@@ -12118,73 +12118,73 @@
         <v>45031.55208333334</v>
       </c>
       <c r="F131" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G131" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="H131">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I131">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J131" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K131">
-        <v>2.4</v>
+        <v>1.75</v>
       </c>
       <c r="L131">
         <v>3.5</v>
       </c>
       <c r="M131">
-        <v>2.75</v>
+        <v>5</v>
       </c>
       <c r="N131">
-        <v>2.4</v>
+        <v>1.65</v>
       </c>
       <c r="O131">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="P131">
-        <v>2.75</v>
+        <v>5.25</v>
       </c>
       <c r="Q131">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="R131">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="S131">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="T131">
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
       <c r="U131">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="V131">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="W131">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="X131">
         <v>-1</v>
       </c>
       <c r="Y131">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z131">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA131">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB131">
-        <v>1.025</v>
+        <v>1</v>
       </c>
       <c r="AC131">
         <v>-1</v>
@@ -12818,7 +12818,7 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>6390442</v>
+        <v>6390066</v>
       </c>
       <c r="C139" t="s">
         <v>28</v>
@@ -12830,73 +12830,73 @@
         <v>45039.5625</v>
       </c>
       <c r="F139" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G139" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H139">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I139">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J139" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K139">
-        <v>1.333</v>
+        <v>3</v>
       </c>
       <c r="L139">
-        <v>5</v>
+        <v>3.6</v>
       </c>
       <c r="M139">
-        <v>8</v>
+        <v>2.15</v>
       </c>
       <c r="N139">
-        <v>1.3</v>
+        <v>2.8</v>
       </c>
       <c r="O139">
-        <v>5.25</v>
+        <v>3.6</v>
       </c>
       <c r="P139">
-        <v>8.5</v>
+        <v>2.25</v>
       </c>
       <c r="Q139">
-        <v>-1.75</v>
+        <v>0.25</v>
       </c>
       <c r="R139">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="S139">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="T139">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="U139">
-        <v>2.025</v>
+        <v>1.8</v>
       </c>
       <c r="V139">
-        <v>1.825</v>
+        <v>2.05</v>
       </c>
       <c r="W139">
-        <v>0.3</v>
+        <v>-1</v>
       </c>
       <c r="X139">
         <v>-1</v>
       </c>
       <c r="Y139">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="Z139">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA139">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AB139">
-        <v>1.025</v>
+        <v>0.8</v>
       </c>
       <c r="AC139">
         <v>-1</v>
@@ -12907,7 +12907,7 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>6390066</v>
+        <v>6390442</v>
       </c>
       <c r="C140" t="s">
         <v>28</v>
@@ -12919,73 +12919,73 @@
         <v>45039.5625</v>
       </c>
       <c r="F140" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G140" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H140">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I140">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J140" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K140">
-        <v>3</v>
+        <v>1.333</v>
       </c>
       <c r="L140">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="M140">
-        <v>2.15</v>
+        <v>8</v>
       </c>
       <c r="N140">
-        <v>2.8</v>
+        <v>1.3</v>
       </c>
       <c r="O140">
-        <v>3.6</v>
+        <v>5.25</v>
       </c>
       <c r="P140">
-        <v>2.25</v>
+        <v>8.5</v>
       </c>
       <c r="Q140">
-        <v>0.25</v>
+        <v>-1.75</v>
       </c>
       <c r="R140">
+        <v>1.975</v>
+      </c>
+      <c r="S140">
+        <v>1.875</v>
+      </c>
+      <c r="T140">
+        <v>3.75</v>
+      </c>
+      <c r="U140">
+        <v>2.025</v>
+      </c>
+      <c r="V140">
         <v>1.825</v>
       </c>
-      <c r="S140">
-        <v>2.025</v>
-      </c>
-      <c r="T140">
-        <v>3</v>
-      </c>
-      <c r="U140">
-        <v>1.8</v>
-      </c>
-      <c r="V140">
-        <v>2.05</v>
-      </c>
       <c r="W140">
-        <v>-1</v>
+        <v>0.3</v>
       </c>
       <c r="X140">
         <v>-1</v>
       </c>
       <c r="Y140">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="Z140">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA140">
+        <v>-1</v>
+      </c>
+      <c r="AB140">
         <v>1.025</v>
-      </c>
-      <c r="AB140">
-        <v>0.8</v>
       </c>
       <c r="AC140">
         <v>-1</v>
@@ -12996,7 +12996,7 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>6390043</v>
+        <v>6390693</v>
       </c>
       <c r="C141" t="s">
         <v>28</v>
@@ -13008,76 +13008,76 @@
         <v>45039.5625</v>
       </c>
       <c r="F141" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G141" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H141">
+        <v>3</v>
+      </c>
+      <c r="I141">
+        <v>2</v>
+      </c>
+      <c r="J141" t="s">
+        <v>50</v>
+      </c>
+      <c r="K141">
+        <v>2.5</v>
+      </c>
+      <c r="L141">
+        <v>3.6</v>
+      </c>
+      <c r="M141">
+        <v>2.45</v>
+      </c>
+      <c r="N141">
+        <v>2.4</v>
+      </c>
+      <c r="O141">
+        <v>3.8</v>
+      </c>
+      <c r="P141">
+        <v>2.45</v>
+      </c>
+      <c r="Q141">
+        <v>0</v>
+      </c>
+      <c r="R141">
+        <v>1.9</v>
+      </c>
+      <c r="S141">
+        <v>1.95</v>
+      </c>
+      <c r="T141">
+        <v>3.25</v>
+      </c>
+      <c r="U141">
+        <v>2</v>
+      </c>
+      <c r="V141">
+        <v>1.85</v>
+      </c>
+      <c r="W141">
+        <v>1.4</v>
+      </c>
+      <c r="X141">
+        <v>-1</v>
+      </c>
+      <c r="Y141">
+        <v>-1</v>
+      </c>
+      <c r="Z141">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="AA141">
+        <v>-1</v>
+      </c>
+      <c r="AB141">
         <v>1</v>
       </c>
-      <c r="I141">
-        <v>2</v>
-      </c>
-      <c r="J141" t="s">
-        <v>49</v>
-      </c>
-      <c r="K141">
-        <v>1.222</v>
-      </c>
-      <c r="L141">
-        <v>5.75</v>
-      </c>
-      <c r="M141">
-        <v>11</v>
-      </c>
-      <c r="N141">
-        <v>1.142</v>
-      </c>
-      <c r="O141">
-        <v>7.5</v>
-      </c>
-      <c r="P141">
-        <v>15</v>
-      </c>
-      <c r="Q141">
-        <v>-2.25</v>
-      </c>
-      <c r="R141">
-        <v>1.975</v>
-      </c>
-      <c r="S141">
-        <v>1.875</v>
-      </c>
-      <c r="T141">
-        <v>3.5</v>
-      </c>
-      <c r="U141">
-        <v>1.95</v>
-      </c>
-      <c r="V141">
-        <v>1.9</v>
-      </c>
-      <c r="W141">
-        <v>-1</v>
-      </c>
-      <c r="X141">
-        <v>-1</v>
-      </c>
-      <c r="Y141">
-        <v>14</v>
-      </c>
-      <c r="Z141">
-        <v>-1</v>
-      </c>
-      <c r="AA141">
-        <v>0.875</v>
-      </c>
-      <c r="AB141">
-        <v>-1</v>
-      </c>
       <c r="AC141">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="142" spans="1:29">
@@ -13085,7 +13085,7 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>6389865</v>
+        <v>6390043</v>
       </c>
       <c r="C142" t="s">
         <v>28</v>
@@ -13097,49 +13097,49 @@
         <v>45039.5625</v>
       </c>
       <c r="F142" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G142" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H142">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I142">
         <v>2</v>
       </c>
       <c r="J142" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K142">
+        <v>1.222</v>
+      </c>
+      <c r="L142">
+        <v>5.75</v>
+      </c>
+      <c r="M142">
+        <v>11</v>
+      </c>
+      <c r="N142">
+        <v>1.142</v>
+      </c>
+      <c r="O142">
+        <v>7.5</v>
+      </c>
+      <c r="P142">
+        <v>15</v>
+      </c>
+      <c r="Q142">
+        <v>-2.25</v>
+      </c>
+      <c r="R142">
+        <v>1.975</v>
+      </c>
+      <c r="S142">
+        <v>1.875</v>
+      </c>
+      <c r="T142">
         <v>3.5</v>
-      </c>
-      <c r="L142">
-        <v>3.6</v>
-      </c>
-      <c r="M142">
-        <v>1.95</v>
-      </c>
-      <c r="N142">
-        <v>2.8</v>
-      </c>
-      <c r="O142">
-        <v>3.5</v>
-      </c>
-      <c r="P142">
-        <v>2.3</v>
-      </c>
-      <c r="Q142">
-        <v>0.25</v>
-      </c>
-      <c r="R142">
-        <v>1.8</v>
-      </c>
-      <c r="S142">
-        <v>2.05</v>
-      </c>
-      <c r="T142">
-        <v>3</v>
       </c>
       <c r="U142">
         <v>1.95</v>
@@ -13151,22 +13151,22 @@
         <v>-1</v>
       </c>
       <c r="X142">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y142">
-        <v>-1</v>
+        <v>14</v>
       </c>
       <c r="Z142">
-        <v>0.4</v>
+        <v>-1</v>
       </c>
       <c r="AA142">
-        <v>-0.5</v>
+        <v>0.875</v>
       </c>
       <c r="AB142">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC142">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="143" spans="1:29">
@@ -13174,7 +13174,7 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>6385540</v>
+        <v>6389819</v>
       </c>
       <c r="C143" t="s">
         <v>28</v>
@@ -13186,55 +13186,55 @@
         <v>45039.5625</v>
       </c>
       <c r="F143" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G143" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H143">
         <v>2</v>
       </c>
       <c r="I143">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J143" t="s">
         <v>49</v>
       </c>
       <c r="K143">
-        <v>1.363</v>
+        <v>5.25</v>
       </c>
       <c r="L143">
-        <v>5</v>
+        <v>4.2</v>
       </c>
       <c r="M143">
-        <v>7</v>
+        <v>1.533</v>
       </c>
       <c r="N143">
-        <v>1.55</v>
+        <v>6.5</v>
       </c>
       <c r="O143">
-        <v>4.2</v>
+        <v>4.75</v>
       </c>
       <c r="P143">
-        <v>5</v>
+        <v>1.4</v>
       </c>
       <c r="Q143">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="R143">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="S143">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="T143">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U143">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="V143">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="W143">
         <v>-1</v>
@@ -13243,16 +13243,16 @@
         <v>-1</v>
       </c>
       <c r="Y143">
-        <v>4</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="Z143">
         <v>-1</v>
       </c>
       <c r="AA143">
-        <v>0.925</v>
+        <v>0.95</v>
       </c>
       <c r="AB143">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="AC143">
         <v>-1</v>
@@ -13263,7 +13263,7 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>6390693</v>
+        <v>6389865</v>
       </c>
       <c r="C144" t="s">
         <v>28</v>
@@ -13275,73 +13275,73 @@
         <v>45039.5625</v>
       </c>
       <c r="F144" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G144" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H144">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I144">
         <v>2</v>
       </c>
       <c r="J144" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K144">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="L144">
         <v>3.6</v>
       </c>
       <c r="M144">
-        <v>2.45</v>
+        <v>1.95</v>
       </c>
       <c r="N144">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="O144">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="P144">
-        <v>2.45</v>
+        <v>2.3</v>
       </c>
       <c r="Q144">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R144">
+        <v>1.8</v>
+      </c>
+      <c r="S144">
+        <v>2.05</v>
+      </c>
+      <c r="T144">
+        <v>3</v>
+      </c>
+      <c r="U144">
+        <v>1.95</v>
+      </c>
+      <c r="V144">
         <v>1.9</v>
       </c>
-      <c r="S144">
-        <v>1.95</v>
-      </c>
-      <c r="T144">
-        <v>3.25</v>
-      </c>
-      <c r="U144">
-        <v>2</v>
-      </c>
-      <c r="V144">
-        <v>1.85</v>
-      </c>
       <c r="W144">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X144">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y144">
         <v>-1</v>
       </c>
       <c r="Z144">
-        <v>0.8999999999999999</v>
+        <v>0.4</v>
       </c>
       <c r="AA144">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB144">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="AC144">
         <v>-1</v>
@@ -13352,7 +13352,7 @@
         <v>143</v>
       </c>
       <c r="B145">
-        <v>6389819</v>
+        <v>6385540</v>
       </c>
       <c r="C145" t="s">
         <v>28</v>
@@ -13364,55 +13364,55 @@
         <v>45039.5625</v>
       </c>
       <c r="F145" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G145" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H145">
         <v>2</v>
       </c>
       <c r="I145">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J145" t="s">
         <v>49</v>
       </c>
       <c r="K145">
-        <v>5.25</v>
+        <v>1.363</v>
       </c>
       <c r="L145">
+        <v>5</v>
+      </c>
+      <c r="M145">
+        <v>7</v>
+      </c>
+      <c r="N145">
+        <v>1.55</v>
+      </c>
+      <c r="O145">
         <v>4.2</v>
       </c>
-      <c r="M145">
-        <v>1.533</v>
-      </c>
-      <c r="N145">
-        <v>6.5</v>
-      </c>
-      <c r="O145">
-        <v>4.75</v>
-      </c>
       <c r="P145">
-        <v>1.4</v>
+        <v>5</v>
       </c>
       <c r="Q145">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="R145">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="S145">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="T145">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U145">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="V145">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="W145">
         <v>-1</v>
@@ -13421,16 +13421,16 @@
         <v>-1</v>
       </c>
       <c r="Y145">
-        <v>0.3999999999999999</v>
+        <v>4</v>
       </c>
       <c r="Z145">
         <v>-1</v>
       </c>
       <c r="AA145">
-        <v>0.95</v>
+        <v>0.925</v>
       </c>
       <c r="AB145">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="AC145">
         <v>-1</v>
@@ -17357,7 +17357,7 @@
         <v>188</v>
       </c>
       <c r="B190">
-        <v>7030334</v>
+        <v>6810007</v>
       </c>
       <c r="C190" t="s">
         <v>28</v>
@@ -17369,55 +17369,55 @@
         <v>45151.45833333334</v>
       </c>
       <c r="F190" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G190" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H190">
         <v>0</v>
       </c>
       <c r="I190">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J190" t="s">
         <v>49</v>
       </c>
       <c r="K190">
-        <v>2.75</v>
+        <v>4.75</v>
       </c>
       <c r="L190">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="M190">
-        <v>2.25</v>
+        <v>1.571</v>
       </c>
       <c r="N190">
-        <v>2.4</v>
+        <v>7</v>
       </c>
       <c r="O190">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="P190">
-        <v>2.55</v>
+        <v>1.333</v>
       </c>
       <c r="Q190">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="R190">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="S190">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="T190">
         <v>3</v>
       </c>
       <c r="U190">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V190">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W190">
         <v>-1</v>
@@ -17426,19 +17426,19 @@
         <v>-1</v>
       </c>
       <c r="Y190">
-        <v>1.55</v>
+        <v>0.333</v>
       </c>
       <c r="Z190">
         <v>-1</v>
       </c>
       <c r="AA190">
-        <v>1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB190">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AC190">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="191" spans="1:29">
@@ -17446,7 +17446,7 @@
         <v>189</v>
       </c>
       <c r="B191">
-        <v>6810007</v>
+        <v>7030334</v>
       </c>
       <c r="C191" t="s">
         <v>28</v>
@@ -17458,55 +17458,55 @@
         <v>45151.45833333334</v>
       </c>
       <c r="F191" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G191" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H191">
         <v>0</v>
       </c>
       <c r="I191">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J191" t="s">
         <v>49</v>
       </c>
       <c r="K191">
-        <v>4.75</v>
+        <v>2.75</v>
       </c>
       <c r="L191">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="M191">
-        <v>1.571</v>
+        <v>2.25</v>
       </c>
       <c r="N191">
-        <v>7</v>
+        <v>2.4</v>
       </c>
       <c r="O191">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="P191">
-        <v>1.333</v>
+        <v>2.55</v>
       </c>
       <c r="Q191">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="R191">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="S191">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="T191">
         <v>3</v>
       </c>
       <c r="U191">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V191">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W191">
         <v>-1</v>
@@ -17515,19 +17515,19 @@
         <v>-1</v>
       </c>
       <c r="Y191">
-        <v>0.333</v>
+        <v>1.55</v>
       </c>
       <c r="Z191">
         <v>-1</v>
       </c>
       <c r="AA191">
-        <v>0.9750000000000001</v>
+        <v>1</v>
       </c>
       <c r="AB191">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC191">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="192" spans="1:29">
@@ -28838,7 +28838,7 @@
         <v>317</v>
       </c>
       <c r="B319">
-        <v>6810130</v>
+        <v>6810132</v>
       </c>
       <c r="C319" t="s">
         <v>28</v>
@@ -28850,76 +28850,76 @@
         <v>45283.59375</v>
       </c>
       <c r="F319" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="G319" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="H319">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I319">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J319" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K319">
-        <v>1.363</v>
+        <v>2.2</v>
       </c>
       <c r="L319">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="M319">
-        <v>7.5</v>
+        <v>3.2</v>
       </c>
       <c r="N319">
-        <v>1.333</v>
+        <v>2.3</v>
       </c>
       <c r="O319">
-        <v>5.25</v>
+        <v>3.3</v>
       </c>
       <c r="P319">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="Q319">
-        <v>-1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R319">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="S319">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="T319">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="U319">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="V319">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="W319">
-        <v>-1</v>
+        <v>1.3</v>
       </c>
       <c r="X319">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y319">
         <v>-1</v>
       </c>
       <c r="Z319">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AA319">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB319">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AC319">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="320" spans="1:29">
@@ -28927,7 +28927,7 @@
         <v>318</v>
       </c>
       <c r="B320">
-        <v>6810132</v>
+        <v>6810130</v>
       </c>
       <c r="C320" t="s">
         <v>28</v>
@@ -28939,76 +28939,76 @@
         <v>45283.59375</v>
       </c>
       <c r="F320" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="G320" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H320">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I320">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J320" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K320">
-        <v>2.2</v>
+        <v>1.363</v>
       </c>
       <c r="L320">
-        <v>3.4</v>
+        <v>5</v>
       </c>
       <c r="M320">
-        <v>3.2</v>
+        <v>7.5</v>
       </c>
       <c r="N320">
-        <v>2.3</v>
+        <v>1.333</v>
       </c>
       <c r="O320">
-        <v>3.3</v>
+        <v>5.25</v>
       </c>
       <c r="P320">
+        <v>8</v>
+      </c>
+      <c r="Q320">
+        <v>-1.5</v>
+      </c>
+      <c r="R320">
+        <v>1.9</v>
+      </c>
+      <c r="S320">
+        <v>1.95</v>
+      </c>
+      <c r="T320">
         <v>3</v>
       </c>
-      <c r="Q320">
-        <v>-0.25</v>
-      </c>
-      <c r="R320">
-        <v>2</v>
-      </c>
-      <c r="S320">
-        <v>1.85</v>
-      </c>
-      <c r="T320">
-        <v>2.25</v>
-      </c>
       <c r="U320">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="V320">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="W320">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="X320">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y320">
         <v>-1</v>
       </c>
       <c r="Z320">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AA320">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB320">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AC320">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="321" spans="1:29">
@@ -29194,7 +29194,7 @@
         <v>321</v>
       </c>
       <c r="B323">
-        <v>6810142</v>
+        <v>6810145</v>
       </c>
       <c r="C323" t="s">
         <v>28</v>
@@ -29206,76 +29206,76 @@
         <v>45286.5</v>
       </c>
       <c r="F323" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G323" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="H323">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I323">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J323" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K323">
-        <v>1.75</v>
+        <v>7</v>
       </c>
       <c r="L323">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M323">
-        <v>4</v>
+        <v>1.4</v>
       </c>
       <c r="N323">
+        <v>8.5</v>
+      </c>
+      <c r="O323">
+        <v>5.75</v>
+      </c>
+      <c r="P323">
+        <v>1.285</v>
+      </c>
+      <c r="Q323">
+        <v>1.5</v>
+      </c>
+      <c r="R323">
+        <v>2.025</v>
+      </c>
+      <c r="S323">
+        <v>1.825</v>
+      </c>
+      <c r="T323">
+        <v>3.25</v>
+      </c>
+      <c r="U323">
+        <v>2.05</v>
+      </c>
+      <c r="V323">
         <v>1.8</v>
       </c>
-      <c r="O323">
-        <v>3.8</v>
-      </c>
-      <c r="P323">
-        <v>3.8</v>
-      </c>
-      <c r="Q323">
-        <v>-0.5</v>
-      </c>
-      <c r="R323">
-        <v>1.825</v>
-      </c>
-      <c r="S323">
-        <v>2.025</v>
-      </c>
-      <c r="T323">
-        <v>3</v>
-      </c>
-      <c r="U323">
-        <v>1.975</v>
-      </c>
-      <c r="V323">
-        <v>1.875</v>
-      </c>
       <c r="W323">
+        <v>-1</v>
+      </c>
+      <c r="X323">
+        <v>-1</v>
+      </c>
+      <c r="Y323">
+        <v>0.2849999999999999</v>
+      </c>
+      <c r="Z323">
+        <v>-1</v>
+      </c>
+      <c r="AA323">
+        <v>0.825</v>
+      </c>
+      <c r="AB323">
+        <v>-1</v>
+      </c>
+      <c r="AC323">
         <v>0.8</v>
-      </c>
-      <c r="X323">
-        <v>-1</v>
-      </c>
-      <c r="Y323">
-        <v>-1</v>
-      </c>
-      <c r="Z323">
-        <v>0.825</v>
-      </c>
-      <c r="AA323">
-        <v>-1</v>
-      </c>
-      <c r="AB323">
-        <v>0</v>
-      </c>
-      <c r="AC323">
-        <v>-0</v>
       </c>
     </row>
     <row r="324" spans="1:29">
@@ -29283,7 +29283,7 @@
         <v>322</v>
       </c>
       <c r="B324">
-        <v>6810145</v>
+        <v>6810142</v>
       </c>
       <c r="C324" t="s">
         <v>28</v>
@@ -29295,76 +29295,76 @@
         <v>45286.5</v>
       </c>
       <c r="F324" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G324" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="H324">
+        <v>3</v>
+      </c>
+      <c r="I324">
         <v>0</v>
       </c>
-      <c r="I324">
-        <v>2</v>
-      </c>
       <c r="J324" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K324">
-        <v>7</v>
+        <v>1.75</v>
       </c>
       <c r="L324">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M324">
-        <v>1.4</v>
+        <v>4</v>
       </c>
       <c r="N324">
-        <v>8.5</v>
+        <v>1.8</v>
       </c>
       <c r="O324">
-        <v>5.75</v>
+        <v>3.8</v>
       </c>
       <c r="P324">
-        <v>1.285</v>
+        <v>3.8</v>
       </c>
       <c r="Q324">
-        <v>1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="R324">
+        <v>1.825</v>
+      </c>
+      <c r="S324">
         <v>2.025</v>
       </c>
-      <c r="S324">
-        <v>1.825</v>
-      </c>
       <c r="T324">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U324">
-        <v>2.05</v>
+        <v>1.975</v>
       </c>
       <c r="V324">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="W324">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="X324">
         <v>-1</v>
       </c>
       <c r="Y324">
-        <v>0.2849999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z324">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AA324">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB324">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC324">
-        <v>0.8</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="325" spans="1:29">
@@ -30618,7 +30618,7 @@
         <v>337</v>
       </c>
       <c r="B339">
-        <v>6810158</v>
+        <v>6810159</v>
       </c>
       <c r="C339" t="s">
         <v>28</v>
@@ -30630,73 +30630,73 @@
         <v>45318.69791666666</v>
       </c>
       <c r="F339" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G339" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H339">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I339">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J339" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K339">
-        <v>1.363</v>
+        <v>5.5</v>
       </c>
       <c r="L339">
-        <v>5</v>
+        <v>4.2</v>
       </c>
       <c r="M339">
-        <v>6.5</v>
+        <v>1.5</v>
       </c>
       <c r="N339">
-        <v>1.444</v>
+        <v>6</v>
       </c>
       <c r="O339">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="P339">
-        <v>5.75</v>
+        <v>1.45</v>
       </c>
       <c r="Q339">
-        <v>-1.25</v>
+        <v>1.25</v>
       </c>
       <c r="R339">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="S339">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="T339">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U339">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="V339">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="W339">
         <v>-1</v>
       </c>
       <c r="X339">
-        <v>3.5</v>
+        <v>-1</v>
       </c>
       <c r="Y339">
-        <v>-1</v>
+        <v>0.45</v>
       </c>
       <c r="Z339">
         <v>-1</v>
       </c>
       <c r="AA339">
-        <v>0.8500000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="AB339">
-        <v>1.025</v>
+        <v>0.95</v>
       </c>
       <c r="AC339">
         <v>-1</v>
@@ -30707,7 +30707,7 @@
         <v>338</v>
       </c>
       <c r="B340">
-        <v>6810159</v>
+        <v>6810158</v>
       </c>
       <c r="C340" t="s">
         <v>28</v>
@@ -30719,73 +30719,73 @@
         <v>45318.69791666666</v>
       </c>
       <c r="F340" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G340" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H340">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I340">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J340" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K340">
-        <v>5.5</v>
+        <v>1.363</v>
       </c>
       <c r="L340">
-        <v>4.2</v>
+        <v>5</v>
       </c>
       <c r="M340">
-        <v>1.5</v>
+        <v>6.5</v>
       </c>
       <c r="N340">
-        <v>6</v>
+        <v>1.444</v>
       </c>
       <c r="O340">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="P340">
-        <v>1.45</v>
+        <v>5.75</v>
       </c>
       <c r="Q340">
-        <v>1.25</v>
+        <v>-1.25</v>
       </c>
       <c r="R340">
+        <v>2</v>
+      </c>
+      <c r="S340">
+        <v>1.85</v>
+      </c>
+      <c r="T340">
+        <v>3</v>
+      </c>
+      <c r="U340">
+        <v>2.025</v>
+      </c>
+      <c r="V340">
         <v>1.825</v>
       </c>
-      <c r="S340">
-        <v>2.025</v>
-      </c>
-      <c r="T340">
-        <v>2.75</v>
-      </c>
-      <c r="U340">
-        <v>1.95</v>
-      </c>
-      <c r="V340">
-        <v>1.9</v>
-      </c>
       <c r="W340">
         <v>-1</v>
       </c>
       <c r="X340">
-        <v>-1</v>
+        <v>3.5</v>
       </c>
       <c r="Y340">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
       <c r="Z340">
         <v>-1</v>
       </c>
       <c r="AA340">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AB340">
         <v>1.025</v>
-      </c>
-      <c r="AB340">
-        <v>0.95</v>
       </c>
       <c r="AC340">
         <v>-1</v>
@@ -31330,7 +31330,7 @@
         <v>345</v>
       </c>
       <c r="B347">
-        <v>6810168</v>
+        <v>6810165</v>
       </c>
       <c r="C347" t="s">
         <v>28</v>
@@ -31342,58 +31342,58 @@
         <v>45322.61458333334</v>
       </c>
       <c r="F347" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G347" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H347">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I347">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J347" t="s">
         <v>50</v>
       </c>
       <c r="K347">
-        <v>4.5</v>
+        <v>1.6</v>
       </c>
       <c r="L347">
+        <v>4</v>
+      </c>
+      <c r="M347">
+        <v>5</v>
+      </c>
+      <c r="N347">
+        <v>1.8</v>
+      </c>
+      <c r="O347">
+        <v>3.75</v>
+      </c>
+      <c r="P347">
         <v>4.2</v>
       </c>
-      <c r="M347">
-        <v>1.666</v>
-      </c>
-      <c r="N347">
-        <v>4.333</v>
-      </c>
-      <c r="O347">
-        <v>4</v>
-      </c>
-      <c r="P347">
-        <v>1.7</v>
-      </c>
       <c r="Q347">
-        <v>0.75</v>
+        <v>-0.75</v>
       </c>
       <c r="R347">
+        <v>2.05</v>
+      </c>
+      <c r="S347">
+        <v>1.8</v>
+      </c>
+      <c r="T347">
+        <v>2.75</v>
+      </c>
+      <c r="U347">
         <v>1.95</v>
       </c>
-      <c r="S347">
+      <c r="V347">
         <v>1.9</v>
       </c>
-      <c r="T347">
-        <v>3</v>
-      </c>
-      <c r="U347">
-        <v>1.975</v>
-      </c>
-      <c r="V347">
-        <v>1.875</v>
-      </c>
       <c r="W347">
-        <v>3.333</v>
+        <v>0.8</v>
       </c>
       <c r="X347">
         <v>-1</v>
@@ -31402,16 +31402,16 @@
         <v>-1</v>
       </c>
       <c r="Z347">
-        <v>0.95</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AA347">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB347">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC347">
-        <v>-0</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="348" spans="1:29">
@@ -31419,7 +31419,7 @@
         <v>346</v>
       </c>
       <c r="B348">
-        <v>6810165</v>
+        <v>6810168</v>
       </c>
       <c r="C348" t="s">
         <v>28</v>
@@ -31431,58 +31431,58 @@
         <v>45322.61458333334</v>
       </c>
       <c r="F348" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G348" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H348">
+        <v>2</v>
+      </c>
+      <c r="I348">
         <v>1</v>
-      </c>
-      <c r="I348">
-        <v>0</v>
       </c>
       <c r="J348" t="s">
         <v>50</v>
       </c>
       <c r="K348">
-        <v>1.6</v>
+        <v>4.5</v>
       </c>
       <c r="L348">
+        <v>4.2</v>
+      </c>
+      <c r="M348">
+        <v>1.666</v>
+      </c>
+      <c r="N348">
+        <v>4.333</v>
+      </c>
+      <c r="O348">
         <v>4</v>
       </c>
-      <c r="M348">
-        <v>5</v>
-      </c>
-      <c r="N348">
-        <v>1.8</v>
-      </c>
-      <c r="O348">
-        <v>3.75</v>
-      </c>
       <c r="P348">
-        <v>4.2</v>
+        <v>1.7</v>
       </c>
       <c r="Q348">
-        <v>-0.75</v>
+        <v>0.75</v>
       </c>
       <c r="R348">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="S348">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="T348">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U348">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="V348">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="W348">
-        <v>0.8</v>
+        <v>3.333</v>
       </c>
       <c r="X348">
         <v>-1</v>
@@ -31491,16 +31491,16 @@
         <v>-1</v>
       </c>
       <c r="Z348">
-        <v>0.5249999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="AA348">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB348">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC348">
-        <v>0.8999999999999999</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="349" spans="1:29">
@@ -31686,7 +31686,7 @@
         <v>349</v>
       </c>
       <c r="B351">
-        <v>6810163</v>
+        <v>6810166</v>
       </c>
       <c r="C351" t="s">
         <v>28</v>
@@ -31698,73 +31698,73 @@
         <v>45323.6875</v>
       </c>
       <c r="F351" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G351" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H351">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I351">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J351" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K351">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="L351">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M351">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="N351">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="O351">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P351">
-        <v>2.15</v>
+        <v>2.2</v>
       </c>
       <c r="Q351">
         <v>0.25</v>
       </c>
       <c r="R351">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="S351">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="T351">
         <v>2.5</v>
       </c>
       <c r="U351">
+        <v>1.875</v>
+      </c>
+      <c r="V351">
         <v>1.975</v>
       </c>
-      <c r="V351">
-        <v>1.875</v>
-      </c>
       <c r="W351">
-        <v>2.25</v>
+        <v>-1</v>
       </c>
       <c r="X351">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y351">
         <v>-1</v>
       </c>
       <c r="Z351">
-        <v>0.95</v>
+        <v>0.4625</v>
       </c>
       <c r="AA351">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB351">
-        <v>0.9750000000000001</v>
+        <v>0.875</v>
       </c>
       <c r="AC351">
         <v>-1</v>
@@ -31775,7 +31775,7 @@
         <v>350</v>
       </c>
       <c r="B352">
-        <v>6810166</v>
+        <v>6810163</v>
       </c>
       <c r="C352" t="s">
         <v>28</v>
@@ -31787,73 +31787,73 @@
         <v>45323.6875</v>
       </c>
       <c r="F352" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G352" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H352">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I352">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J352" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K352">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="L352">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M352">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="N352">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="O352">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="P352">
-        <v>2.2</v>
+        <v>2.15</v>
       </c>
       <c r="Q352">
         <v>0.25</v>
       </c>
       <c r="R352">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="S352">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="T352">
         <v>2.5</v>
       </c>
       <c r="U352">
+        <v>1.975</v>
+      </c>
+      <c r="V352">
         <v>1.875</v>
       </c>
-      <c r="V352">
-        <v>1.975</v>
-      </c>
       <c r="W352">
-        <v>-1</v>
+        <v>2.25</v>
       </c>
       <c r="X352">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y352">
         <v>-1</v>
       </c>
       <c r="Z352">
-        <v>0.4625</v>
+        <v>0.95</v>
       </c>
       <c r="AA352">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB352">
-        <v>0.875</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC352">
         <v>-1</v>
@@ -31953,7 +31953,7 @@
         <v>352</v>
       </c>
       <c r="B354">
-        <v>6810174</v>
+        <v>6810171</v>
       </c>
       <c r="C354" t="s">
         <v>28</v>
@@ -31965,76 +31965,76 @@
         <v>45325.59375</v>
       </c>
       <c r="F354" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G354" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H354">
+        <v>1</v>
+      </c>
+      <c r="I354">
         <v>0</v>
       </c>
-      <c r="I354">
-        <v>3</v>
-      </c>
       <c r="J354" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K354">
-        <v>1.909</v>
+        <v>3.2</v>
       </c>
       <c r="L354">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="M354">
-        <v>3.5</v>
+        <v>2.1</v>
       </c>
       <c r="N354">
-        <v>1.909</v>
+        <v>3.4</v>
       </c>
       <c r="O354">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="P354">
-        <v>3.8</v>
+        <v>2.05</v>
       </c>
       <c r="Q354">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R354">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="S354">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="T354">
         <v>2.5</v>
       </c>
       <c r="U354">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="V354">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="W354">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="X354">
         <v>-1</v>
       </c>
       <c r="Y354">
-        <v>2.8</v>
+        <v>-1</v>
       </c>
       <c r="Z354">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AA354">
+        <v>-1</v>
+      </c>
+      <c r="AB354">
+        <v>-1</v>
+      </c>
+      <c r="AC354">
         <v>0.925</v>
-      </c>
-      <c r="AB354">
-        <v>0.8500000000000001</v>
-      </c>
-      <c r="AC354">
-        <v>-1</v>
       </c>
     </row>
     <row r="355" spans="1:29">
@@ -32042,7 +32042,7 @@
         <v>353</v>
       </c>
       <c r="B355">
-        <v>6810171</v>
+        <v>6810174</v>
       </c>
       <c r="C355" t="s">
         <v>28</v>
@@ -32054,76 +32054,76 @@
         <v>45325.59375</v>
       </c>
       <c r="F355" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G355" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H355">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I355">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J355" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K355">
-        <v>3.2</v>
+        <v>1.909</v>
       </c>
       <c r="L355">
+        <v>3.75</v>
+      </c>
+      <c r="M355">
         <v>3.5</v>
       </c>
-      <c r="M355">
-        <v>2.1</v>
-      </c>
       <c r="N355">
-        <v>3.4</v>
+        <v>1.909</v>
       </c>
       <c r="O355">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P355">
-        <v>2.05</v>
+        <v>3.8</v>
       </c>
       <c r="Q355">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R355">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="S355">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="T355">
         <v>2.5</v>
       </c>
       <c r="U355">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="V355">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="W355">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="X355">
         <v>-1</v>
       </c>
       <c r="Y355">
-        <v>-1</v>
+        <v>2.8</v>
       </c>
       <c r="Z355">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AA355">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AB355">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC355">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="356" spans="1:29">
@@ -33283,7 +33283,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="369" spans="1:27">
+    <row r="369" spans="1:29">
       <c r="A369" s="1">
         <v>367</v>
       </c>
@@ -33305,6 +33305,15 @@
       <c r="G369" t="s">
         <v>29</v>
       </c>
+      <c r="H369">
+        <v>2</v>
+      </c>
+      <c r="I369">
+        <v>1</v>
+      </c>
+      <c r="J369" t="s">
+        <v>50</v>
+      </c>
       <c r="K369">
         <v>2.375</v>
       </c>
@@ -33315,13 +33324,13 @@
         <v>2.9</v>
       </c>
       <c r="N369">
-        <v>2.375</v>
+        <v>2.45</v>
       </c>
       <c r="O369">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="P369">
-        <v>3</v>
+        <v>2.875</v>
       </c>
       <c r="Q369">
         <v>-0.25</v>
@@ -33330,34 +33339,40 @@
         <v>2.05</v>
       </c>
       <c r="S369">
-        <v>1.8</v>
+        <v>1.75</v>
       </c>
       <c r="T369">
         <v>2.5</v>
       </c>
       <c r="U369">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="V369">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="W369">
-        <v>0</v>
+        <v>1.45</v>
       </c>
       <c r="X369">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y369">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z369">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="AA369">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="370" spans="1:27">
+        <v>-1</v>
+      </c>
+      <c r="AB369">
+        <v>1.025</v>
+      </c>
+      <c r="AC369">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="370" spans="1:29">
       <c r="A370" s="1">
         <v>368</v>
       </c>
@@ -33431,7 +33446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:27">
+    <row r="371" spans="1:29">
       <c r="A371" s="1">
         <v>369</v>
       </c>
@@ -33466,7 +33481,7 @@
         <v>2.3</v>
       </c>
       <c r="O371">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="P371">
         <v>3</v>
@@ -33484,10 +33499,10 @@
         <v>2.5</v>
       </c>
       <c r="U371">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="V371">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="W371">
         <v>0</v>
@@ -33505,7 +33520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:27">
+    <row r="372" spans="1:29">
       <c r="A372" s="1">
         <v>370</v>
       </c>
@@ -33549,19 +33564,19 @@
         <v>-1</v>
       </c>
       <c r="R372">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="S372">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="T372">
         <v>2.75</v>
       </c>
       <c r="U372">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="V372">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="W372">
         <v>0</v>
@@ -33579,7 +33594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:27">
+    <row r="373" spans="1:29">
       <c r="A373" s="1">
         <v>371</v>
       </c>
@@ -33623,10 +33638,10 @@
         <v>0.5</v>
       </c>
       <c r="R373">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="S373">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="T373">
         <v>2.75</v>
@@ -33653,7 +33668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:27">
+    <row r="374" spans="1:29">
       <c r="A374" s="1">
         <v>372</v>
       </c>
@@ -33727,7 +33742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:27">
+    <row r="375" spans="1:29">
       <c r="A375" s="1">
         <v>373</v>
       </c>
@@ -33801,7 +33816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:27">
+    <row r="376" spans="1:29">
       <c r="A376" s="1">
         <v>374</v>
       </c>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 26-04-2024 às 22:13
</commit_message>
<xml_diff>
--- a/Belgium First Division A/Belgium First Division A.xlsx
+++ b/Belgium First Division A/Belgium First Division A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="54">
   <si>
     <t>id</t>
   </si>
@@ -97,9 +97,6 @@
     <t>PL_AhUnder</t>
   </si>
   <si>
-    <t>7979477</t>
-  </si>
-  <si>
     <t>8009905</t>
   </si>
   <si>
@@ -113,6 +110,9 @@
   </si>
   <si>
     <t>8009321</t>
+  </si>
+  <si>
+    <t>8009888</t>
   </si>
   <si>
     <t>7979555</t>
@@ -537,7 +537,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB287"/>
+  <dimension ref="A1:AB281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2695,7 +2695,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>6810007</v>
+        <v>7030334</v>
       </c>
       <c r="C26" t="s">
         <v>34</v>
@@ -2704,55 +2704,55 @@
         <v>45151.45833333334</v>
       </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F26" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I26" t="s">
         <v>52</v>
       </c>
       <c r="J26">
-        <v>4.75</v>
+        <v>2.75</v>
       </c>
       <c r="K26">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="L26">
-        <v>1.571</v>
+        <v>2.25</v>
       </c>
       <c r="M26">
-        <v>7</v>
+        <v>2.4</v>
       </c>
       <c r="N26">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="O26">
-        <v>1.333</v>
+        <v>2.55</v>
       </c>
       <c r="P26">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="Q26">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="R26">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="S26">
         <v>3</v>
       </c>
       <c r="T26">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="U26">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V26">
         <v>-1</v>
@@ -2761,19 +2761,19 @@
         <v>-1</v>
       </c>
       <c r="X26">
-        <v>0.333</v>
+        <v>1.55</v>
       </c>
       <c r="Y26">
         <v>-1</v>
       </c>
       <c r="Z26">
-        <v>0.9750000000000001</v>
+        <v>1</v>
       </c>
       <c r="AA26">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AB26">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="27" spans="1:28">
@@ -2781,7 +2781,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>7030334</v>
+        <v>6810007</v>
       </c>
       <c r="C27" t="s">
         <v>34</v>
@@ -2790,55 +2790,55 @@
         <v>45151.45833333334</v>
       </c>
       <c r="E27" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I27" t="s">
         <v>52</v>
       </c>
       <c r="J27">
-        <v>2.75</v>
+        <v>4.75</v>
       </c>
       <c r="K27">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="L27">
-        <v>2.25</v>
+        <v>1.571</v>
       </c>
       <c r="M27">
-        <v>2.4</v>
+        <v>7</v>
       </c>
       <c r="N27">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="O27">
-        <v>2.55</v>
+        <v>1.333</v>
       </c>
       <c r="P27">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="Q27">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="R27">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="S27">
         <v>3</v>
       </c>
       <c r="T27">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="U27">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V27">
         <v>-1</v>
@@ -2847,19 +2847,19 @@
         <v>-1</v>
       </c>
       <c r="X27">
-        <v>1.55</v>
+        <v>0.333</v>
       </c>
       <c r="Y27">
         <v>-1</v>
       </c>
       <c r="Z27">
-        <v>1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA27">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AB27">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="28" spans="1:28">
@@ -3383,7 +3383,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>6810012</v>
+        <v>6810015</v>
       </c>
       <c r="C34" t="s">
         <v>34</v>
@@ -3392,61 +3392,61 @@
         <v>45158.45833333334</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F34" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I34" t="s">
         <v>53</v>
       </c>
       <c r="J34">
+        <v>1.45</v>
+      </c>
+      <c r="K34">
+        <v>4.5</v>
+      </c>
+      <c r="L34">
+        <v>7</v>
+      </c>
+      <c r="M34">
         <v>1.533</v>
       </c>
-      <c r="K34">
+      <c r="N34">
         <v>4.2</v>
       </c>
-      <c r="L34">
-        <v>5.5</v>
-      </c>
-      <c r="M34">
-        <v>1.6</v>
-      </c>
-      <c r="N34">
-        <v>4</v>
-      </c>
       <c r="O34">
-        <v>5.25</v>
+        <v>6</v>
       </c>
       <c r="P34">
         <v>-1</v>
       </c>
       <c r="Q34">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="R34">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="S34">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="T34">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="U34">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="V34">
         <v>-1</v>
       </c>
       <c r="W34">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="X34">
         <v>-1</v>
@@ -3455,13 +3455,13 @@
         <v>-1</v>
       </c>
       <c r="Z34">
-        <v>0.875</v>
+        <v>0.95</v>
       </c>
       <c r="AA34">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB34">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="35" spans="1:28">
@@ -3469,7 +3469,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>6810015</v>
+        <v>6810012</v>
       </c>
       <c r="C35" t="s">
         <v>34</v>
@@ -3478,61 +3478,61 @@
         <v>45158.45833333334</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F35" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I35" t="s">
         <v>53</v>
       </c>
       <c r="J35">
-        <v>1.45</v>
+        <v>1.533</v>
       </c>
       <c r="K35">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="L35">
-        <v>7</v>
+        <v>5.5</v>
       </c>
       <c r="M35">
-        <v>1.533</v>
+        <v>1.6</v>
       </c>
       <c r="N35">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="O35">
-        <v>6</v>
+        <v>5.25</v>
       </c>
       <c r="P35">
         <v>-1</v>
       </c>
       <c r="Q35">
+        <v>1.975</v>
+      </c>
+      <c r="R35">
+        <v>1.875</v>
+      </c>
+      <c r="S35">
+        <v>3</v>
+      </c>
+      <c r="T35">
         <v>1.9</v>
       </c>
-      <c r="R35">
+      <c r="U35">
         <v>1.95</v>
       </c>
-      <c r="S35">
-        <v>2.5</v>
-      </c>
-      <c r="T35">
-        <v>1.8</v>
-      </c>
-      <c r="U35">
-        <v>2.05</v>
-      </c>
       <c r="V35">
         <v>-1</v>
       </c>
       <c r="W35">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="X35">
         <v>-1</v>
@@ -3541,13 +3541,13 @@
         <v>-1</v>
       </c>
       <c r="Z35">
+        <v>0.875</v>
+      </c>
+      <c r="AA35">
+        <v>-1</v>
+      </c>
+      <c r="AB35">
         <v>0.95</v>
-      </c>
-      <c r="AA35">
-        <v>0.8</v>
-      </c>
-      <c r="AB35">
-        <v>-1</v>
       </c>
     </row>
     <row r="36" spans="1:28">
@@ -15509,7 +15509,7 @@
         <v>173</v>
       </c>
       <c r="B175">
-        <v>6810158</v>
+        <v>6810159</v>
       </c>
       <c r="C175" t="s">
         <v>34</v>
@@ -15518,73 +15518,73 @@
         <v>45318.69791666666</v>
       </c>
       <c r="E175" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F175" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G175">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H175">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I175" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J175">
-        <v>1.363</v>
+        <v>5.5</v>
       </c>
       <c r="K175">
-        <v>5</v>
+        <v>4.2</v>
       </c>
       <c r="L175">
-        <v>6.5</v>
+        <v>1.5</v>
       </c>
       <c r="M175">
-        <v>1.444</v>
+        <v>6</v>
       </c>
       <c r="N175">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="O175">
-        <v>5.75</v>
+        <v>1.45</v>
       </c>
       <c r="P175">
-        <v>-1.25</v>
+        <v>1.25</v>
       </c>
       <c r="Q175">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="R175">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="S175">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="T175">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="U175">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="V175">
         <v>-1</v>
       </c>
       <c r="W175">
-        <v>3.5</v>
+        <v>-1</v>
       </c>
       <c r="X175">
-        <v>-1</v>
+        <v>0.45</v>
       </c>
       <c r="Y175">
         <v>-1</v>
       </c>
       <c r="Z175">
-        <v>0.8500000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="AA175">
-        <v>1.025</v>
+        <v>0.95</v>
       </c>
       <c r="AB175">
         <v>-1</v>
@@ -15595,7 +15595,7 @@
         <v>174</v>
       </c>
       <c r="B176">
-        <v>6810159</v>
+        <v>6810158</v>
       </c>
       <c r="C176" t="s">
         <v>34</v>
@@ -15604,73 +15604,73 @@
         <v>45318.69791666666</v>
       </c>
       <c r="E176" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F176" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="G176">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H176">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I176" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J176">
-        <v>5.5</v>
+        <v>1.363</v>
       </c>
       <c r="K176">
-        <v>4.2</v>
+        <v>5</v>
       </c>
       <c r="L176">
-        <v>1.5</v>
+        <v>6.5</v>
       </c>
       <c r="M176">
-        <v>6</v>
+        <v>1.444</v>
       </c>
       <c r="N176">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="O176">
-        <v>1.45</v>
+        <v>5.75</v>
       </c>
       <c r="P176">
-        <v>1.25</v>
+        <v>-1.25</v>
       </c>
       <c r="Q176">
+        <v>2</v>
+      </c>
+      <c r="R176">
+        <v>1.85</v>
+      </c>
+      <c r="S176">
+        <v>3</v>
+      </c>
+      <c r="T176">
+        <v>2.025</v>
+      </c>
+      <c r="U176">
         <v>1.825</v>
       </c>
-      <c r="R176">
-        <v>2.025</v>
-      </c>
-      <c r="S176">
-        <v>2.75</v>
-      </c>
-      <c r="T176">
-        <v>1.95</v>
-      </c>
-      <c r="U176">
-        <v>1.9</v>
-      </c>
       <c r="V176">
         <v>-1</v>
       </c>
       <c r="W176">
-        <v>-1</v>
+        <v>3.5</v>
       </c>
       <c r="X176">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
       <c r="Y176">
         <v>-1</v>
       </c>
       <c r="Z176">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AA176">
         <v>1.025</v>
-      </c>
-      <c r="AA176">
-        <v>0.95</v>
       </c>
       <c r="AB176">
         <v>-1</v>
@@ -16025,7 +16025,7 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>6810169</v>
+        <v>6810167</v>
       </c>
       <c r="C181" t="s">
         <v>34</v>
@@ -16034,73 +16034,73 @@
         <v>45321.6875</v>
       </c>
       <c r="E181" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F181" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="G181">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H181">
+        <v>3</v>
+      </c>
+      <c r="I181" t="s">
+        <v>53</v>
+      </c>
+      <c r="J181">
+        <v>1.125</v>
+      </c>
+      <c r="K181">
+        <v>8.5</v>
+      </c>
+      <c r="L181">
+        <v>17</v>
+      </c>
+      <c r="M181">
+        <v>1.125</v>
+      </c>
+      <c r="N181">
+        <v>8.5</v>
+      </c>
+      <c r="O181">
+        <v>17</v>
+      </c>
+      <c r="P181">
+        <v>-2.25</v>
+      </c>
+      <c r="Q181">
+        <v>1.85</v>
+      </c>
+      <c r="R181">
         <v>2</v>
       </c>
-      <c r="I181" t="s">
-        <v>51</v>
-      </c>
-      <c r="J181">
-        <v>3.4</v>
-      </c>
-      <c r="K181">
-        <v>3.8</v>
-      </c>
-      <c r="L181">
+      <c r="S181">
+        <v>3.5</v>
+      </c>
+      <c r="T181">
+        <v>1.9</v>
+      </c>
+      <c r="U181">
         <v>1.95</v>
       </c>
-      <c r="M181">
-        <v>3.3</v>
-      </c>
-      <c r="N181">
-        <v>3.6</v>
-      </c>
-      <c r="O181">
-        <v>2.05</v>
-      </c>
-      <c r="P181">
-        <v>0.25</v>
-      </c>
-      <c r="Q181">
-        <v>2</v>
-      </c>
-      <c r="R181">
-        <v>1.85</v>
-      </c>
-      <c r="S181">
-        <v>2.75</v>
-      </c>
-      <c r="T181">
-        <v>1.975</v>
-      </c>
-      <c r="U181">
-        <v>1.875</v>
-      </c>
       <c r="V181">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="W181">
-        <v>-1</v>
+        <v>7.5</v>
       </c>
       <c r="X181">
         <v>-1</v>
       </c>
       <c r="Y181">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Z181">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AA181">
-        <v>0.9750000000000001</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB181">
         <v>-1</v>
@@ -16111,7 +16111,7 @@
         <v>180</v>
       </c>
       <c r="B182">
-        <v>6810167</v>
+        <v>6810169</v>
       </c>
       <c r="C182" t="s">
         <v>34</v>
@@ -16120,73 +16120,73 @@
         <v>45321.6875</v>
       </c>
       <c r="E182" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F182" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="G182">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H182">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I182" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J182">
-        <v>1.125</v>
+        <v>3.4</v>
       </c>
       <c r="K182">
-        <v>8.5</v>
+        <v>3.8</v>
       </c>
       <c r="L182">
-        <v>17</v>
+        <v>1.95</v>
       </c>
       <c r="M182">
-        <v>1.125</v>
+        <v>3.3</v>
       </c>
       <c r="N182">
-        <v>8.5</v>
+        <v>3.6</v>
       </c>
       <c r="O182">
-        <v>17</v>
+        <v>2.05</v>
       </c>
       <c r="P182">
-        <v>-2.25</v>
+        <v>0.25</v>
       </c>
       <c r="Q182">
+        <v>2</v>
+      </c>
+      <c r="R182">
         <v>1.85</v>
       </c>
-      <c r="R182">
-        <v>2</v>
-      </c>
       <c r="S182">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="T182">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="U182">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V182">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="W182">
-        <v>7.5</v>
+        <v>-1</v>
       </c>
       <c r="X182">
         <v>-1</v>
       </c>
       <c r="Y182">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z182">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AA182">
-        <v>0.8999999999999999</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB182">
         <v>-1</v>
@@ -21185,7 +21185,7 @@
         <v>239</v>
       </c>
       <c r="B241">
-        <v>6810219</v>
+        <v>6870199</v>
       </c>
       <c r="C241" t="s">
         <v>34</v>
@@ -21194,13 +21194,13 @@
         <v>45368.60416666666</v>
       </c>
       <c r="E241" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F241" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G241">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H241">
         <v>0</v>
@@ -21209,25 +21209,25 @@
         <v>51</v>
       </c>
       <c r="J241">
-        <v>2.8</v>
+        <v>1.363</v>
       </c>
       <c r="K241">
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="L241">
-        <v>2.375</v>
+        <v>7.5</v>
       </c>
       <c r="M241">
-        <v>2.7</v>
+        <v>1.3</v>
       </c>
       <c r="N241">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="O241">
-        <v>2.45</v>
+        <v>8.5</v>
       </c>
       <c r="P241">
-        <v>0</v>
+        <v>-1.75</v>
       </c>
       <c r="Q241">
         <v>2.025</v>
@@ -21236,16 +21236,16 @@
         <v>1.825</v>
       </c>
       <c r="S241">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="T241">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="U241">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V241">
-        <v>1.7</v>
+        <v>0.3</v>
       </c>
       <c r="W241">
         <v>-1</v>
@@ -21260,10 +21260,10 @@
         <v>-1</v>
       </c>
       <c r="AA241">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB241">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="242" spans="1:28">
@@ -21271,7 +21271,7 @@
         <v>240</v>
       </c>
       <c r="B242">
-        <v>6942395</v>
+        <v>6957874</v>
       </c>
       <c r="C242" t="s">
         <v>34</v>
@@ -21280,76 +21280,76 @@
         <v>45368.60416666666</v>
       </c>
       <c r="E242" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="F242" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G242">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H242">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I242" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J242">
-        <v>1.571</v>
+        <v>3.6</v>
       </c>
       <c r="K242">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="L242">
-        <v>5.75</v>
+        <v>1.909</v>
       </c>
       <c r="M242">
-        <v>1.4</v>
+        <v>3.6</v>
       </c>
       <c r="N242">
-        <v>4.333</v>
+        <v>3.75</v>
       </c>
       <c r="O242">
-        <v>8</v>
+        <v>1.95</v>
       </c>
       <c r="P242">
-        <v>-1.25</v>
+        <v>0.5</v>
       </c>
       <c r="Q242">
+        <v>1.85</v>
+      </c>
+      <c r="R242">
         <v>2</v>
       </c>
-      <c r="R242">
+      <c r="S242">
+        <v>3</v>
+      </c>
+      <c r="T242">
+        <v>2</v>
+      </c>
+      <c r="U242">
         <v>1.85</v>
       </c>
-      <c r="S242">
+      <c r="V242">
+        <v>-1</v>
+      </c>
+      <c r="W242">
         <v>2.75</v>
       </c>
-      <c r="T242">
-        <v>1.95</v>
-      </c>
-      <c r="U242">
-        <v>1.9</v>
-      </c>
-      <c r="V242">
-        <v>0.3999999999999999</v>
-      </c>
-      <c r="W242">
-        <v>-1</v>
-      </c>
       <c r="X242">
         <v>-1</v>
       </c>
       <c r="Y242">
-        <v>1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z242">
         <v>-1</v>
       </c>
       <c r="AA242">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB242">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="243" spans="1:28">
@@ -21357,7 +21357,7 @@
         <v>241</v>
       </c>
       <c r="B243">
-        <v>6957874</v>
+        <v>6942395</v>
       </c>
       <c r="C243" t="s">
         <v>34</v>
@@ -21366,76 +21366,76 @@
         <v>45368.60416666666</v>
       </c>
       <c r="E243" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="F243" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G243">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H243">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I243" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J243">
-        <v>3.6</v>
+        <v>1.571</v>
       </c>
       <c r="K243">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="L243">
-        <v>1.909</v>
+        <v>5.75</v>
       </c>
       <c r="M243">
-        <v>3.6</v>
+        <v>1.4</v>
       </c>
       <c r="N243">
-        <v>3.75</v>
+        <v>4.333</v>
       </c>
       <c r="O243">
+        <v>8</v>
+      </c>
+      <c r="P243">
+        <v>-1.25</v>
+      </c>
+      <c r="Q243">
+        <v>2</v>
+      </c>
+      <c r="R243">
+        <v>1.85</v>
+      </c>
+      <c r="S243">
+        <v>2.75</v>
+      </c>
+      <c r="T243">
         <v>1.95</v>
       </c>
-      <c r="P243">
-        <v>0.5</v>
-      </c>
-      <c r="Q243">
-        <v>1.85</v>
-      </c>
-      <c r="R243">
-        <v>2</v>
-      </c>
-      <c r="S243">
-        <v>3</v>
-      </c>
-      <c r="T243">
-        <v>2</v>
-      </c>
       <c r="U243">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="V243">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="W243">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="X243">
         <v>-1</v>
       </c>
       <c r="Y243">
-        <v>0.8500000000000001</v>
+        <v>1</v>
       </c>
       <c r="Z243">
         <v>-1</v>
       </c>
       <c r="AA243">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB243">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="244" spans="1:28">
@@ -21443,7 +21443,7 @@
         <v>242</v>
       </c>
       <c r="B244">
-        <v>6870199</v>
+        <v>6810219</v>
       </c>
       <c r="C244" t="s">
         <v>34</v>
@@ -21452,13 +21452,13 @@
         <v>45368.60416666666</v>
       </c>
       <c r="E244" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F244" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G244">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H244">
         <v>0</v>
@@ -21467,25 +21467,25 @@
         <v>51</v>
       </c>
       <c r="J244">
-        <v>1.363</v>
+        <v>2.8</v>
       </c>
       <c r="K244">
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="L244">
-        <v>7.5</v>
+        <v>2.375</v>
       </c>
       <c r="M244">
-        <v>1.3</v>
+        <v>2.7</v>
       </c>
       <c r="N244">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="O244">
-        <v>8.5</v>
+        <v>2.45</v>
       </c>
       <c r="P244">
-        <v>-1.75</v>
+        <v>0</v>
       </c>
       <c r="Q244">
         <v>2.025</v>
@@ -21494,16 +21494,16 @@
         <v>1.825</v>
       </c>
       <c r="S244">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="T244">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="U244">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V244">
-        <v>0.3</v>
+        <v>1.7</v>
       </c>
       <c r="W244">
         <v>-1</v>
@@ -21518,10 +21518,10 @@
         <v>-1</v>
       </c>
       <c r="AA244">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB244">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="245" spans="1:28">
@@ -24108,516 +24108,390 @@
       <c r="A275" s="1">
         <v>273</v>
       </c>
-      <c r="B275">
-        <v>7979346</v>
+      <c r="B275" t="s">
+        <v>27</v>
       </c>
       <c r="C275" t="s">
         <v>34</v>
       </c>
       <c r="D275" s="2">
-        <v>45405.64583333334</v>
+        <v>45409.45833333334</v>
       </c>
       <c r="E275" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F275" t="s">
-        <v>35</v>
-      </c>
-      <c r="G275">
-        <v>0</v>
-      </c>
-      <c r="H275">
-        <v>2</v>
-      </c>
-      <c r="I275" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J275">
+        <v>1.95</v>
+      </c>
+      <c r="K275">
         <v>3.6</v>
       </c>
-      <c r="K275">
+      <c r="L275">
+        <v>3.6</v>
+      </c>
+      <c r="M275">
+        <v>1.95</v>
+      </c>
+      <c r="N275">
+        <v>3.75</v>
+      </c>
+      <c r="O275">
         <v>3.5</v>
       </c>
-      <c r="L275">
-        <v>2</v>
-      </c>
-      <c r="M275">
-        <v>3.3</v>
-      </c>
-      <c r="N275">
-        <v>3.6</v>
-      </c>
-      <c r="O275">
-        <v>2.05</v>
-      </c>
       <c r="P275">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q275">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="R275">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="S275">
         <v>3</v>
       </c>
       <c r="T275">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="U275">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="V275">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="W275">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X275">
-        <v>1.05</v>
-      </c>
-      <c r="Y275">
-        <v>-1</v>
-      </c>
-      <c r="Z275">
-        <v>0.825</v>
-      </c>
-      <c r="AA275">
-        <v>-1</v>
-      </c>
-      <c r="AB275">
-        <v>0.875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="276" spans="1:28">
       <c r="A276" s="1">
         <v>274</v>
       </c>
-      <c r="B276">
-        <v>7979470</v>
+      <c r="B276" t="s">
+        <v>28</v>
       </c>
       <c r="C276" t="s">
         <v>34</v>
       </c>
       <c r="D276" s="2">
-        <v>45405.64583333334</v>
+        <v>45409.55208333334</v>
       </c>
       <c r="E276" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F276" t="s">
-        <v>46</v>
-      </c>
-      <c r="G276">
-        <v>1</v>
-      </c>
-      <c r="H276">
-        <v>1</v>
-      </c>
-      <c r="I276" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J276">
+        <v>2.2</v>
+      </c>
+      <c r="K276">
+        <v>3.4</v>
+      </c>
+      <c r="L276">
+        <v>3.25</v>
+      </c>
+      <c r="M276">
+        <v>2.2</v>
+      </c>
+      <c r="N276">
+        <v>3.4</v>
+      </c>
+      <c r="O276">
+        <v>3.2</v>
+      </c>
+      <c r="P276">
+        <v>-0.25</v>
+      </c>
+      <c r="Q276">
+        <v>1.9</v>
+      </c>
+      <c r="R276">
+        <v>1.95</v>
+      </c>
+      <c r="S276">
         <v>2.5</v>
       </c>
-      <c r="K276">
-        <v>3.6</v>
-      </c>
-      <c r="L276">
-        <v>2.6</v>
-      </c>
-      <c r="M276">
-        <v>2.45</v>
-      </c>
-      <c r="N276">
-        <v>3.75</v>
-      </c>
-      <c r="O276">
-        <v>2.55</v>
-      </c>
-      <c r="P276">
-        <v>0</v>
-      </c>
-      <c r="Q276">
+      <c r="T276">
         <v>1.875</v>
       </c>
-      <c r="R276">
+      <c r="U276">
         <v>1.975</v>
       </c>
-      <c r="S276">
-        <v>3</v>
-      </c>
-      <c r="T276">
-        <v>1.85</v>
-      </c>
-      <c r="U276">
-        <v>2</v>
-      </c>
       <c r="V276">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="W276">
-        <v>2.75</v>
+        <v>0</v>
       </c>
       <c r="X276">
-        <v>-1</v>
-      </c>
-      <c r="Y276">
-        <v>0</v>
-      </c>
-      <c r="Z276">
-        <v>0</v>
-      </c>
-      <c r="AA276">
-        <v>-1</v>
-      </c>
-      <c r="AB276">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="277" spans="1:28">
       <c r="A277" s="1">
         <v>275</v>
       </c>
-      <c r="B277">
-        <v>7979471</v>
+      <c r="B277" t="s">
+        <v>29</v>
       </c>
       <c r="C277" t="s">
         <v>34</v>
       </c>
       <c r="D277" s="2">
-        <v>45405.64583333334</v>
+        <v>45409.65625</v>
       </c>
       <c r="E277" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F277" t="s">
-        <v>48</v>
-      </c>
-      <c r="G277">
-        <v>0</v>
-      </c>
-      <c r="H277">
-        <v>0</v>
-      </c>
-      <c r="I277" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J277">
-        <v>2.5</v>
+        <v>1.4</v>
       </c>
       <c r="K277">
-        <v>3.4</v>
+        <v>5</v>
       </c>
       <c r="L277">
-        <v>2.7</v>
+        <v>7</v>
       </c>
       <c r="M277">
-        <v>2.5</v>
+        <v>1.333</v>
       </c>
       <c r="N277">
+        <v>5.5</v>
+      </c>
+      <c r="O277">
+        <v>7</v>
+      </c>
+      <c r="P277">
+        <v>-1.5</v>
+      </c>
+      <c r="Q277">
+        <v>1.9</v>
+      </c>
+      <c r="R277">
+        <v>1.95</v>
+      </c>
+      <c r="S277">
         <v>3.5</v>
       </c>
-      <c r="O277">
-        <v>2.625</v>
-      </c>
-      <c r="P277">
-        <v>0</v>
-      </c>
-      <c r="Q277">
-        <v>1.875</v>
-      </c>
-      <c r="R277">
-        <v>1.975</v>
-      </c>
-      <c r="S277">
-        <v>2.75</v>
-      </c>
       <c r="T277">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="U277">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="V277">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="W277">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="X277">
-        <v>-1</v>
-      </c>
-      <c r="Y277">
-        <v>0</v>
-      </c>
-      <c r="Z277">
-        <v>0</v>
-      </c>
-      <c r="AA277">
-        <v>-1</v>
-      </c>
-      <c r="AB277">
-        <v>0.925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="278" spans="1:28">
       <c r="A278" s="1">
         <v>276</v>
       </c>
-      <c r="B278">
-        <v>7979473</v>
+      <c r="B278" t="s">
+        <v>30</v>
       </c>
       <c r="C278" t="s">
         <v>34</v>
       </c>
       <c r="D278" s="2">
-        <v>45406.64583333334</v>
+        <v>45410.35416666666</v>
       </c>
       <c r="E278" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="F278" t="s">
-        <v>36</v>
-      </c>
-      <c r="G278">
-        <v>3</v>
-      </c>
-      <c r="H278">
-        <v>0</v>
-      </c>
-      <c r="I278" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J278">
-        <v>1.909</v>
+        <v>2.9</v>
       </c>
       <c r="K278">
         <v>3.6</v>
       </c>
       <c r="L278">
-        <v>3.8</v>
+        <v>2.25</v>
       </c>
       <c r="M278">
-        <v>1.8</v>
+        <v>2.9</v>
       </c>
       <c r="N278">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="O278">
-        <v>4</v>
+        <v>2.25</v>
       </c>
       <c r="P278">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Q278">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="R278">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="S278">
         <v>2.75</v>
       </c>
       <c r="T278">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="U278">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="V278">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="W278">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X278">
-        <v>-1</v>
-      </c>
-      <c r="Y278">
-        <v>0.8500000000000001</v>
-      </c>
-      <c r="Z278">
-        <v>-1</v>
-      </c>
-      <c r="AA278">
-        <v>0.425</v>
-      </c>
-      <c r="AB278">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:28">
       <c r="A279" s="1">
         <v>277</v>
       </c>
-      <c r="B279">
-        <v>7979357</v>
+      <c r="B279" t="s">
+        <v>31</v>
       </c>
       <c r="C279" t="s">
         <v>34</v>
       </c>
       <c r="D279" s="2">
-        <v>45406.64583333334</v>
+        <v>45410.45833333334</v>
       </c>
       <c r="E279" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F279" t="s">
-        <v>38</v>
-      </c>
-      <c r="G279">
-        <v>4</v>
-      </c>
-      <c r="H279">
-        <v>0</v>
-      </c>
-      <c r="I279" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J279">
-        <v>1.85</v>
+        <v>2.8</v>
       </c>
       <c r="K279">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="L279">
-        <v>3.9</v>
+        <v>2.375</v>
       </c>
       <c r="M279">
-        <v>1.75</v>
+        <v>2.875</v>
       </c>
       <c r="N279">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="O279">
-        <v>4.5</v>
+        <v>2.3</v>
       </c>
       <c r="P279">
-        <v>-0.75</v>
+        <v>0.25</v>
       </c>
       <c r="Q279">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="R279">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="S279">
         <v>2.75</v>
       </c>
       <c r="T279">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="U279">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="V279">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="W279">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X279">
-        <v>-1</v>
-      </c>
-      <c r="Y279">
-        <v>1</v>
-      </c>
-      <c r="Z279">
-        <v>-1</v>
-      </c>
-      <c r="AA279">
-        <v>1.025</v>
-      </c>
-      <c r="AB279">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:28">
       <c r="A280" s="1">
         <v>278</v>
       </c>
-      <c r="B280">
-        <v>7979358</v>
+      <c r="B280" t="s">
+        <v>32</v>
       </c>
       <c r="C280" t="s">
         <v>34</v>
       </c>
       <c r="D280" s="2">
-        <v>45407.64583333334</v>
+        <v>45410.5625</v>
       </c>
       <c r="E280" t="s">
+        <v>37</v>
+      </c>
+      <c r="F280" t="s">
         <v>42</v>
       </c>
-      <c r="F280" t="s">
-        <v>37</v>
-      </c>
-      <c r="G280">
-        <v>0</v>
-      </c>
-      <c r="H280">
-        <v>3</v>
-      </c>
-      <c r="I280" t="s">
-        <v>52</v>
-      </c>
       <c r="J280">
-        <v>2.8</v>
+        <v>1.666</v>
       </c>
       <c r="K280">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="L280">
-        <v>2.375</v>
+        <v>4.75</v>
       </c>
       <c r="M280">
-        <v>3</v>
+        <v>1.666</v>
       </c>
       <c r="N280">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="O280">
-        <v>2.15</v>
+        <v>4.75</v>
       </c>
       <c r="P280">
-        <v>0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="Q280">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="R280">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="S280">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="T280">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="U280">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="V280">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="W280">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X280">
-        <v>1.15</v>
-      </c>
-      <c r="Y280">
-        <v>-1</v>
-      </c>
-      <c r="Z280">
-        <v>0.925</v>
-      </c>
-      <c r="AA280">
-        <v>0.925</v>
-      </c>
-      <c r="AB280">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:28">
@@ -24625,56 +24499,56 @@
         <v>279</v>
       </c>
       <c r="B281" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C281" t="s">
         <v>34</v>
       </c>
       <c r="D281" s="2">
-        <v>45408.65625</v>
+        <v>45410.59375</v>
       </c>
       <c r="E281" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F281" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J281">
-        <v>2.875</v>
+        <v>2.25</v>
       </c>
       <c r="K281">
+        <v>3.5</v>
+      </c>
+      <c r="L281">
+        <v>3</v>
+      </c>
+      <c r="M281">
+        <v>2.375</v>
+      </c>
+      <c r="N281">
         <v>3.4</v>
       </c>
-      <c r="L281">
-        <v>2.375</v>
-      </c>
-      <c r="M281">
-        <v>3.25</v>
-      </c>
-      <c r="N281">
-        <v>3.3</v>
-      </c>
       <c r="O281">
-        <v>2.2</v>
+        <v>2.9</v>
       </c>
       <c r="P281">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="Q281">
+        <v>2.05</v>
+      </c>
+      <c r="R281">
+        <v>1.8</v>
+      </c>
+      <c r="S281">
+        <v>2.5</v>
+      </c>
+      <c r="T281">
         <v>1.925</v>
       </c>
-      <c r="R281">
+      <c r="U281">
         <v>1.925</v>
       </c>
-      <c r="S281">
-        <v>2.25</v>
-      </c>
-      <c r="T281">
-        <v>1.85</v>
-      </c>
-      <c r="U281">
-        <v>2</v>
-      </c>
       <c r="V281">
         <v>0</v>
       </c>
@@ -24682,396 +24556,6 @@
         <v>0</v>
       </c>
       <c r="X281">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="282" spans="1:28">
-      <c r="A282" s="1">
-        <v>280</v>
-      </c>
-      <c r="B282" t="s">
-        <v>28</v>
-      </c>
-      <c r="C282" t="s">
-        <v>34</v>
-      </c>
-      <c r="D282" s="2">
-        <v>45409.45833333334</v>
-      </c>
-      <c r="E282" t="s">
-        <v>48</v>
-      </c>
-      <c r="F282" t="s">
-        <v>46</v>
-      </c>
-      <c r="J282">
-        <v>1.95</v>
-      </c>
-      <c r="K282">
-        <v>3.6</v>
-      </c>
-      <c r="L282">
-        <v>3.6</v>
-      </c>
-      <c r="M282">
-        <v>1.95</v>
-      </c>
-      <c r="N282">
-        <v>3.75</v>
-      </c>
-      <c r="O282">
-        <v>3.6</v>
-      </c>
-      <c r="P282">
-        <v>-0.5</v>
-      </c>
-      <c r="Q282">
-        <v>1.95</v>
-      </c>
-      <c r="R282">
-        <v>1.9</v>
-      </c>
-      <c r="S282">
-        <v>2.75</v>
-      </c>
-      <c r="T282">
-        <v>1.875</v>
-      </c>
-      <c r="U282">
-        <v>1.975</v>
-      </c>
-      <c r="V282">
-        <v>0</v>
-      </c>
-      <c r="W282">
-        <v>0</v>
-      </c>
-      <c r="X282">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="283" spans="1:28">
-      <c r="A283" s="1">
-        <v>281</v>
-      </c>
-      <c r="B283" t="s">
-        <v>29</v>
-      </c>
-      <c r="C283" t="s">
-        <v>34</v>
-      </c>
-      <c r="D283" s="2">
-        <v>45409.55208333334</v>
-      </c>
-      <c r="E283" t="s">
-        <v>45</v>
-      </c>
-      <c r="F283" t="s">
-        <v>44</v>
-      </c>
-      <c r="J283">
-        <v>2.2</v>
-      </c>
-      <c r="K283">
-        <v>3.4</v>
-      </c>
-      <c r="L283">
-        <v>3.25</v>
-      </c>
-      <c r="M283">
-        <v>2.25</v>
-      </c>
-      <c r="N283">
-        <v>3.4</v>
-      </c>
-      <c r="O283">
-        <v>3.1</v>
-      </c>
-      <c r="P283">
-        <v>-0.25</v>
-      </c>
-      <c r="Q283">
-        <v>1.95</v>
-      </c>
-      <c r="R283">
-        <v>1.9</v>
-      </c>
-      <c r="S283">
-        <v>2.5</v>
-      </c>
-      <c r="T283">
-        <v>1.875</v>
-      </c>
-      <c r="U283">
-        <v>1.975</v>
-      </c>
-      <c r="V283">
-        <v>0</v>
-      </c>
-      <c r="W283">
-        <v>0</v>
-      </c>
-      <c r="X283">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284" spans="1:28">
-      <c r="A284" s="1">
-        <v>282</v>
-      </c>
-      <c r="B284" t="s">
-        <v>30</v>
-      </c>
-      <c r="C284" t="s">
-        <v>34</v>
-      </c>
-      <c r="D284" s="2">
-        <v>45409.65625</v>
-      </c>
-      <c r="E284" t="s">
-        <v>35</v>
-      </c>
-      <c r="F284" t="s">
-        <v>49</v>
-      </c>
-      <c r="J284">
-        <v>1.4</v>
-      </c>
-      <c r="K284">
-        <v>5</v>
-      </c>
-      <c r="L284">
-        <v>7</v>
-      </c>
-      <c r="M284">
-        <v>1.363</v>
-      </c>
-      <c r="N284">
-        <v>5.25</v>
-      </c>
-      <c r="O284">
-        <v>7</v>
-      </c>
-      <c r="P284">
-        <v>-1.5</v>
-      </c>
-      <c r="Q284">
-        <v>1.95</v>
-      </c>
-      <c r="R284">
-        <v>1.9</v>
-      </c>
-      <c r="S284">
-        <v>3.25</v>
-      </c>
-      <c r="T284">
-        <v>1.85</v>
-      </c>
-      <c r="U284">
-        <v>2</v>
-      </c>
-      <c r="V284">
-        <v>0</v>
-      </c>
-      <c r="W284">
-        <v>0</v>
-      </c>
-      <c r="X284">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="285" spans="1:28">
-      <c r="A285" s="1">
-        <v>283</v>
-      </c>
-      <c r="B285" t="s">
-        <v>31</v>
-      </c>
-      <c r="C285" t="s">
-        <v>34</v>
-      </c>
-      <c r="D285" s="2">
-        <v>45410.35416666666</v>
-      </c>
-      <c r="E285" t="s">
-        <v>38</v>
-      </c>
-      <c r="F285" t="s">
-        <v>43</v>
-      </c>
-      <c r="J285">
-        <v>2.9</v>
-      </c>
-      <c r="K285">
-        <v>3.6</v>
-      </c>
-      <c r="L285">
-        <v>2.25</v>
-      </c>
-      <c r="M285">
-        <v>2.9</v>
-      </c>
-      <c r="N285">
-        <v>3.6</v>
-      </c>
-      <c r="O285">
-        <v>2.25</v>
-      </c>
-      <c r="P285">
-        <v>0.25</v>
-      </c>
-      <c r="Q285">
-        <v>1.875</v>
-      </c>
-      <c r="R285">
-        <v>1.975</v>
-      </c>
-      <c r="S285">
-        <v>2.75</v>
-      </c>
-      <c r="T285">
-        <v>1.825</v>
-      </c>
-      <c r="U285">
-        <v>2.025</v>
-      </c>
-      <c r="V285">
-        <v>0</v>
-      </c>
-      <c r="W285">
-        <v>0</v>
-      </c>
-      <c r="X285">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="286" spans="1:28">
-      <c r="A286" s="1">
-        <v>284</v>
-      </c>
-      <c r="B286" t="s">
-        <v>32</v>
-      </c>
-      <c r="C286" t="s">
-        <v>34</v>
-      </c>
-      <c r="D286" s="2">
-        <v>45410.45833333334</v>
-      </c>
-      <c r="E286" t="s">
-        <v>36</v>
-      </c>
-      <c r="F286" t="s">
-        <v>47</v>
-      </c>
-      <c r="J286">
-        <v>2.8</v>
-      </c>
-      <c r="K286">
-        <v>3.5</v>
-      </c>
-      <c r="L286">
-        <v>2.375</v>
-      </c>
-      <c r="M286">
-        <v>2.8</v>
-      </c>
-      <c r="N286">
-        <v>3.5</v>
-      </c>
-      <c r="O286">
-        <v>2.375</v>
-      </c>
-      <c r="P286">
-        <v>0</v>
-      </c>
-      <c r="Q286">
-        <v>2.1</v>
-      </c>
-      <c r="R286">
-        <v>1.775</v>
-      </c>
-      <c r="S286">
-        <v>2.75</v>
-      </c>
-      <c r="T286">
-        <v>1.925</v>
-      </c>
-      <c r="U286">
-        <v>1.925</v>
-      </c>
-      <c r="V286">
-        <v>0</v>
-      </c>
-      <c r="W286">
-        <v>0</v>
-      </c>
-      <c r="X286">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="287" spans="1:28">
-      <c r="A287" s="1">
-        <v>285</v>
-      </c>
-      <c r="B287" t="s">
-        <v>33</v>
-      </c>
-      <c r="C287" t="s">
-        <v>34</v>
-      </c>
-      <c r="D287" s="2">
-        <v>45410.59375</v>
-      </c>
-      <c r="E287" t="s">
-        <v>41</v>
-      </c>
-      <c r="F287" t="s">
-        <v>50</v>
-      </c>
-      <c r="J287">
-        <v>2.25</v>
-      </c>
-      <c r="K287">
-        <v>3.5</v>
-      </c>
-      <c r="L287">
-        <v>3</v>
-      </c>
-      <c r="M287">
-        <v>2.375</v>
-      </c>
-      <c r="N287">
-        <v>3.4</v>
-      </c>
-      <c r="O287">
-        <v>2.9</v>
-      </c>
-      <c r="P287">
-        <v>-0.25</v>
-      </c>
-      <c r="Q287">
-        <v>2.05</v>
-      </c>
-      <c r="R287">
-        <v>1.8</v>
-      </c>
-      <c r="S287">
-        <v>2.5</v>
-      </c>
-      <c r="T287">
-        <v>1.925</v>
-      </c>
-      <c r="U287">
-        <v>1.925</v>
-      </c>
-      <c r="V287">
-        <v>0</v>
-      </c>
-      <c r="W287">
-        <v>0</v>
-      </c>
-      <c r="X287">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 25-05-2024 às 15:10
</commit_message>
<xml_diff>
--- a/Belgium First Division A/Belgium First Division A.xlsx
+++ b/Belgium First Division A/Belgium First Division A.xlsx
@@ -16796,7 +16796,7 @@
         <v>188</v>
       </c>
       <c r="B190">
-        <v>6810174</v>
+        <v>6810171</v>
       </c>
       <c r="C190" t="s">
         <v>33</v>
@@ -16805,76 +16805,76 @@
         <v>45325.59375</v>
       </c>
       <c r="E190" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F190" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H190">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I190" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J190">
-        <v>1.909</v>
+        <v>3.2</v>
       </c>
       <c r="K190">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="L190">
-        <v>3.5</v>
+        <v>2.1</v>
       </c>
       <c r="M190">
-        <v>1.909</v>
+        <v>3.4</v>
       </c>
       <c r="N190">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="O190">
-        <v>3.8</v>
+        <v>2.05</v>
       </c>
       <c r="P190">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Q190">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="R190">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="S190">
         <v>2.5</v>
       </c>
       <c r="T190">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="U190">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V190">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="W190">
         <v>-1</v>
       </c>
       <c r="X190">
-        <v>2.8</v>
+        <v>-1</v>
       </c>
       <c r="Y190">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z190">
+        <v>-1</v>
+      </c>
+      <c r="AA190">
+        <v>-1</v>
+      </c>
+      <c r="AB190">
         <v>0.925</v>
-      </c>
-      <c r="AA190">
-        <v>0.8500000000000001</v>
-      </c>
-      <c r="AB190">
-        <v>-1</v>
       </c>
     </row>
     <row r="191" spans="1:28">
@@ -16882,7 +16882,7 @@
         <v>189</v>
       </c>
       <c r="B191">
-        <v>6810171</v>
+        <v>6810174</v>
       </c>
       <c r="C191" t="s">
         <v>33</v>
@@ -16891,76 +16891,76 @@
         <v>45325.59375</v>
       </c>
       <c r="E191" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F191" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G191">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H191">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I191" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J191">
-        <v>3.2</v>
+        <v>1.909</v>
       </c>
       <c r="K191">
+        <v>3.75</v>
+      </c>
+      <c r="L191">
         <v>3.5</v>
       </c>
-      <c r="L191">
-        <v>2.1</v>
-      </c>
       <c r="M191">
-        <v>3.4</v>
+        <v>1.909</v>
       </c>
       <c r="N191">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="O191">
-        <v>2.05</v>
+        <v>3.8</v>
       </c>
       <c r="P191">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q191">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="R191">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="S191">
         <v>2.5</v>
       </c>
       <c r="T191">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="U191">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V191">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="W191">
         <v>-1</v>
       </c>
       <c r="X191">
-        <v>-1</v>
+        <v>2.8</v>
       </c>
       <c r="Y191">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Z191">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA191">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB191">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="192" spans="1:28">
@@ -21182,7 +21182,7 @@
         <v>239</v>
       </c>
       <c r="B241">
-        <v>6957874</v>
+        <v>6810219</v>
       </c>
       <c r="C241" t="s">
         <v>33</v>
@@ -21191,67 +21191,67 @@
         <v>45368.60416666666</v>
       </c>
       <c r="E241" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F241" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G241">
         <v>1</v>
       </c>
       <c r="H241">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I241" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J241">
-        <v>3.6</v>
+        <v>2.8</v>
       </c>
       <c r="K241">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="L241">
-        <v>1.909</v>
+        <v>2.375</v>
       </c>
       <c r="M241">
-        <v>3.6</v>
+        <v>2.7</v>
       </c>
       <c r="N241">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="O241">
-        <v>1.95</v>
+        <v>2.45</v>
       </c>
       <c r="P241">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Q241">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="R241">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="S241">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="T241">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="U241">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="V241">
-        <v>-1</v>
+        <v>1.7</v>
       </c>
       <c r="W241">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="X241">
         <v>-1</v>
       </c>
       <c r="Y241">
-        <v>0.8500000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="Z241">
         <v>-1</v>
@@ -21260,7 +21260,7 @@
         <v>-1</v>
       </c>
       <c r="AB241">
-        <v>0.8500000000000001</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="242" spans="1:28">
@@ -21268,7 +21268,7 @@
         <v>240</v>
       </c>
       <c r="B242">
-        <v>6810219</v>
+        <v>6957874</v>
       </c>
       <c r="C242" t="s">
         <v>33</v>
@@ -21277,67 +21277,67 @@
         <v>45368.60416666666</v>
       </c>
       <c r="E242" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F242" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="G242">
         <v>1</v>
       </c>
       <c r="H242">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I242" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J242">
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
       <c r="K242">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="L242">
-        <v>2.375</v>
+        <v>1.909</v>
       </c>
       <c r="M242">
-        <v>2.7</v>
+        <v>3.6</v>
       </c>
       <c r="N242">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="O242">
-        <v>2.45</v>
+        <v>1.95</v>
       </c>
       <c r="P242">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q242">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="R242">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="S242">
+        <v>3</v>
+      </c>
+      <c r="T242">
+        <v>2</v>
+      </c>
+      <c r="U242">
+        <v>1.85</v>
+      </c>
+      <c r="V242">
+        <v>-1</v>
+      </c>
+      <c r="W242">
         <v>2.75</v>
       </c>
-      <c r="T242">
-        <v>1.925</v>
-      </c>
-      <c r="U242">
-        <v>1.925</v>
-      </c>
-      <c r="V242">
-        <v>1.7</v>
-      </c>
-      <c r="W242">
-        <v>-1</v>
-      </c>
       <c r="X242">
         <v>-1</v>
       </c>
       <c r="Y242">
-        <v>1.025</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z242">
         <v>-1</v>
@@ -21346,7 +21346,7 @@
         <v>-1</v>
       </c>
       <c r="AB242">
-        <v>0.925</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="243" spans="1:28">
@@ -21354,7 +21354,7 @@
         <v>241</v>
       </c>
       <c r="B243">
-        <v>6870199</v>
+        <v>6942395</v>
       </c>
       <c r="C243" t="s">
         <v>33</v>
@@ -21363,13 +21363,13 @@
         <v>45368.60416666666</v>
       </c>
       <c r="E243" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F243" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G243">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H243">
         <v>0</v>
@@ -21378,34 +21378,34 @@
         <v>50</v>
       </c>
       <c r="J243">
-        <v>1.363</v>
+        <v>1.571</v>
       </c>
       <c r="K243">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="L243">
-        <v>7.5</v>
+        <v>5.75</v>
       </c>
       <c r="M243">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="N243">
-        <v>6</v>
+        <v>4.333</v>
       </c>
       <c r="O243">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="P243">
-        <v>-1.75</v>
+        <v>-1.25</v>
       </c>
       <c r="Q243">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="R243">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="S243">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="T243">
         <v>1.95</v>
@@ -21414,7 +21414,7 @@
         <v>1.9</v>
       </c>
       <c r="V243">
-        <v>0.3</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="W243">
         <v>-1</v>
@@ -21423,7 +21423,7 @@
         <v>-1</v>
       </c>
       <c r="Y243">
-        <v>1.025</v>
+        <v>1</v>
       </c>
       <c r="Z243">
         <v>-1</v>
@@ -21440,7 +21440,7 @@
         <v>242</v>
       </c>
       <c r="B244">
-        <v>6942395</v>
+        <v>6870199</v>
       </c>
       <c r="C244" t="s">
         <v>33</v>
@@ -21449,13 +21449,13 @@
         <v>45368.60416666666</v>
       </c>
       <c r="E244" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F244" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G244">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H244">
         <v>0</v>
@@ -21464,34 +21464,34 @@
         <v>50</v>
       </c>
       <c r="J244">
-        <v>1.571</v>
+        <v>1.363</v>
       </c>
       <c r="K244">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="L244">
-        <v>5.75</v>
+        <v>7.5</v>
       </c>
       <c r="M244">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="N244">
-        <v>4.333</v>
+        <v>6</v>
       </c>
       <c r="O244">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="P244">
-        <v>-1.25</v>
+        <v>-1.75</v>
       </c>
       <c r="Q244">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="R244">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="S244">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="T244">
         <v>1.95</v>
@@ -21500,7 +21500,7 @@
         <v>1.9</v>
       </c>
       <c r="V244">
-        <v>0.3999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="W244">
         <v>-1</v>
@@ -21509,7 +21509,7 @@
         <v>-1</v>
       </c>
       <c r="Y244">
-        <v>1</v>
+        <v>1.025</v>
       </c>
       <c r="Z244">
         <v>-1</v>
@@ -24192,7 +24192,7 @@
         <v>274</v>
       </c>
       <c r="B276">
-        <v>7979346</v>
+        <v>7979470</v>
       </c>
       <c r="C276" t="s">
         <v>33</v>
@@ -24201,76 +24201,76 @@
         <v>45405.64583333334</v>
       </c>
       <c r="E276" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F276" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G276">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H276">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I276" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J276">
+        <v>2.5</v>
+      </c>
+      <c r="K276">
         <v>3.6</v>
       </c>
-      <c r="K276">
-        <v>3.5</v>
-      </c>
       <c r="L276">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="M276">
-        <v>3.3</v>
+        <v>2.45</v>
       </c>
       <c r="N276">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="O276">
-        <v>2.05</v>
+        <v>2.55</v>
       </c>
       <c r="P276">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="Q276">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="R276">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="S276">
         <v>3</v>
       </c>
       <c r="T276">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="U276">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="V276">
         <v>-1</v>
       </c>
       <c r="W276">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="X276">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Y276">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z276">
-        <v>0.825</v>
+        <v>0</v>
       </c>
       <c r="AA276">
         <v>-1</v>
       </c>
       <c r="AB276">
-        <v>0.875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="277" spans="1:28">
@@ -24278,7 +24278,7 @@
         <v>275</v>
       </c>
       <c r="B277">
-        <v>7979470</v>
+        <v>7979346</v>
       </c>
       <c r="C277" t="s">
         <v>33</v>
@@ -24287,76 +24287,76 @@
         <v>45405.64583333334</v>
       </c>
       <c r="E277" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F277" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G277">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H277">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I277" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J277">
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="K277">
+        <v>3.5</v>
+      </c>
+      <c r="L277">
+        <v>2</v>
+      </c>
+      <c r="M277">
+        <v>3.3</v>
+      </c>
+      <c r="N277">
         <v>3.6</v>
       </c>
-      <c r="L277">
-        <v>2.6</v>
-      </c>
-      <c r="M277">
-        <v>2.45</v>
-      </c>
-      <c r="N277">
-        <v>3.75</v>
-      </c>
       <c r="O277">
-        <v>2.55</v>
+        <v>2.05</v>
       </c>
       <c r="P277">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="Q277">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="R277">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="S277">
         <v>3</v>
       </c>
       <c r="T277">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="U277">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="V277">
         <v>-1</v>
       </c>
       <c r="W277">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="X277">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Y277">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z277">
-        <v>0</v>
+        <v>0.825</v>
       </c>
       <c r="AA277">
         <v>-1</v>
       </c>
       <c r="AB277">
-        <v>1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="278" spans="1:28">
@@ -27140,31 +27140,31 @@
         <v>5.25</v>
       </c>
       <c r="M310">
-        <v>1.5</v>
+        <v>1.45</v>
       </c>
       <c r="N310">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="O310">
-        <v>5.25</v>
+        <v>5.5</v>
       </c>
       <c r="P310">
-        <v>-1</v>
+        <v>-1.25</v>
       </c>
       <c r="Q310">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="R310">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="S310">
         <v>3.5</v>
       </c>
       <c r="T310">
+        <v>1.85</v>
+      </c>
+      <c r="U310">
         <v>2</v>
-      </c>
-      <c r="U310">
-        <v>1.85</v>
       </c>
       <c r="V310">
         <v>0</v>
@@ -27205,31 +27205,31 @@
         <v>3.2</v>
       </c>
       <c r="M311">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="N311">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="O311">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="P311">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q311">
+        <v>2.025</v>
+      </c>
+      <c r="R311">
         <v>1.825</v>
-      </c>
-      <c r="R311">
-        <v>2.025</v>
       </c>
       <c r="S311">
         <v>3.25</v>
       </c>
       <c r="T311">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="U311">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="V311">
         <v>0</v>
@@ -27273,28 +27273,28 @@
         <v>1.85</v>
       </c>
       <c r="N312">
-        <v>3.7</v>
+        <v>4</v>
       </c>
       <c r="O312">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="P312">
         <v>-0.5</v>
       </c>
       <c r="Q312">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="R312">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="S312">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="T312">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="U312">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="V312">
         <v>0</v>
@@ -27335,31 +27335,31 @@
         <v>1.833</v>
       </c>
       <c r="M313">
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
       <c r="N313">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="O313">
-        <v>1.727</v>
+        <v>1.75</v>
       </c>
       <c r="P313">
         <v>0.75</v>
       </c>
       <c r="Q313">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="R313">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="S313">
         <v>2.75</v>
       </c>
       <c r="T313">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="U313">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V313">
         <v>0</v>
@@ -27400,31 +27400,31 @@
         <v>4.333</v>
       </c>
       <c r="M314">
-        <v>1.65</v>
+        <v>1.55</v>
       </c>
       <c r="N314">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="O314">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="P314">
-        <v>-0.75</v>
+        <v>-1</v>
       </c>
       <c r="Q314">
+        <v>2</v>
+      </c>
+      <c r="R314">
         <v>1.85</v>
-      </c>
-      <c r="R314">
-        <v>2</v>
       </c>
       <c r="S314">
         <v>3</v>
       </c>
       <c r="T314">
+        <v>1.9</v>
+      </c>
+      <c r="U314">
         <v>1.95</v>
-      </c>
-      <c r="U314">
-        <v>1.9</v>
       </c>
       <c r="V314">
         <v>0</v>
@@ -27465,31 +27465,31 @@
         <v>5.5</v>
       </c>
       <c r="M315">
-        <v>1.5</v>
+        <v>1.48</v>
       </c>
       <c r="N315">
-        <v>4.333</v>
+        <v>4.1</v>
       </c>
       <c r="O315">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="P315">
         <v>-1</v>
       </c>
       <c r="Q315">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="R315">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="S315">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="T315">
+        <v>2</v>
+      </c>
+      <c r="U315">
         <v>1.85</v>
-      </c>
-      <c r="U315">
-        <v>2</v>
       </c>
       <c r="V315">
         <v>0</v>

</xml_diff>